<commit_message>
Rat in a Maze added.
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harsh\Desktop\FINAL 450\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0892E0F8-4BE5-4A42-AB49-F63430039FE7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2AD5C02-1682-4B95-B08B-C7F63A30A51C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -2014,8 +2014,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:D492"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A373" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B388" sqref="B388"/>
+    <sheetView tabSelected="1" topLeftCell="A361" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D372" sqref="D372"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -5967,8 +5967,8 @@
       <c r="B372" s="6" t="s">
         <v>348</v>
       </c>
-      <c r="C372" s="4" t="s">
-        <v>4</v>
+      <c r="C372" s="11" t="s">
+        <v>464</v>
       </c>
     </row>
     <row r="373" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Steps by Knight added.
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harsh\Desktop\FINAL 450\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harsh\Desktop\Data-Structures-and-Algorithms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2AD5C02-1682-4B95-B08B-C7F63A30A51C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5606BF89-E6F9-45CA-ACD5-556F3E6FF32F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -2014,8 +2014,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:D492"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A361" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D372" sqref="D372"/>
+    <sheetView tabSelected="1" topLeftCell="A365" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C373" sqref="C373"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -5978,8 +5978,8 @@
       <c r="B373" s="6" t="s">
         <v>349</v>
       </c>
-      <c r="C373" s="4" t="s">
-        <v>4</v>
+      <c r="C373" s="11" t="s">
+        <v>464</v>
       </c>
     </row>
     <row r="374" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Clone an Undirected Graph added.
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harsh\Desktop\Data-Structures-and-Algorithms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84E44456-D9FA-4234-9C89-0688A11172D3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE6F9197-33CD-428F-AD05-CC4CC89C94B6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -2015,7 +2015,7 @@
   <dimension ref="A1:D492"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A365" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C375" sqref="C375"/>
+      <selection activeCell="C376" sqref="C376"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -6000,8 +6000,8 @@
       <c r="B375" s="6" t="s">
         <v>351</v>
       </c>
-      <c r="C375" s="4" t="s">
-        <v>4</v>
+      <c r="C375" s="11" t="s">
+        <v>464</v>
       </c>
     </row>
     <row r="376" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Number of Operations to Make Network Connected
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harsh\Desktop\Data-Structures-and-Algorithms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9739515F-6277-422C-BAFE-53A0F303450D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F26D1631-F98E-4F28-9DE0-CC062F4EC06F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -2015,7 +2015,7 @@
   <dimension ref="A1:D492"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A365" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C376" sqref="C376"/>
+      <selection activeCell="B376" sqref="B376"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -6011,8 +6011,8 @@
       <c r="B376" s="6" t="s">
         <v>352</v>
       </c>
-      <c r="C376" s="4" t="s">
-        <v>4</v>
+      <c r="C376" s="11" t="s">
+        <v>464</v>
       </c>
     </row>
     <row r="377" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Minimum time taken by each job to be completed given by a Directed Acyclic Graph
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harsh\Desktop\Data-Structures-and-Algorithms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4426A472-AF62-43A0-9AC1-7D099AE16D70}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AA37914-DE07-467E-B0C5-50382C26E21A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -2023,8 +2023,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:D492"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A364" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C378" sqref="C378"/>
+    <sheetView tabSelected="1" topLeftCell="A369" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C381" sqref="C381"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -6064,8 +6064,8 @@
       <c r="B380" s="6" t="s">
         <v>356</v>
       </c>
-      <c r="C380" s="4" t="s">
-        <v>4</v>
+      <c r="C380" s="11" t="s">
+        <v>464</v>
       </c>
     </row>
     <row r="381" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Bipartite Graph and Graph Coloring
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harsh\Desktop\Data-Structures-and-Algorithms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D4C3631-1D00-45C7-8551-7ACA9F26BA7D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08A9464A-2088-4E90-8E2A-AD9B8C1895FE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1403" uniqueCount="491">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1406" uniqueCount="492">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1498,6 +1498,9 @@
   </si>
   <si>
     <t>Sum of all leaf nodes of binary tree</t>
+  </si>
+  <si>
+    <t>Bipartite Graph</t>
   </si>
 </sst>
 </file>
@@ -2024,10 +2027,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
-  <dimension ref="A1:D493"/>
+  <dimension ref="A1:D494"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A176" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B186" sqref="B186"/>
+    <sheetView tabSelected="1" topLeftCell="A384" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B393" sqref="B393"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -6186,10 +6189,10 @@
         <v>342</v>
       </c>
       <c r="B391" s="6" t="s">
-        <v>366</v>
-      </c>
-      <c r="C391" s="4" t="s">
-        <v>4</v>
+        <v>491</v>
+      </c>
+      <c r="C391" s="11" t="s">
+        <v>464</v>
       </c>
     </row>
     <row r="392" spans="1:3" ht="21">
@@ -6197,10 +6200,10 @@
         <v>342</v>
       </c>
       <c r="B392" s="6" t="s">
-        <v>367</v>
-      </c>
-      <c r="C392" s="4" t="s">
-        <v>4</v>
+        <v>366</v>
+      </c>
+      <c r="C392" s="11" t="s">
+        <v>464</v>
       </c>
     </row>
     <row r="393" spans="1:3" ht="21">
@@ -6208,7 +6211,7 @@
         <v>342</v>
       </c>
       <c r="B393" s="6" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="C393" s="4" t="s">
         <v>4</v>
@@ -6219,7 +6222,7 @@
         <v>342</v>
       </c>
       <c r="B394" s="6" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C394" s="4" t="s">
         <v>4</v>
@@ -6230,7 +6233,7 @@
         <v>342</v>
       </c>
       <c r="B395" s="6" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="C395" s="4" t="s">
         <v>4</v>
@@ -6241,7 +6244,7 @@
         <v>342</v>
       </c>
       <c r="B396" s="6" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="C396" s="4" t="s">
         <v>4</v>
@@ -6252,7 +6255,7 @@
         <v>342</v>
       </c>
       <c r="B397" s="6" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="C397" s="4" t="s">
         <v>4</v>
@@ -6263,7 +6266,7 @@
         <v>342</v>
       </c>
       <c r="B398" s="6" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C398" s="4" t="s">
         <v>4</v>
@@ -6274,7 +6277,7 @@
         <v>342</v>
       </c>
       <c r="B399" s="6" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C399" s="4" t="s">
         <v>4</v>
@@ -6285,7 +6288,7 @@
         <v>342</v>
       </c>
       <c r="B400" s="6" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C400" s="4" t="s">
         <v>4</v>
@@ -6296,7 +6299,7 @@
         <v>342</v>
       </c>
       <c r="B401" s="6" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="C401" s="4" t="s">
         <v>4</v>
@@ -6318,7 +6321,7 @@
         <v>342</v>
       </c>
       <c r="B403" s="6" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="C403" s="4" t="s">
         <v>4</v>
@@ -6329,7 +6332,7 @@
         <v>342</v>
       </c>
       <c r="B404" s="6" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="C404" s="4" t="s">
         <v>4</v>
@@ -6340,7 +6343,7 @@
         <v>342</v>
       </c>
       <c r="B405" s="6" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C405" s="4" t="s">
         <v>4</v>
@@ -6351,7 +6354,7 @@
         <v>342</v>
       </c>
       <c r="B406" s="6" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="C406" s="4" t="s">
         <v>4</v>
@@ -6362,7 +6365,7 @@
         <v>342</v>
       </c>
       <c r="B407" s="6" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C407" s="4" t="s">
         <v>4</v>
@@ -6373,7 +6376,7 @@
         <v>342</v>
       </c>
       <c r="B408" s="6" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="C408" s="4" t="s">
         <v>4</v>
@@ -6384,7 +6387,7 @@
         <v>342</v>
       </c>
       <c r="B409" s="6" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="C409" s="4" t="s">
         <v>4</v>
@@ -6395,7 +6398,7 @@
         <v>342</v>
       </c>
       <c r="B410" s="6" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="C410" s="4" t="s">
         <v>4</v>
@@ -6406,37 +6409,37 @@
         <v>342</v>
       </c>
       <c r="B411" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="C411" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="412" spans="1:3" ht="21">
+      <c r="A412" s="8" t="s">
+        <v>342</v>
+      </c>
+      <c r="B412" s="6" t="s">
         <v>385</v>
       </c>
-      <c r="C411" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="412" spans="1:3" ht="21">
-      <c r="B412" s="7"/>
-      <c r="C412" s="4"/>
+      <c r="C412" s="4" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="413" spans="1:3" ht="21">
       <c r="B413" s="7"/>
       <c r="C413" s="4"/>
     </row>
     <row r="414" spans="1:3" ht="21">
-      <c r="A414" s="8" t="s">
-        <v>386</v>
-      </c>
-      <c r="B414" s="6" t="s">
-        <v>387</v>
-      </c>
-      <c r="C414" s="4" t="s">
-        <v>4</v>
-      </c>
+      <c r="B414" s="7"/>
+      <c r="C414" s="4"/>
     </row>
     <row r="415" spans="1:3" ht="21">
       <c r="A415" s="8" t="s">
         <v>386</v>
       </c>
       <c r="B415" s="6" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="C415" s="4" t="s">
         <v>4</v>
@@ -6447,7 +6450,7 @@
         <v>386</v>
       </c>
       <c r="B416" s="6" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="C416" s="4" t="s">
         <v>4</v>
@@ -6458,7 +6461,7 @@
         <v>386</v>
       </c>
       <c r="B417" s="6" t="s">
-        <v>89</v>
+        <v>389</v>
       </c>
       <c r="C417" s="4" t="s">
         <v>4</v>
@@ -6469,7 +6472,7 @@
         <v>386</v>
       </c>
       <c r="B418" s="6" t="s">
-        <v>390</v>
+        <v>89</v>
       </c>
       <c r="C418" s="4" t="s">
         <v>4</v>
@@ -6480,37 +6483,37 @@
         <v>386</v>
       </c>
       <c r="B419" s="6" t="s">
+        <v>390</v>
+      </c>
+      <c r="C419" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="420" spans="1:3" ht="21">
+      <c r="A420" s="8" t="s">
+        <v>386</v>
+      </c>
+      <c r="B420" s="6" t="s">
         <v>391</v>
       </c>
-      <c r="C419" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="420" spans="1:3" ht="21">
-      <c r="B420" s="7"/>
-      <c r="C420" s="4"/>
+      <c r="C420" s="4" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="421" spans="1:3" ht="21">
       <c r="B421" s="7"/>
       <c r="C421" s="4"/>
     </row>
     <row r="422" spans="1:3" ht="21">
-      <c r="A422" s="5" t="s">
-        <v>392</v>
-      </c>
-      <c r="B422" s="6" t="s">
-        <v>393</v>
-      </c>
-      <c r="C422" s="4" t="s">
-        <v>4</v>
-      </c>
+      <c r="B422" s="7"/>
+      <c r="C422" s="4"/>
     </row>
     <row r="423" spans="1:3" ht="21">
       <c r="A423" s="5" t="s">
         <v>392</v>
       </c>
       <c r="B423" s="6" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="C423" s="4" t="s">
         <v>4</v>
@@ -6521,7 +6524,7 @@
         <v>392</v>
       </c>
       <c r="B424" s="6" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C424" s="4" t="s">
         <v>4</v>
@@ -6532,7 +6535,7 @@
         <v>392</v>
       </c>
       <c r="B425" s="6" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="C425" s="4" t="s">
         <v>4</v>
@@ -6543,7 +6546,7 @@
         <v>392</v>
       </c>
       <c r="B426" s="6" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="C426" s="4" t="s">
         <v>4</v>
@@ -6554,7 +6557,7 @@
         <v>392</v>
       </c>
       <c r="B427" s="6" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="C427" s="4" t="s">
         <v>4</v>
@@ -6565,7 +6568,7 @@
         <v>392</v>
       </c>
       <c r="B428" s="6" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="C428" s="4" t="s">
         <v>4</v>
@@ -6576,7 +6579,7 @@
         <v>392</v>
       </c>
       <c r="B429" s="6" t="s">
-        <v>272</v>
+        <v>399</v>
       </c>
       <c r="C429" s="4" t="s">
         <v>4</v>
@@ -6587,7 +6590,7 @@
         <v>392</v>
       </c>
       <c r="B430" s="6" t="s">
-        <v>400</v>
+        <v>272</v>
       </c>
       <c r="C430" s="4" t="s">
         <v>4</v>
@@ -6598,7 +6601,7 @@
         <v>392</v>
       </c>
       <c r="B431" s="6" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="C431" s="4" t="s">
         <v>4</v>
@@ -6609,7 +6612,7 @@
         <v>392</v>
       </c>
       <c r="B432" s="6" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="C432" s="4" t="s">
         <v>4</v>
@@ -6620,7 +6623,7 @@
         <v>392</v>
       </c>
       <c r="B433" s="6" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="C433" s="4" t="s">
         <v>4</v>
@@ -6631,7 +6634,7 @@
         <v>392</v>
       </c>
       <c r="B434" s="6" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="C434" s="4" t="s">
         <v>4</v>
@@ -6642,7 +6645,7 @@
         <v>392</v>
       </c>
       <c r="B435" s="6" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="C435" s="4" t="s">
         <v>4</v>
@@ -6653,7 +6656,7 @@
         <v>392</v>
       </c>
       <c r="B436" s="6" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="C436" s="4" t="s">
         <v>4</v>
@@ -6664,7 +6667,7 @@
         <v>392</v>
       </c>
       <c r="B437" s="6" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="C437" s="4" t="s">
         <v>4</v>
@@ -6675,7 +6678,7 @@
         <v>392</v>
       </c>
       <c r="B438" s="6" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="C438" s="4" t="s">
         <v>4</v>
@@ -6686,7 +6689,7 @@
         <v>392</v>
       </c>
       <c r="B439" s="6" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="C439" s="4" t="s">
         <v>4</v>
@@ -6697,7 +6700,7 @@
         <v>392</v>
       </c>
       <c r="B440" s="6" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="C440" s="4" t="s">
         <v>4</v>
@@ -6708,7 +6711,7 @@
         <v>392</v>
       </c>
       <c r="B441" s="6" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="C441" s="4" t="s">
         <v>4</v>
@@ -6719,7 +6722,7 @@
         <v>392</v>
       </c>
       <c r="B442" s="6" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C442" s="4" t="s">
         <v>4</v>
@@ -6730,7 +6733,7 @@
         <v>392</v>
       </c>
       <c r="B443" s="6" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="C443" s="4" t="s">
         <v>4</v>
@@ -6741,7 +6744,7 @@
         <v>392</v>
       </c>
       <c r="B444" s="6" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C444" s="4" t="s">
         <v>4</v>
@@ -6752,7 +6755,7 @@
         <v>392</v>
       </c>
       <c r="B445" s="6" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C445" s="4" t="s">
         <v>4</v>
@@ -6763,7 +6766,7 @@
         <v>392</v>
       </c>
       <c r="B446" s="6" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C446" s="4" t="s">
         <v>4</v>
@@ -6774,7 +6777,7 @@
         <v>392</v>
       </c>
       <c r="B447" s="6" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C447" s="4" t="s">
         <v>4</v>
@@ -6785,7 +6788,7 @@
         <v>392</v>
       </c>
       <c r="B448" s="6" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="C448" s="4" t="s">
         <v>4</v>
@@ -6796,7 +6799,7 @@
         <v>392</v>
       </c>
       <c r="B449" s="6" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="C449" s="4" t="s">
         <v>4</v>
@@ -6807,7 +6810,7 @@
         <v>392</v>
       </c>
       <c r="B450" s="6" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="C450" s="4" t="s">
         <v>4</v>
@@ -6818,7 +6821,7 @@
         <v>392</v>
       </c>
       <c r="B451" s="6" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="C451" s="4" t="s">
         <v>4</v>
@@ -6829,7 +6832,7 @@
         <v>392</v>
       </c>
       <c r="B452" s="6" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="C452" s="4" t="s">
         <v>4</v>
@@ -6840,7 +6843,7 @@
         <v>392</v>
       </c>
       <c r="B453" s="6" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="C453" s="4" t="s">
         <v>4</v>
@@ -6851,7 +6854,7 @@
         <v>392</v>
       </c>
       <c r="B454" s="6" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="C454" s="4" t="s">
         <v>4</v>
@@ -6862,7 +6865,7 @@
         <v>392</v>
       </c>
       <c r="B455" s="6" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C455" s="4" t="s">
         <v>4</v>
@@ -6873,7 +6876,7 @@
         <v>392</v>
       </c>
       <c r="B456" s="6" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="C456" s="4" t="s">
         <v>4</v>
@@ -6884,7 +6887,7 @@
         <v>392</v>
       </c>
       <c r="B457" s="6" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="C457" s="4" t="s">
         <v>4</v>
@@ -6895,7 +6898,7 @@
         <v>392</v>
       </c>
       <c r="B458" s="6" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="C458" s="4" t="s">
         <v>4</v>
@@ -6906,7 +6909,7 @@
         <v>392</v>
       </c>
       <c r="B459" s="6" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="C459" s="4" t="s">
         <v>4</v>
@@ -6917,7 +6920,7 @@
         <v>392</v>
       </c>
       <c r="B460" s="6" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="C460" s="4" t="s">
         <v>4</v>
@@ -6928,7 +6931,7 @@
         <v>392</v>
       </c>
       <c r="B461" s="6" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C461" s="4" t="s">
         <v>4</v>
@@ -6939,7 +6942,7 @@
         <v>392</v>
       </c>
       <c r="B462" s="6" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="C462" s="4" t="s">
         <v>4</v>
@@ -6950,7 +6953,7 @@
         <v>392</v>
       </c>
       <c r="B463" s="6" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C463" s="4" t="s">
         <v>4</v>
@@ -6961,7 +6964,7 @@
         <v>392</v>
       </c>
       <c r="B464" s="6" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C464" s="4" t="s">
         <v>4</v>
@@ -6972,7 +6975,7 @@
         <v>392</v>
       </c>
       <c r="B465" s="6" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="C465" s="4" t="s">
         <v>4</v>
@@ -6983,7 +6986,7 @@
         <v>392</v>
       </c>
       <c r="B466" s="6" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="C466" s="4" t="s">
         <v>4</v>
@@ -6994,7 +6997,7 @@
         <v>392</v>
       </c>
       <c r="B467" s="6" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="C467" s="4" t="s">
         <v>4</v>
@@ -7005,7 +7008,7 @@
         <v>392</v>
       </c>
       <c r="B468" s="6" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="C468" s="4" t="s">
         <v>4</v>
@@ -7016,7 +7019,7 @@
         <v>392</v>
       </c>
       <c r="B469" s="6" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="C469" s="4" t="s">
         <v>4</v>
@@ -7027,7 +7030,7 @@
         <v>392</v>
       </c>
       <c r="B470" s="6" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="C470" s="4" t="s">
         <v>4</v>
@@ -7038,7 +7041,7 @@
         <v>392</v>
       </c>
       <c r="B471" s="6" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="C471" s="4" t="s">
         <v>4</v>
@@ -7049,7 +7052,7 @@
         <v>392</v>
       </c>
       <c r="B472" s="6" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="C472" s="4" t="s">
         <v>4</v>
@@ -7060,7 +7063,7 @@
         <v>392</v>
       </c>
       <c r="B473" s="6" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="C473" s="4" t="s">
         <v>4</v>
@@ -7071,7 +7074,7 @@
         <v>392</v>
       </c>
       <c r="B474" s="6" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="C474" s="4" t="s">
         <v>4</v>
@@ -7082,7 +7085,7 @@
         <v>392</v>
       </c>
       <c r="B475" s="6" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="C475" s="4" t="s">
         <v>4</v>
@@ -7093,7 +7096,7 @@
         <v>392</v>
       </c>
       <c r="B476" s="6" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="C476" s="4" t="s">
         <v>4</v>
@@ -7104,7 +7107,7 @@
         <v>392</v>
       </c>
       <c r="B477" s="6" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="C477" s="4" t="s">
         <v>4</v>
@@ -7115,7 +7118,7 @@
         <v>392</v>
       </c>
       <c r="B478" s="6" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="C478" s="4" t="s">
         <v>4</v>
@@ -7126,7 +7129,7 @@
         <v>392</v>
       </c>
       <c r="B479" s="6" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="C479" s="4" t="s">
         <v>4</v>
@@ -7137,7 +7140,7 @@
         <v>392</v>
       </c>
       <c r="B480" s="6" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="C480" s="4" t="s">
         <v>4</v>
@@ -7148,38 +7151,38 @@
         <v>392</v>
       </c>
       <c r="B481" s="6" t="s">
+        <v>450</v>
+      </c>
+      <c r="C481" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="482" spans="1:3" ht="21">
+      <c r="A482" s="5" t="s">
+        <v>392</v>
+      </c>
+      <c r="B482" s="6" t="s">
         <v>451</v>
       </c>
-      <c r="C481" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="482" spans="1:3" ht="21">
-      <c r="B482" s="7"/>
-      <c r="C482" s="4"/>
+      <c r="C482" s="4" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="483" spans="1:3" ht="21">
-      <c r="A483" s="8"/>
       <c r="B483" s="7"/>
       <c r="C483" s="4"/>
     </row>
     <row r="484" spans="1:3" ht="21">
-      <c r="A484" s="5" t="s">
-        <v>452</v>
-      </c>
-      <c r="B484" s="6" t="s">
-        <v>453</v>
-      </c>
-      <c r="C484" s="4" t="s">
-        <v>4</v>
-      </c>
+      <c r="A484" s="8"/>
+      <c r="B484" s="7"/>
+      <c r="C484" s="4"/>
     </row>
     <row r="485" spans="1:3" ht="21">
       <c r="A485" s="5" t="s">
         <v>452</v>
       </c>
       <c r="B485" s="6" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="C485" s="4" t="s">
         <v>4</v>
@@ -7190,7 +7193,7 @@
         <v>452</v>
       </c>
       <c r="B486" s="6" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="C486" s="4" t="s">
         <v>4</v>
@@ -7201,7 +7204,7 @@
         <v>452</v>
       </c>
       <c r="B487" s="6" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="C487" s="4" t="s">
         <v>4</v>
@@ -7212,7 +7215,7 @@
         <v>452</v>
       </c>
       <c r="B488" s="6" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="C488" s="4" t="s">
         <v>4</v>
@@ -7223,7 +7226,7 @@
         <v>452</v>
       </c>
       <c r="B489" s="6" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="C489" s="4" t="s">
         <v>4</v>
@@ -7234,7 +7237,7 @@
         <v>452</v>
       </c>
       <c r="B490" s="6" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="C490" s="4" t="s">
         <v>4</v>
@@ -7245,7 +7248,7 @@
         <v>452</v>
       </c>
       <c r="B491" s="6" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="C491" s="4" t="s">
         <v>4</v>
@@ -7256,7 +7259,7 @@
         <v>452</v>
       </c>
       <c r="B492" s="6" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="C492" s="4" t="s">
         <v>4</v>
@@ -7267,9 +7270,20 @@
         <v>452</v>
       </c>
       <c r="B493" s="6" t="s">
+        <v>461</v>
+      </c>
+      <c r="C493" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="494" spans="1:3" ht="21">
+      <c r="A494" s="5" t="s">
+        <v>452</v>
+      </c>
+      <c r="B494" s="6" t="s">
         <v>462</v>
       </c>
-      <c r="C493" s="4" t="s">
+      <c r="C494" s="4" t="s">
         <v>4</v>
       </c>
     </row>
@@ -7620,103 +7634,103 @@
     <hyperlink ref="B388" r:id="rId343" xr:uid="{FA9B4BE7-85CC-B24F-9461-5E9B42DDD824}"/>
     <hyperlink ref="B389" r:id="rId344" xr:uid="{A75ACEA2-CDF6-A147-8540-A6DF55B15F45}"/>
     <hyperlink ref="B390" r:id="rId345" xr:uid="{62FF87E2-E658-AB4D-AC57-7BCF9D49516E}"/>
-    <hyperlink ref="B391" r:id="rId346" location=":~:text=Graph%20coloring%20problem%20is%20to,are%20colored%20using%20same%20color." xr:uid="{269338A6-5145-6944-9F7F-BD2A86DFA308}"/>
-    <hyperlink ref="B392" r:id="rId347" xr:uid="{8F583049-CE8D-CD42-88CD-CF3857942670}"/>
-    <hyperlink ref="B393" r:id="rId348" xr:uid="{EE2348AD-E296-894A-B5AE-5884A3C5E419}"/>
-    <hyperlink ref="B394" r:id="rId349" xr:uid="{6EACB34E-B32E-8F43-8055-2406F7417A7E}"/>
-    <hyperlink ref="B395" r:id="rId350" xr:uid="{2446F10A-B762-B64C-97B2-6131A0BECC1F}"/>
-    <hyperlink ref="B396" r:id="rId351" xr:uid="{6FDFCC53-17A6-7244-88A7-49406D7C9200}"/>
-    <hyperlink ref="B397" r:id="rId352" xr:uid="{3EC43646-EAB1-E443-A2F6-8E6E5FC77083}"/>
-    <hyperlink ref="B398" r:id="rId353" xr:uid="{659D9F20-C862-C947-B422-84143CFE317F}"/>
-    <hyperlink ref="B399" r:id="rId354" xr:uid="{3F5192FE-1C50-C049-88D5-68FA0F5430A0}"/>
-    <hyperlink ref="B400" r:id="rId355" xr:uid="{5EAD7CDA-9545-454B-BE77-9AFEC6AC1083}"/>
-    <hyperlink ref="B401" r:id="rId356" xr:uid="{761E5451-736B-6745-9CF5-4C6EF5D4C099}"/>
-    <hyperlink ref="B402" r:id="rId357" xr:uid="{4C8677A9-D94C-134F-AF31-E424751BF867}"/>
-    <hyperlink ref="B403" r:id="rId358" xr:uid="{CCF7920F-D5CE-004A-86C3-D821FB230970}"/>
-    <hyperlink ref="B404" r:id="rId359" xr:uid="{B4C07A0A-1EDD-7947-9646-3FD603441AD7}"/>
-    <hyperlink ref="B405" r:id="rId360" xr:uid="{49F7BB43-6851-0641-9DC5-27DBC66706F6}"/>
-    <hyperlink ref="B406" r:id="rId361" xr:uid="{77038647-48C7-5547-8E0F-898610362465}"/>
-    <hyperlink ref="B408" r:id="rId362" xr:uid="{EEFFE19C-6571-C64F-A0E1-5A4A700D94D4}"/>
-    <hyperlink ref="B407" r:id="rId363" xr:uid="{A4A2BFC4-6B88-2E4E-B362-17D8EE041C89}"/>
-    <hyperlink ref="B409" r:id="rId364" xr:uid="{DC5B603A-8D65-3648-A08A-E5FFA0FAE879}"/>
-    <hyperlink ref="B410" r:id="rId365" xr:uid="{F8807DD9-F4F2-B147-9C31-DBC93B2E477B}"/>
-    <hyperlink ref="B411" r:id="rId366" xr:uid="{6F7B396C-D7E9-C04E-BAE2-53D2EE07172B}"/>
-    <hyperlink ref="B414" r:id="rId367" xr:uid="{0D4A5941-C669-4A49-BAE3-9B553D03BD0F}"/>
-    <hyperlink ref="B415" r:id="rId368" xr:uid="{54144336-5BCA-D749-962A-E448C2CED3D3}"/>
-    <hyperlink ref="B416" r:id="rId369" xr:uid="{3A41DD21-CACF-1F48-A7C7-F568C6F31F3E}"/>
-    <hyperlink ref="B417" r:id="rId370" xr:uid="{A36160A8-F45E-3443-9645-42C1004B8F8C}"/>
-    <hyperlink ref="B418" r:id="rId371" xr:uid="{8B0A00A3-6AC0-DF46-AD87-A4DA016A2A00}"/>
-    <hyperlink ref="B419" r:id="rId372" xr:uid="{62A81CB4-A961-C543-B31C-92059DB6C105}"/>
-    <hyperlink ref="B422" r:id="rId373" xr:uid="{08030975-009C-C34A-A875-72FE2718F44C}"/>
-    <hyperlink ref="B423" r:id="rId374" xr:uid="{A113C7A9-2359-B643-9C08-E845813439C0}"/>
-    <hyperlink ref="B424" r:id="rId375" xr:uid="{FE300343-4633-AD47-A64D-2086629EB398}"/>
-    <hyperlink ref="B425" r:id="rId376" xr:uid="{4FC9F782-D38F-C642-A863-887B17AD05CD}"/>
-    <hyperlink ref="B426" r:id="rId377" xr:uid="{830C5466-10E3-7A48-B3E7-35C15A1CA4EF}"/>
-    <hyperlink ref="B427" r:id="rId378" xr:uid="{1B987077-E9D3-6F40-89EE-0D4E7180D884}"/>
-    <hyperlink ref="B428" r:id="rId379" xr:uid="{D4843E1F-7226-864E-A4BB-264D5A487B6D}"/>
-    <hyperlink ref="B429" r:id="rId380" xr:uid="{61816592-2D19-9946-8253-47A60218F2EA}"/>
-    <hyperlink ref="B430" r:id="rId381" xr:uid="{736C840F-19A3-0A4B-8863-ECB772B46385}"/>
-    <hyperlink ref="B431" r:id="rId382" xr:uid="{05A238AD-3C5B-C546-94E9-75BBF964711A}"/>
-    <hyperlink ref="B432" r:id="rId383" xr:uid="{7029629C-3F2A-4A49-997B-CFE86EC8B3C2}"/>
-    <hyperlink ref="B433" r:id="rId384" xr:uid="{ADA66B57-2FAC-AB42-BD83-4931708F3AB5}"/>
-    <hyperlink ref="B434" r:id="rId385" xr:uid="{F16BF1F9-755B-B045-B9A8-0B97E3BAC8B0}"/>
-    <hyperlink ref="B435" r:id="rId386" xr:uid="{ECCE930A-B960-234C-81EC-4B8514282AE9}"/>
-    <hyperlink ref="B436" r:id="rId387" xr:uid="{7AA58141-7D24-7C42-A0C1-F852B21CFFD9}"/>
-    <hyperlink ref="B437" r:id="rId388" xr:uid="{B1FCB47D-7921-3446-B2C7-72CBA815D056}"/>
-    <hyperlink ref="B438" r:id="rId389" xr:uid="{8C547719-AA03-3543-B31F-7300674AF4C5}"/>
-    <hyperlink ref="B439" r:id="rId390" xr:uid="{09922668-AFC0-F242-860E-9967E0F0FEF4}"/>
-    <hyperlink ref="B440" r:id="rId391" xr:uid="{0DA963DA-238B-D44E-9E03-6E6BD933B35E}"/>
-    <hyperlink ref="B441" r:id="rId392" xr:uid="{89518AFF-2526-C845-BC9D-95FE77AF416E}"/>
-    <hyperlink ref="B442" r:id="rId393" xr:uid="{FAECBBBE-196C-7A41-A0FB-E0597CB2CF51}"/>
-    <hyperlink ref="B443" r:id="rId394" xr:uid="{8126B039-0B25-B040-A0F6-C3457341A2E9}"/>
-    <hyperlink ref="B444" r:id="rId395" xr:uid="{6CB326E6-E698-EB42-884B-C89FFA33E3BA}"/>
-    <hyperlink ref="B445" r:id="rId396" xr:uid="{8C97EFD1-933F-A44F-A1CF-6386233104A2}"/>
-    <hyperlink ref="B446" r:id="rId397" xr:uid="{8F019F07-8532-E147-8BE1-4EBE833F61CA}"/>
-    <hyperlink ref="B447" r:id="rId398" xr:uid="{00F1A08F-3767-784A-97A3-4603DE38BACC}"/>
-    <hyperlink ref="B448" r:id="rId399" xr:uid="{2A84ADCB-071F-9A48-994D-7A838307EFD8}"/>
-    <hyperlink ref="B449" r:id="rId400" xr:uid="{132F8C6D-D5E8-6440-AC4E-B81EA2100416}"/>
-    <hyperlink ref="B450" r:id="rId401" xr:uid="{2DA6EAC2-1A1D-754F-9613-226CBC7890AF}"/>
-    <hyperlink ref="B451" r:id="rId402" xr:uid="{05BED99A-4562-D14E-8627-D07CF5335A9B}"/>
-    <hyperlink ref="B452" r:id="rId403" xr:uid="{111D902A-3F60-2D4B-89D3-5BCBD8AA38DD}"/>
-    <hyperlink ref="B453" r:id="rId404" xr:uid="{F19236BE-AC32-3542-9214-DFC3BAE04ED0}"/>
-    <hyperlink ref="B454" r:id="rId405" xr:uid="{4D97CD96-EA1B-664E-9380-EFD27077D273}"/>
-    <hyperlink ref="B455" r:id="rId406" xr:uid="{49A46D91-633F-A148-ACFA-49B7D1AA4B33}"/>
-    <hyperlink ref="B456" r:id="rId407" xr:uid="{7C3B7901-67E3-EA4D-BC64-21A78BC03AC6}"/>
-    <hyperlink ref="B457" r:id="rId408" xr:uid="{B27CA8C3-D34F-5E4D-94A5-11D14AFD0F82}"/>
-    <hyperlink ref="B458" r:id="rId409" xr:uid="{8FECE038-9764-5E4A-8C6E-9B3209812651}"/>
-    <hyperlink ref="B459" r:id="rId410" xr:uid="{95696D4B-89CB-5640-BE92-53B3C043F7EB}"/>
-    <hyperlink ref="B460" r:id="rId411" xr:uid="{DA74B737-802A-4944-A93E-0B9C8417630B}"/>
-    <hyperlink ref="B461" r:id="rId412" xr:uid="{B2C4C168-50FA-AF41-8F56-9E70613CF17D}"/>
-    <hyperlink ref="B463" r:id="rId413" xr:uid="{B7090C60-AC27-3F4F-8F0D-42F0791928C6}"/>
-    <hyperlink ref="B462" r:id="rId414" xr:uid="{07400041-66C6-514B-B3E3-427F2947C2B7}"/>
-    <hyperlink ref="B464" r:id="rId415" xr:uid="{B7E78172-8FB8-4E42-87D8-6A4654D79C62}"/>
-    <hyperlink ref="B465" r:id="rId416" xr:uid="{9A5D4670-BC64-334A-88CF-6F8287692C5E}"/>
-    <hyperlink ref="B466" r:id="rId417" xr:uid="{604283B6-53BC-044F-8D9D-E6094E798317}"/>
-    <hyperlink ref="B467" r:id="rId418" xr:uid="{5EB15AC7-3E0E-E44C-A5B9-32F30F234B5A}"/>
-    <hyperlink ref="B468" r:id="rId419" xr:uid="{3076BD5F-4B23-4146-A50A-499C9FF4C3D2}"/>
-    <hyperlink ref="B469" r:id="rId420" xr:uid="{6A29D9C2-1E78-1B43-A251-0AB0A97FA70E}"/>
-    <hyperlink ref="B470" r:id="rId421" xr:uid="{00597D5E-D693-DF4E-84C0-47E58A6ACA8F}"/>
-    <hyperlink ref="B471" r:id="rId422" xr:uid="{48640988-9964-0B4C-A014-83E2CEB3D632}"/>
-    <hyperlink ref="B472" r:id="rId423" xr:uid="{617AADC9-7534-FE45-96B0-EF4C1867B793}"/>
-    <hyperlink ref="B473" r:id="rId424" xr:uid="{7F8CDAA4-5094-8E4E-961B-41CDE5ACC0C0}"/>
-    <hyperlink ref="B474" r:id="rId425" xr:uid="{63F28ABD-12CF-5947-80DA-229E3CA3133E}"/>
-    <hyperlink ref="B481" r:id="rId426" xr:uid="{0A1DB92C-3315-1942-B27D-4B90986A6D9D}"/>
-    <hyperlink ref="B480" r:id="rId427" xr:uid="{11738B67-CADD-5D45-8417-8BE7A03FC79F}"/>
-    <hyperlink ref="B479" r:id="rId428" xr:uid="{B2B23748-D9E4-BE4F-A93E-49ECB4063831}"/>
-    <hyperlink ref="B478" r:id="rId429" xr:uid="{A2FB8A72-37B9-7E4A-B050-FD6CD20BCE73}"/>
-    <hyperlink ref="B477" r:id="rId430" xr:uid="{5A93C9AF-BFEB-EB40-95AC-C309ED09A604}"/>
-    <hyperlink ref="B476" r:id="rId431" xr:uid="{CC203923-2DC2-874B-B846-A8455E3CC2F2}"/>
-    <hyperlink ref="B475" r:id="rId432" xr:uid="{FCB0246E-0179-B447-B3CE-C60CDB388472}"/>
-    <hyperlink ref="B484" r:id="rId433" xr:uid="{F06CEE72-8CA4-C547-862C-39B86CD3226A}"/>
-    <hyperlink ref="B485" r:id="rId434" xr:uid="{CB3045F2-8D63-0F4E-85BC-AF016DB4F247}"/>
-    <hyperlink ref="B486" r:id="rId435" xr:uid="{667D57F5-E5AD-674F-A2F5-AFF4A14E4026}"/>
-    <hyperlink ref="B487" r:id="rId436" xr:uid="{27A13A65-56CE-BF4D-BA0D-EB87D910272D}"/>
-    <hyperlink ref="B488" r:id="rId437" xr:uid="{2C72A52E-6F06-0246-AEB5-93CD0DEA8866}"/>
-    <hyperlink ref="B489" r:id="rId438" xr:uid="{24B29046-B4DD-674B-9EDF-6C94BEC3FDD8}"/>
-    <hyperlink ref="B490" r:id="rId439" xr:uid="{D018EBC3-3FB3-AC4D-9D64-D218345A46C8}"/>
-    <hyperlink ref="B493" r:id="rId440" xr:uid="{1E1D3964-01E0-3145-ACFE-B6A5BF0EECB0}"/>
-    <hyperlink ref="B491" r:id="rId441" xr:uid="{FA0E5061-A7E2-C045-9671-1CD9446D1932}"/>
-    <hyperlink ref="B492" r:id="rId442" location=":~:text=Given%20an%20integer%20n%2C%20calculate,*%2C%20%2F%20and%20pow().&amp;text=A%20Simple%20Solution%20is%20to%20repeatedly%20add%20n%20to%20result." xr:uid="{92704F5B-7B31-2F42-80DD-764B2206D9DB}"/>
+    <hyperlink ref="B392" r:id="rId346" xr:uid="{269338A6-5145-6944-9F7F-BD2A86DFA308}"/>
+    <hyperlink ref="B393" r:id="rId347" xr:uid="{8F583049-CE8D-CD42-88CD-CF3857942670}"/>
+    <hyperlink ref="B394" r:id="rId348" xr:uid="{EE2348AD-E296-894A-B5AE-5884A3C5E419}"/>
+    <hyperlink ref="B395" r:id="rId349" xr:uid="{6EACB34E-B32E-8F43-8055-2406F7417A7E}"/>
+    <hyperlink ref="B396" r:id="rId350" xr:uid="{2446F10A-B762-B64C-97B2-6131A0BECC1F}"/>
+    <hyperlink ref="B397" r:id="rId351" xr:uid="{6FDFCC53-17A6-7244-88A7-49406D7C9200}"/>
+    <hyperlink ref="B398" r:id="rId352" xr:uid="{3EC43646-EAB1-E443-A2F6-8E6E5FC77083}"/>
+    <hyperlink ref="B399" r:id="rId353" xr:uid="{659D9F20-C862-C947-B422-84143CFE317F}"/>
+    <hyperlink ref="B400" r:id="rId354" xr:uid="{3F5192FE-1C50-C049-88D5-68FA0F5430A0}"/>
+    <hyperlink ref="B401" r:id="rId355" xr:uid="{5EAD7CDA-9545-454B-BE77-9AFEC6AC1083}"/>
+    <hyperlink ref="B402" r:id="rId356" xr:uid="{761E5451-736B-6745-9CF5-4C6EF5D4C099}"/>
+    <hyperlink ref="B403" r:id="rId357" xr:uid="{4C8677A9-D94C-134F-AF31-E424751BF867}"/>
+    <hyperlink ref="B404" r:id="rId358" xr:uid="{CCF7920F-D5CE-004A-86C3-D821FB230970}"/>
+    <hyperlink ref="B405" r:id="rId359" xr:uid="{B4C07A0A-1EDD-7947-9646-3FD603441AD7}"/>
+    <hyperlink ref="B406" r:id="rId360" xr:uid="{49F7BB43-6851-0641-9DC5-27DBC66706F6}"/>
+    <hyperlink ref="B407" r:id="rId361" xr:uid="{77038647-48C7-5547-8E0F-898610362465}"/>
+    <hyperlink ref="B409" r:id="rId362" xr:uid="{EEFFE19C-6571-C64F-A0E1-5A4A700D94D4}"/>
+    <hyperlink ref="B408" r:id="rId363" xr:uid="{A4A2BFC4-6B88-2E4E-B362-17D8EE041C89}"/>
+    <hyperlink ref="B410" r:id="rId364" xr:uid="{DC5B603A-8D65-3648-A08A-E5FFA0FAE879}"/>
+    <hyperlink ref="B411" r:id="rId365" xr:uid="{F8807DD9-F4F2-B147-9C31-DBC93B2E477B}"/>
+    <hyperlink ref="B412" r:id="rId366" xr:uid="{6F7B396C-D7E9-C04E-BAE2-53D2EE07172B}"/>
+    <hyperlink ref="B415" r:id="rId367" xr:uid="{0D4A5941-C669-4A49-BAE3-9B553D03BD0F}"/>
+    <hyperlink ref="B416" r:id="rId368" xr:uid="{54144336-5BCA-D749-962A-E448C2CED3D3}"/>
+    <hyperlink ref="B417" r:id="rId369" xr:uid="{3A41DD21-CACF-1F48-A7C7-F568C6F31F3E}"/>
+    <hyperlink ref="B418" r:id="rId370" xr:uid="{A36160A8-F45E-3443-9645-42C1004B8F8C}"/>
+    <hyperlink ref="B419" r:id="rId371" xr:uid="{8B0A00A3-6AC0-DF46-AD87-A4DA016A2A00}"/>
+    <hyperlink ref="B420" r:id="rId372" xr:uid="{62A81CB4-A961-C543-B31C-92059DB6C105}"/>
+    <hyperlink ref="B423" r:id="rId373" xr:uid="{08030975-009C-C34A-A875-72FE2718F44C}"/>
+    <hyperlink ref="B424" r:id="rId374" xr:uid="{A113C7A9-2359-B643-9C08-E845813439C0}"/>
+    <hyperlink ref="B425" r:id="rId375" xr:uid="{FE300343-4633-AD47-A64D-2086629EB398}"/>
+    <hyperlink ref="B426" r:id="rId376" xr:uid="{4FC9F782-D38F-C642-A863-887B17AD05CD}"/>
+    <hyperlink ref="B427" r:id="rId377" xr:uid="{830C5466-10E3-7A48-B3E7-35C15A1CA4EF}"/>
+    <hyperlink ref="B428" r:id="rId378" xr:uid="{1B987077-E9D3-6F40-89EE-0D4E7180D884}"/>
+    <hyperlink ref="B429" r:id="rId379" xr:uid="{D4843E1F-7226-864E-A4BB-264D5A487B6D}"/>
+    <hyperlink ref="B430" r:id="rId380" xr:uid="{61816592-2D19-9946-8253-47A60218F2EA}"/>
+    <hyperlink ref="B431" r:id="rId381" xr:uid="{736C840F-19A3-0A4B-8863-ECB772B46385}"/>
+    <hyperlink ref="B432" r:id="rId382" xr:uid="{05A238AD-3C5B-C546-94E9-75BBF964711A}"/>
+    <hyperlink ref="B433" r:id="rId383" xr:uid="{7029629C-3F2A-4A49-997B-CFE86EC8B3C2}"/>
+    <hyperlink ref="B434" r:id="rId384" xr:uid="{ADA66B57-2FAC-AB42-BD83-4931708F3AB5}"/>
+    <hyperlink ref="B435" r:id="rId385" xr:uid="{F16BF1F9-755B-B045-B9A8-0B97E3BAC8B0}"/>
+    <hyperlink ref="B436" r:id="rId386" xr:uid="{ECCE930A-B960-234C-81EC-4B8514282AE9}"/>
+    <hyperlink ref="B437" r:id="rId387" xr:uid="{7AA58141-7D24-7C42-A0C1-F852B21CFFD9}"/>
+    <hyperlink ref="B438" r:id="rId388" xr:uid="{B1FCB47D-7921-3446-B2C7-72CBA815D056}"/>
+    <hyperlink ref="B439" r:id="rId389" xr:uid="{8C547719-AA03-3543-B31F-7300674AF4C5}"/>
+    <hyperlink ref="B440" r:id="rId390" xr:uid="{09922668-AFC0-F242-860E-9967E0F0FEF4}"/>
+    <hyperlink ref="B441" r:id="rId391" xr:uid="{0DA963DA-238B-D44E-9E03-6E6BD933B35E}"/>
+    <hyperlink ref="B442" r:id="rId392" xr:uid="{89518AFF-2526-C845-BC9D-95FE77AF416E}"/>
+    <hyperlink ref="B443" r:id="rId393" xr:uid="{FAECBBBE-196C-7A41-A0FB-E0597CB2CF51}"/>
+    <hyperlink ref="B444" r:id="rId394" xr:uid="{8126B039-0B25-B040-A0F6-C3457341A2E9}"/>
+    <hyperlink ref="B445" r:id="rId395" xr:uid="{6CB326E6-E698-EB42-884B-C89FFA33E3BA}"/>
+    <hyperlink ref="B446" r:id="rId396" xr:uid="{8C97EFD1-933F-A44F-A1CF-6386233104A2}"/>
+    <hyperlink ref="B447" r:id="rId397" xr:uid="{8F019F07-8532-E147-8BE1-4EBE833F61CA}"/>
+    <hyperlink ref="B448" r:id="rId398" xr:uid="{00F1A08F-3767-784A-97A3-4603DE38BACC}"/>
+    <hyperlink ref="B449" r:id="rId399" xr:uid="{2A84ADCB-071F-9A48-994D-7A838307EFD8}"/>
+    <hyperlink ref="B450" r:id="rId400" xr:uid="{132F8C6D-D5E8-6440-AC4E-B81EA2100416}"/>
+    <hyperlink ref="B451" r:id="rId401" xr:uid="{2DA6EAC2-1A1D-754F-9613-226CBC7890AF}"/>
+    <hyperlink ref="B452" r:id="rId402" xr:uid="{05BED99A-4562-D14E-8627-D07CF5335A9B}"/>
+    <hyperlink ref="B453" r:id="rId403" xr:uid="{111D902A-3F60-2D4B-89D3-5BCBD8AA38DD}"/>
+    <hyperlink ref="B454" r:id="rId404" xr:uid="{F19236BE-AC32-3542-9214-DFC3BAE04ED0}"/>
+    <hyperlink ref="B455" r:id="rId405" xr:uid="{4D97CD96-EA1B-664E-9380-EFD27077D273}"/>
+    <hyperlink ref="B456" r:id="rId406" xr:uid="{49A46D91-633F-A148-ACFA-49B7D1AA4B33}"/>
+    <hyperlink ref="B457" r:id="rId407" xr:uid="{7C3B7901-67E3-EA4D-BC64-21A78BC03AC6}"/>
+    <hyperlink ref="B458" r:id="rId408" xr:uid="{B27CA8C3-D34F-5E4D-94A5-11D14AFD0F82}"/>
+    <hyperlink ref="B459" r:id="rId409" xr:uid="{8FECE038-9764-5E4A-8C6E-9B3209812651}"/>
+    <hyperlink ref="B460" r:id="rId410" xr:uid="{95696D4B-89CB-5640-BE92-53B3C043F7EB}"/>
+    <hyperlink ref="B461" r:id="rId411" xr:uid="{DA74B737-802A-4944-A93E-0B9C8417630B}"/>
+    <hyperlink ref="B462" r:id="rId412" xr:uid="{B2C4C168-50FA-AF41-8F56-9E70613CF17D}"/>
+    <hyperlink ref="B464" r:id="rId413" xr:uid="{B7090C60-AC27-3F4F-8F0D-42F0791928C6}"/>
+    <hyperlink ref="B463" r:id="rId414" xr:uid="{07400041-66C6-514B-B3E3-427F2947C2B7}"/>
+    <hyperlink ref="B465" r:id="rId415" xr:uid="{B7E78172-8FB8-4E42-87D8-6A4654D79C62}"/>
+    <hyperlink ref="B466" r:id="rId416" xr:uid="{9A5D4670-BC64-334A-88CF-6F8287692C5E}"/>
+    <hyperlink ref="B467" r:id="rId417" xr:uid="{604283B6-53BC-044F-8D9D-E6094E798317}"/>
+    <hyperlink ref="B468" r:id="rId418" xr:uid="{5EB15AC7-3E0E-E44C-A5B9-32F30F234B5A}"/>
+    <hyperlink ref="B469" r:id="rId419" xr:uid="{3076BD5F-4B23-4146-A50A-499C9FF4C3D2}"/>
+    <hyperlink ref="B470" r:id="rId420" xr:uid="{6A29D9C2-1E78-1B43-A251-0AB0A97FA70E}"/>
+    <hyperlink ref="B471" r:id="rId421" xr:uid="{00597D5E-D693-DF4E-84C0-47E58A6ACA8F}"/>
+    <hyperlink ref="B472" r:id="rId422" xr:uid="{48640988-9964-0B4C-A014-83E2CEB3D632}"/>
+    <hyperlink ref="B473" r:id="rId423" xr:uid="{617AADC9-7534-FE45-96B0-EF4C1867B793}"/>
+    <hyperlink ref="B474" r:id="rId424" xr:uid="{7F8CDAA4-5094-8E4E-961B-41CDE5ACC0C0}"/>
+    <hyperlink ref="B475" r:id="rId425" xr:uid="{63F28ABD-12CF-5947-80DA-229E3CA3133E}"/>
+    <hyperlink ref="B482" r:id="rId426" xr:uid="{0A1DB92C-3315-1942-B27D-4B90986A6D9D}"/>
+    <hyperlink ref="B481" r:id="rId427" xr:uid="{11738B67-CADD-5D45-8417-8BE7A03FC79F}"/>
+    <hyperlink ref="B480" r:id="rId428" xr:uid="{B2B23748-D9E4-BE4F-A93E-49ECB4063831}"/>
+    <hyperlink ref="B479" r:id="rId429" xr:uid="{A2FB8A72-37B9-7E4A-B050-FD6CD20BCE73}"/>
+    <hyperlink ref="B478" r:id="rId430" xr:uid="{5A93C9AF-BFEB-EB40-95AC-C309ED09A604}"/>
+    <hyperlink ref="B477" r:id="rId431" xr:uid="{CC203923-2DC2-874B-B846-A8455E3CC2F2}"/>
+    <hyperlink ref="B476" r:id="rId432" xr:uid="{FCB0246E-0179-B447-B3CE-C60CDB388472}"/>
+    <hyperlink ref="B485" r:id="rId433" xr:uid="{F06CEE72-8CA4-C547-862C-39B86CD3226A}"/>
+    <hyperlink ref="B486" r:id="rId434" xr:uid="{CB3045F2-8D63-0F4E-85BC-AF016DB4F247}"/>
+    <hyperlink ref="B487" r:id="rId435" xr:uid="{667D57F5-E5AD-674F-A2F5-AFF4A14E4026}"/>
+    <hyperlink ref="B488" r:id="rId436" xr:uid="{27A13A65-56CE-BF4D-BA0D-EB87D910272D}"/>
+    <hyperlink ref="B489" r:id="rId437" xr:uid="{2C72A52E-6F06-0246-AEB5-93CD0DEA8866}"/>
+    <hyperlink ref="B490" r:id="rId438" xr:uid="{24B29046-B4DD-674B-9EDF-6C94BEC3FDD8}"/>
+    <hyperlink ref="B491" r:id="rId439" xr:uid="{D018EBC3-3FB3-AC4D-9D64-D218345A46C8}"/>
+    <hyperlink ref="B494" r:id="rId440" xr:uid="{1E1D3964-01E0-3145-ACFE-B6A5BF0EECB0}"/>
+    <hyperlink ref="B492" r:id="rId441" xr:uid="{FA0E5061-A7E2-C045-9671-1CD9446D1932}"/>
+    <hyperlink ref="B493" r:id="rId442" location=":~:text=Given%20an%20integer%20n%2C%20calculate,*%2C%20%2F%20and%20pow().&amp;text=A%20Simple%20Solution%20is%20to%20repeatedly%20add%20n%20to%20result." xr:uid="{92704F5B-7B31-2F42-80DD-764B2206D9DB}"/>
     <hyperlink ref="B368" r:id="rId443" xr:uid="{A48B1A24-83B1-7A4C-8129-CD37804DF849}"/>
     <hyperlink ref="B2" r:id="rId444" xr:uid="{E07D4FE5-46C7-AC4D-9E01-2300AA43B58A}"/>
     <hyperlink ref="B39" r:id="rId445" xr:uid="{F2DE2162-BD02-7549-AC1A-27455F78131F}"/>
@@ -7733,8 +7747,9 @@
     <hyperlink ref="B327" r:id="rId456" xr:uid="{AFA4A056-B723-4AB3-9153-0CC7FBCA9ED5}"/>
     <hyperlink ref="B339" r:id="rId457" xr:uid="{F8CC22D8-AF7C-48B1-8C17-A071BF5C7F07}"/>
     <hyperlink ref="B185" r:id="rId458" xr:uid="{AEB61F80-6C73-454E-98EC-F97D434F5EB5}"/>
+    <hyperlink ref="B391" r:id="rId459" xr:uid="{FF5FD771-6B03-42F1-BD02-B7B19A3A0362}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId459"/>
+  <pageSetup orientation="portrait" r:id="rId460"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Shortest Path in Directed Acyclic Graph
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harsh\Desktop\Data-Structures-and-Algorithms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A66F039-736B-4019-A5FD-315C5A239DD3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E0E1B1C-1CD6-4E7F-9DE5-7A7031AAEE05}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1409" uniqueCount="493">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1412" uniqueCount="494">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1504,6 +1504,9 @@
   </si>
   <si>
     <t>Possible Bipartition</t>
+  </si>
+  <si>
+    <t>Shortest Path in Directed Acyclic Graph</t>
   </si>
 </sst>
 </file>
@@ -2030,9 +2033,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
-  <dimension ref="A1:D495"/>
+  <dimension ref="A1:D496"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A394" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A390" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="B399" sqref="B399"/>
     </sheetView>
   </sheetViews>
@@ -6280,10 +6283,10 @@
         <v>342</v>
       </c>
       <c r="B399" s="6" t="s">
-        <v>372</v>
-      </c>
-      <c r="C399" s="4" t="s">
-        <v>4</v>
+        <v>493</v>
+      </c>
+      <c r="C399" s="11" t="s">
+        <v>464</v>
       </c>
     </row>
     <row r="400" spans="1:3" ht="21">
@@ -6291,7 +6294,7 @@
         <v>342</v>
       </c>
       <c r="B400" s="6" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C400" s="4" t="s">
         <v>4</v>
@@ -6302,7 +6305,7 @@
         <v>342</v>
       </c>
       <c r="B401" s="6" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C401" s="4" t="s">
         <v>4</v>
@@ -6313,7 +6316,7 @@
         <v>342</v>
       </c>
       <c r="B402" s="6" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C402" s="4" t="s">
         <v>4</v>
@@ -6324,7 +6327,7 @@
         <v>342</v>
       </c>
       <c r="B403" s="6" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="C403" s="4" t="s">
         <v>4</v>
@@ -6346,7 +6349,7 @@
         <v>342</v>
       </c>
       <c r="B405" s="6" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="C405" s="4" t="s">
         <v>4</v>
@@ -6357,10 +6360,10 @@
         <v>342</v>
       </c>
       <c r="B406" s="6" t="s">
-        <v>378</v>
-      </c>
-      <c r="C406" s="11" t="s">
-        <v>464</v>
+        <v>377</v>
+      </c>
+      <c r="C406" s="4" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="407" spans="1:3" ht="21">
@@ -6368,10 +6371,10 @@
         <v>342</v>
       </c>
       <c r="B407" s="6" t="s">
-        <v>379</v>
-      </c>
-      <c r="C407" s="4" t="s">
-        <v>4</v>
+        <v>378</v>
+      </c>
+      <c r="C407" s="11" t="s">
+        <v>464</v>
       </c>
     </row>
     <row r="408" spans="1:3" ht="21">
@@ -6379,7 +6382,7 @@
         <v>342</v>
       </c>
       <c r="B408" s="6" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="C408" s="4" t="s">
         <v>4</v>
@@ -6390,7 +6393,7 @@
         <v>342</v>
       </c>
       <c r="B409" s="6" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C409" s="4" t="s">
         <v>4</v>
@@ -6401,7 +6404,7 @@
         <v>342</v>
       </c>
       <c r="B410" s="6" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="C410" s="4" t="s">
         <v>4</v>
@@ -6412,7 +6415,7 @@
         <v>342</v>
       </c>
       <c r="B411" s="6" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="C411" s="4" t="s">
         <v>4</v>
@@ -6423,7 +6426,7 @@
         <v>342</v>
       </c>
       <c r="B412" s="6" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="C412" s="4" t="s">
         <v>4</v>
@@ -6434,37 +6437,37 @@
         <v>342</v>
       </c>
       <c r="B413" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="C413" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="414" spans="1:3" ht="21">
+      <c r="A414" s="8" t="s">
+        <v>342</v>
+      </c>
+      <c r="B414" s="6" t="s">
         <v>385</v>
       </c>
-      <c r="C413" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="414" spans="1:3" ht="21">
-      <c r="B414" s="7"/>
-      <c r="C414" s="4"/>
+      <c r="C414" s="4" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="415" spans="1:3" ht="21">
       <c r="B415" s="7"/>
       <c r="C415" s="4"/>
     </row>
     <row r="416" spans="1:3" ht="21">
-      <c r="A416" s="8" t="s">
-        <v>386</v>
-      </c>
-      <c r="B416" s="6" t="s">
-        <v>387</v>
-      </c>
-      <c r="C416" s="4" t="s">
-        <v>4</v>
-      </c>
+      <c r="B416" s="7"/>
+      <c r="C416" s="4"/>
     </row>
     <row r="417" spans="1:3" ht="21">
       <c r="A417" s="8" t="s">
         <v>386</v>
       </c>
       <c r="B417" s="6" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="C417" s="4" t="s">
         <v>4</v>
@@ -6475,7 +6478,7 @@
         <v>386</v>
       </c>
       <c r="B418" s="6" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="C418" s="4" t="s">
         <v>4</v>
@@ -6486,7 +6489,7 @@
         <v>386</v>
       </c>
       <c r="B419" s="6" t="s">
-        <v>89</v>
+        <v>389</v>
       </c>
       <c r="C419" s="4" t="s">
         <v>4</v>
@@ -6497,7 +6500,7 @@
         <v>386</v>
       </c>
       <c r="B420" s="6" t="s">
-        <v>390</v>
+        <v>89</v>
       </c>
       <c r="C420" s="4" t="s">
         <v>4</v>
@@ -6508,37 +6511,37 @@
         <v>386</v>
       </c>
       <c r="B421" s="6" t="s">
+        <v>390</v>
+      </c>
+      <c r="C421" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="422" spans="1:3" ht="21">
+      <c r="A422" s="8" t="s">
+        <v>386</v>
+      </c>
+      <c r="B422" s="6" t="s">
         <v>391</v>
       </c>
-      <c r="C421" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="422" spans="1:3" ht="21">
-      <c r="B422" s="7"/>
-      <c r="C422" s="4"/>
+      <c r="C422" s="4" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="423" spans="1:3" ht="21">
       <c r="B423" s="7"/>
       <c r="C423" s="4"/>
     </row>
     <row r="424" spans="1:3" ht="21">
-      <c r="A424" s="5" t="s">
-        <v>392</v>
-      </c>
-      <c r="B424" s="6" t="s">
-        <v>393</v>
-      </c>
-      <c r="C424" s="4" t="s">
-        <v>4</v>
-      </c>
+      <c r="B424" s="7"/>
+      <c r="C424" s="4"/>
     </row>
     <row r="425" spans="1:3" ht="21">
       <c r="A425" s="5" t="s">
         <v>392</v>
       </c>
       <c r="B425" s="6" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="C425" s="4" t="s">
         <v>4</v>
@@ -6549,7 +6552,7 @@
         <v>392</v>
       </c>
       <c r="B426" s="6" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C426" s="4" t="s">
         <v>4</v>
@@ -6560,7 +6563,7 @@
         <v>392</v>
       </c>
       <c r="B427" s="6" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="C427" s="4" t="s">
         <v>4</v>
@@ -6571,7 +6574,7 @@
         <v>392</v>
       </c>
       <c r="B428" s="6" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="C428" s="4" t="s">
         <v>4</v>
@@ -6582,7 +6585,7 @@
         <v>392</v>
       </c>
       <c r="B429" s="6" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="C429" s="4" t="s">
         <v>4</v>
@@ -6593,7 +6596,7 @@
         <v>392</v>
       </c>
       <c r="B430" s="6" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="C430" s="4" t="s">
         <v>4</v>
@@ -6604,7 +6607,7 @@
         <v>392</v>
       </c>
       <c r="B431" s="6" t="s">
-        <v>272</v>
+        <v>399</v>
       </c>
       <c r="C431" s="4" t="s">
         <v>4</v>
@@ -6615,7 +6618,7 @@
         <v>392</v>
       </c>
       <c r="B432" s="6" t="s">
-        <v>400</v>
+        <v>272</v>
       </c>
       <c r="C432" s="4" t="s">
         <v>4</v>
@@ -6626,7 +6629,7 @@
         <v>392</v>
       </c>
       <c r="B433" s="6" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="C433" s="4" t="s">
         <v>4</v>
@@ -6637,7 +6640,7 @@
         <v>392</v>
       </c>
       <c r="B434" s="6" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="C434" s="4" t="s">
         <v>4</v>
@@ -6648,7 +6651,7 @@
         <v>392</v>
       </c>
       <c r="B435" s="6" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="C435" s="4" t="s">
         <v>4</v>
@@ -6659,7 +6662,7 @@
         <v>392</v>
       </c>
       <c r="B436" s="6" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="C436" s="4" t="s">
         <v>4</v>
@@ -6670,7 +6673,7 @@
         <v>392</v>
       </c>
       <c r="B437" s="6" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="C437" s="4" t="s">
         <v>4</v>
@@ -6681,7 +6684,7 @@
         <v>392</v>
       </c>
       <c r="B438" s="6" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="C438" s="4" t="s">
         <v>4</v>
@@ -6692,7 +6695,7 @@
         <v>392</v>
       </c>
       <c r="B439" s="6" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="C439" s="4" t="s">
         <v>4</v>
@@ -6703,7 +6706,7 @@
         <v>392</v>
       </c>
       <c r="B440" s="6" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="C440" s="4" t="s">
         <v>4</v>
@@ -6714,7 +6717,7 @@
         <v>392</v>
       </c>
       <c r="B441" s="6" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="C441" s="4" t="s">
         <v>4</v>
@@ -6725,7 +6728,7 @@
         <v>392</v>
       </c>
       <c r="B442" s="6" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="C442" s="4" t="s">
         <v>4</v>
@@ -6736,7 +6739,7 @@
         <v>392</v>
       </c>
       <c r="B443" s="6" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="C443" s="4" t="s">
         <v>4</v>
@@ -6747,7 +6750,7 @@
         <v>392</v>
       </c>
       <c r="B444" s="6" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C444" s="4" t="s">
         <v>4</v>
@@ -6758,7 +6761,7 @@
         <v>392</v>
       </c>
       <c r="B445" s="6" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="C445" s="4" t="s">
         <v>4</v>
@@ -6769,7 +6772,7 @@
         <v>392</v>
       </c>
       <c r="B446" s="6" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C446" s="4" t="s">
         <v>4</v>
@@ -6780,7 +6783,7 @@
         <v>392</v>
       </c>
       <c r="B447" s="6" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C447" s="4" t="s">
         <v>4</v>
@@ -6791,7 +6794,7 @@
         <v>392</v>
       </c>
       <c r="B448" s="6" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C448" s="4" t="s">
         <v>4</v>
@@ -6802,7 +6805,7 @@
         <v>392</v>
       </c>
       <c r="B449" s="6" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C449" s="4" t="s">
         <v>4</v>
@@ -6813,7 +6816,7 @@
         <v>392</v>
       </c>
       <c r="B450" s="6" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="C450" s="4" t="s">
         <v>4</v>
@@ -6824,7 +6827,7 @@
         <v>392</v>
       </c>
       <c r="B451" s="6" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="C451" s="4" t="s">
         <v>4</v>
@@ -6835,7 +6838,7 @@
         <v>392</v>
       </c>
       <c r="B452" s="6" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="C452" s="4" t="s">
         <v>4</v>
@@ -6846,7 +6849,7 @@
         <v>392</v>
       </c>
       <c r="B453" s="6" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="C453" s="4" t="s">
         <v>4</v>
@@ -6857,7 +6860,7 @@
         <v>392</v>
       </c>
       <c r="B454" s="6" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="C454" s="4" t="s">
         <v>4</v>
@@ -6868,7 +6871,7 @@
         <v>392</v>
       </c>
       <c r="B455" s="6" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="C455" s="4" t="s">
         <v>4</v>
@@ -6879,7 +6882,7 @@
         <v>392</v>
       </c>
       <c r="B456" s="6" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="C456" s="4" t="s">
         <v>4</v>
@@ -6890,7 +6893,7 @@
         <v>392</v>
       </c>
       <c r="B457" s="6" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C457" s="4" t="s">
         <v>4</v>
@@ -6901,7 +6904,7 @@
         <v>392</v>
       </c>
       <c r="B458" s="6" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="C458" s="4" t="s">
         <v>4</v>
@@ -6912,7 +6915,7 @@
         <v>392</v>
       </c>
       <c r="B459" s="6" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="C459" s="4" t="s">
         <v>4</v>
@@ -6923,7 +6926,7 @@
         <v>392</v>
       </c>
       <c r="B460" s="6" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="C460" s="4" t="s">
         <v>4</v>
@@ -6934,7 +6937,7 @@
         <v>392</v>
       </c>
       <c r="B461" s="6" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="C461" s="4" t="s">
         <v>4</v>
@@ -6945,7 +6948,7 @@
         <v>392</v>
       </c>
       <c r="B462" s="6" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="C462" s="4" t="s">
         <v>4</v>
@@ -6956,7 +6959,7 @@
         <v>392</v>
       </c>
       <c r="B463" s="6" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C463" s="4" t="s">
         <v>4</v>
@@ -6967,7 +6970,7 @@
         <v>392</v>
       </c>
       <c r="B464" s="6" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="C464" s="4" t="s">
         <v>4</v>
@@ -6978,7 +6981,7 @@
         <v>392</v>
       </c>
       <c r="B465" s="6" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C465" s="4" t="s">
         <v>4</v>
@@ -6989,7 +6992,7 @@
         <v>392</v>
       </c>
       <c r="B466" s="6" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C466" s="4" t="s">
         <v>4</v>
@@ -7000,7 +7003,7 @@
         <v>392</v>
       </c>
       <c r="B467" s="6" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="C467" s="4" t="s">
         <v>4</v>
@@ -7011,7 +7014,7 @@
         <v>392</v>
       </c>
       <c r="B468" s="6" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="C468" s="4" t="s">
         <v>4</v>
@@ -7022,7 +7025,7 @@
         <v>392</v>
       </c>
       <c r="B469" s="6" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="C469" s="4" t="s">
         <v>4</v>
@@ -7033,7 +7036,7 @@
         <v>392</v>
       </c>
       <c r="B470" s="6" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="C470" s="4" t="s">
         <v>4</v>
@@ -7044,7 +7047,7 @@
         <v>392</v>
       </c>
       <c r="B471" s="6" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="C471" s="4" t="s">
         <v>4</v>
@@ -7055,7 +7058,7 @@
         <v>392</v>
       </c>
       <c r="B472" s="6" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="C472" s="4" t="s">
         <v>4</v>
@@ -7066,7 +7069,7 @@
         <v>392</v>
       </c>
       <c r="B473" s="6" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="C473" s="4" t="s">
         <v>4</v>
@@ -7077,7 +7080,7 @@
         <v>392</v>
       </c>
       <c r="B474" s="6" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="C474" s="4" t="s">
         <v>4</v>
@@ -7088,7 +7091,7 @@
         <v>392</v>
       </c>
       <c r="B475" s="6" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="C475" s="4" t="s">
         <v>4</v>
@@ -7099,7 +7102,7 @@
         <v>392</v>
       </c>
       <c r="B476" s="6" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="C476" s="4" t="s">
         <v>4</v>
@@ -7110,7 +7113,7 @@
         <v>392</v>
       </c>
       <c r="B477" s="6" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="C477" s="4" t="s">
         <v>4</v>
@@ -7121,7 +7124,7 @@
         <v>392</v>
       </c>
       <c r="B478" s="6" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="C478" s="4" t="s">
         <v>4</v>
@@ -7132,7 +7135,7 @@
         <v>392</v>
       </c>
       <c r="B479" s="6" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="C479" s="4" t="s">
         <v>4</v>
@@ -7143,7 +7146,7 @@
         <v>392</v>
       </c>
       <c r="B480" s="6" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="C480" s="4" t="s">
         <v>4</v>
@@ -7154,7 +7157,7 @@
         <v>392</v>
       </c>
       <c r="B481" s="6" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="C481" s="4" t="s">
         <v>4</v>
@@ -7165,7 +7168,7 @@
         <v>392</v>
       </c>
       <c r="B482" s="6" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="C482" s="4" t="s">
         <v>4</v>
@@ -7176,38 +7179,38 @@
         <v>392</v>
       </c>
       <c r="B483" s="6" t="s">
+        <v>450</v>
+      </c>
+      <c r="C483" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="484" spans="1:3" ht="21">
+      <c r="A484" s="5" t="s">
+        <v>392</v>
+      </c>
+      <c r="B484" s="6" t="s">
         <v>451</v>
       </c>
-      <c r="C483" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="484" spans="1:3" ht="21">
-      <c r="B484" s="7"/>
-      <c r="C484" s="4"/>
+      <c r="C484" s="4" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="485" spans="1:3" ht="21">
-      <c r="A485" s="8"/>
       <c r="B485" s="7"/>
       <c r="C485" s="4"/>
     </row>
     <row r="486" spans="1:3" ht="21">
-      <c r="A486" s="5" t="s">
-        <v>452</v>
-      </c>
-      <c r="B486" s="6" t="s">
-        <v>453</v>
-      </c>
-      <c r="C486" s="4" t="s">
-        <v>4</v>
-      </c>
+      <c r="A486" s="8"/>
+      <c r="B486" s="7"/>
+      <c r="C486" s="4"/>
     </row>
     <row r="487" spans="1:3" ht="21">
       <c r="A487" s="5" t="s">
         <v>452</v>
       </c>
       <c r="B487" s="6" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="C487" s="4" t="s">
         <v>4</v>
@@ -7218,7 +7221,7 @@
         <v>452</v>
       </c>
       <c r="B488" s="6" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="C488" s="4" t="s">
         <v>4</v>
@@ -7229,7 +7232,7 @@
         <v>452</v>
       </c>
       <c r="B489" s="6" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="C489" s="4" t="s">
         <v>4</v>
@@ -7240,7 +7243,7 @@
         <v>452</v>
       </c>
       <c r="B490" s="6" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="C490" s="4" t="s">
         <v>4</v>
@@ -7251,7 +7254,7 @@
         <v>452</v>
       </c>
       <c r="B491" s="6" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="C491" s="4" t="s">
         <v>4</v>
@@ -7262,7 +7265,7 @@
         <v>452</v>
       </c>
       <c r="B492" s="6" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="C492" s="4" t="s">
         <v>4</v>
@@ -7273,7 +7276,7 @@
         <v>452</v>
       </c>
       <c r="B493" s="6" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="C493" s="4" t="s">
         <v>4</v>
@@ -7284,7 +7287,7 @@
         <v>452</v>
       </c>
       <c r="B494" s="6" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="C494" s="4" t="s">
         <v>4</v>
@@ -7295,9 +7298,20 @@
         <v>452</v>
       </c>
       <c r="B495" s="6" t="s">
+        <v>461</v>
+      </c>
+      <c r="C495" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="496" spans="1:3" ht="21">
+      <c r="A496" s="5" t="s">
+        <v>452</v>
+      </c>
+      <c r="B496" s="6" t="s">
         <v>462</v>
       </c>
-      <c r="C495" s="4" t="s">
+      <c r="C496" s="4" t="s">
         <v>4</v>
       </c>
     </row>
@@ -7654,97 +7668,97 @@
     <hyperlink ref="B396" r:id="rId349" xr:uid="{6EACB34E-B32E-8F43-8055-2406F7417A7E}"/>
     <hyperlink ref="B397" r:id="rId350" xr:uid="{2446F10A-B762-B64C-97B2-6131A0BECC1F}"/>
     <hyperlink ref="B398" r:id="rId351" xr:uid="{6FDFCC53-17A6-7244-88A7-49406D7C9200}"/>
-    <hyperlink ref="B399" r:id="rId352" xr:uid="{3EC43646-EAB1-E443-A2F6-8E6E5FC77083}"/>
-    <hyperlink ref="B400" r:id="rId353" xr:uid="{659D9F20-C862-C947-B422-84143CFE317F}"/>
-    <hyperlink ref="B401" r:id="rId354" xr:uid="{3F5192FE-1C50-C049-88D5-68FA0F5430A0}"/>
-    <hyperlink ref="B402" r:id="rId355" xr:uid="{5EAD7CDA-9545-454B-BE77-9AFEC6AC1083}"/>
-    <hyperlink ref="B403" r:id="rId356" xr:uid="{761E5451-736B-6745-9CF5-4C6EF5D4C099}"/>
-    <hyperlink ref="B404" r:id="rId357" xr:uid="{4C8677A9-D94C-134F-AF31-E424751BF867}"/>
-    <hyperlink ref="B405" r:id="rId358" xr:uid="{CCF7920F-D5CE-004A-86C3-D821FB230970}"/>
-    <hyperlink ref="B406" r:id="rId359" xr:uid="{B4C07A0A-1EDD-7947-9646-3FD603441AD7}"/>
-    <hyperlink ref="B407" r:id="rId360" xr:uid="{49F7BB43-6851-0641-9DC5-27DBC66706F6}"/>
-    <hyperlink ref="B408" r:id="rId361" xr:uid="{77038647-48C7-5547-8E0F-898610362465}"/>
-    <hyperlink ref="B410" r:id="rId362" xr:uid="{EEFFE19C-6571-C64F-A0E1-5A4A700D94D4}"/>
-    <hyperlink ref="B409" r:id="rId363" xr:uid="{A4A2BFC4-6B88-2E4E-B362-17D8EE041C89}"/>
-    <hyperlink ref="B411" r:id="rId364" xr:uid="{DC5B603A-8D65-3648-A08A-E5FFA0FAE879}"/>
-    <hyperlink ref="B412" r:id="rId365" xr:uid="{F8807DD9-F4F2-B147-9C31-DBC93B2E477B}"/>
-    <hyperlink ref="B413" r:id="rId366" xr:uid="{6F7B396C-D7E9-C04E-BAE2-53D2EE07172B}"/>
-    <hyperlink ref="B416" r:id="rId367" xr:uid="{0D4A5941-C669-4A49-BAE3-9B553D03BD0F}"/>
-    <hyperlink ref="B417" r:id="rId368" xr:uid="{54144336-5BCA-D749-962A-E448C2CED3D3}"/>
-    <hyperlink ref="B418" r:id="rId369" xr:uid="{3A41DD21-CACF-1F48-A7C7-F568C6F31F3E}"/>
-    <hyperlink ref="B419" r:id="rId370" xr:uid="{A36160A8-F45E-3443-9645-42C1004B8F8C}"/>
-    <hyperlink ref="B420" r:id="rId371" xr:uid="{8B0A00A3-6AC0-DF46-AD87-A4DA016A2A00}"/>
-    <hyperlink ref="B421" r:id="rId372" xr:uid="{62A81CB4-A961-C543-B31C-92059DB6C105}"/>
-    <hyperlink ref="B424" r:id="rId373" xr:uid="{08030975-009C-C34A-A875-72FE2718F44C}"/>
-    <hyperlink ref="B425" r:id="rId374" xr:uid="{A113C7A9-2359-B643-9C08-E845813439C0}"/>
-    <hyperlink ref="B426" r:id="rId375" xr:uid="{FE300343-4633-AD47-A64D-2086629EB398}"/>
-    <hyperlink ref="B427" r:id="rId376" xr:uid="{4FC9F782-D38F-C642-A863-887B17AD05CD}"/>
-    <hyperlink ref="B428" r:id="rId377" xr:uid="{830C5466-10E3-7A48-B3E7-35C15A1CA4EF}"/>
-    <hyperlink ref="B429" r:id="rId378" xr:uid="{1B987077-E9D3-6F40-89EE-0D4E7180D884}"/>
-    <hyperlink ref="B430" r:id="rId379" xr:uid="{D4843E1F-7226-864E-A4BB-264D5A487B6D}"/>
-    <hyperlink ref="B431" r:id="rId380" xr:uid="{61816592-2D19-9946-8253-47A60218F2EA}"/>
-    <hyperlink ref="B432" r:id="rId381" xr:uid="{736C840F-19A3-0A4B-8863-ECB772B46385}"/>
-    <hyperlink ref="B433" r:id="rId382" xr:uid="{05A238AD-3C5B-C546-94E9-75BBF964711A}"/>
-    <hyperlink ref="B434" r:id="rId383" xr:uid="{7029629C-3F2A-4A49-997B-CFE86EC8B3C2}"/>
-    <hyperlink ref="B435" r:id="rId384" xr:uid="{ADA66B57-2FAC-AB42-BD83-4931708F3AB5}"/>
-    <hyperlink ref="B436" r:id="rId385" xr:uid="{F16BF1F9-755B-B045-B9A8-0B97E3BAC8B0}"/>
-    <hyperlink ref="B437" r:id="rId386" xr:uid="{ECCE930A-B960-234C-81EC-4B8514282AE9}"/>
-    <hyperlink ref="B438" r:id="rId387" xr:uid="{7AA58141-7D24-7C42-A0C1-F852B21CFFD9}"/>
-    <hyperlink ref="B439" r:id="rId388" xr:uid="{B1FCB47D-7921-3446-B2C7-72CBA815D056}"/>
-    <hyperlink ref="B440" r:id="rId389" xr:uid="{8C547719-AA03-3543-B31F-7300674AF4C5}"/>
-    <hyperlink ref="B441" r:id="rId390" xr:uid="{09922668-AFC0-F242-860E-9967E0F0FEF4}"/>
-    <hyperlink ref="B442" r:id="rId391" xr:uid="{0DA963DA-238B-D44E-9E03-6E6BD933B35E}"/>
-    <hyperlink ref="B443" r:id="rId392" xr:uid="{89518AFF-2526-C845-BC9D-95FE77AF416E}"/>
-    <hyperlink ref="B444" r:id="rId393" xr:uid="{FAECBBBE-196C-7A41-A0FB-E0597CB2CF51}"/>
-    <hyperlink ref="B445" r:id="rId394" xr:uid="{8126B039-0B25-B040-A0F6-C3457341A2E9}"/>
-    <hyperlink ref="B446" r:id="rId395" xr:uid="{6CB326E6-E698-EB42-884B-C89FFA33E3BA}"/>
-    <hyperlink ref="B447" r:id="rId396" xr:uid="{8C97EFD1-933F-A44F-A1CF-6386233104A2}"/>
-    <hyperlink ref="B448" r:id="rId397" xr:uid="{8F019F07-8532-E147-8BE1-4EBE833F61CA}"/>
-    <hyperlink ref="B449" r:id="rId398" xr:uid="{00F1A08F-3767-784A-97A3-4603DE38BACC}"/>
-    <hyperlink ref="B450" r:id="rId399" xr:uid="{2A84ADCB-071F-9A48-994D-7A838307EFD8}"/>
-    <hyperlink ref="B451" r:id="rId400" xr:uid="{132F8C6D-D5E8-6440-AC4E-B81EA2100416}"/>
-    <hyperlink ref="B452" r:id="rId401" xr:uid="{2DA6EAC2-1A1D-754F-9613-226CBC7890AF}"/>
-    <hyperlink ref="B453" r:id="rId402" xr:uid="{05BED99A-4562-D14E-8627-D07CF5335A9B}"/>
-    <hyperlink ref="B454" r:id="rId403" xr:uid="{111D902A-3F60-2D4B-89D3-5BCBD8AA38DD}"/>
-    <hyperlink ref="B455" r:id="rId404" xr:uid="{F19236BE-AC32-3542-9214-DFC3BAE04ED0}"/>
-    <hyperlink ref="B456" r:id="rId405" xr:uid="{4D97CD96-EA1B-664E-9380-EFD27077D273}"/>
-    <hyperlink ref="B457" r:id="rId406" xr:uid="{49A46D91-633F-A148-ACFA-49B7D1AA4B33}"/>
-    <hyperlink ref="B458" r:id="rId407" xr:uid="{7C3B7901-67E3-EA4D-BC64-21A78BC03AC6}"/>
-    <hyperlink ref="B459" r:id="rId408" xr:uid="{B27CA8C3-D34F-5E4D-94A5-11D14AFD0F82}"/>
-    <hyperlink ref="B460" r:id="rId409" xr:uid="{8FECE038-9764-5E4A-8C6E-9B3209812651}"/>
-    <hyperlink ref="B461" r:id="rId410" xr:uid="{95696D4B-89CB-5640-BE92-53B3C043F7EB}"/>
-    <hyperlink ref="B462" r:id="rId411" xr:uid="{DA74B737-802A-4944-A93E-0B9C8417630B}"/>
-    <hyperlink ref="B463" r:id="rId412" xr:uid="{B2C4C168-50FA-AF41-8F56-9E70613CF17D}"/>
-    <hyperlink ref="B465" r:id="rId413" xr:uid="{B7090C60-AC27-3F4F-8F0D-42F0791928C6}"/>
-    <hyperlink ref="B464" r:id="rId414" xr:uid="{07400041-66C6-514B-B3E3-427F2947C2B7}"/>
-    <hyperlink ref="B466" r:id="rId415" xr:uid="{B7E78172-8FB8-4E42-87D8-6A4654D79C62}"/>
-    <hyperlink ref="B467" r:id="rId416" xr:uid="{9A5D4670-BC64-334A-88CF-6F8287692C5E}"/>
-    <hyperlink ref="B468" r:id="rId417" xr:uid="{604283B6-53BC-044F-8D9D-E6094E798317}"/>
-    <hyperlink ref="B469" r:id="rId418" xr:uid="{5EB15AC7-3E0E-E44C-A5B9-32F30F234B5A}"/>
-    <hyperlink ref="B470" r:id="rId419" xr:uid="{3076BD5F-4B23-4146-A50A-499C9FF4C3D2}"/>
-    <hyperlink ref="B471" r:id="rId420" xr:uid="{6A29D9C2-1E78-1B43-A251-0AB0A97FA70E}"/>
-    <hyperlink ref="B472" r:id="rId421" xr:uid="{00597D5E-D693-DF4E-84C0-47E58A6ACA8F}"/>
-    <hyperlink ref="B473" r:id="rId422" xr:uid="{48640988-9964-0B4C-A014-83E2CEB3D632}"/>
-    <hyperlink ref="B474" r:id="rId423" xr:uid="{617AADC9-7534-FE45-96B0-EF4C1867B793}"/>
-    <hyperlink ref="B475" r:id="rId424" xr:uid="{7F8CDAA4-5094-8E4E-961B-41CDE5ACC0C0}"/>
-    <hyperlink ref="B476" r:id="rId425" xr:uid="{63F28ABD-12CF-5947-80DA-229E3CA3133E}"/>
-    <hyperlink ref="B483" r:id="rId426" xr:uid="{0A1DB92C-3315-1942-B27D-4B90986A6D9D}"/>
-    <hyperlink ref="B482" r:id="rId427" xr:uid="{11738B67-CADD-5D45-8417-8BE7A03FC79F}"/>
-    <hyperlink ref="B481" r:id="rId428" xr:uid="{B2B23748-D9E4-BE4F-A93E-49ECB4063831}"/>
-    <hyperlink ref="B480" r:id="rId429" xr:uid="{A2FB8A72-37B9-7E4A-B050-FD6CD20BCE73}"/>
-    <hyperlink ref="B479" r:id="rId430" xr:uid="{5A93C9AF-BFEB-EB40-95AC-C309ED09A604}"/>
-    <hyperlink ref="B478" r:id="rId431" xr:uid="{CC203923-2DC2-874B-B846-A8455E3CC2F2}"/>
-    <hyperlink ref="B477" r:id="rId432" xr:uid="{FCB0246E-0179-B447-B3CE-C60CDB388472}"/>
-    <hyperlink ref="B486" r:id="rId433" xr:uid="{F06CEE72-8CA4-C547-862C-39B86CD3226A}"/>
-    <hyperlink ref="B487" r:id="rId434" xr:uid="{CB3045F2-8D63-0F4E-85BC-AF016DB4F247}"/>
-    <hyperlink ref="B488" r:id="rId435" xr:uid="{667D57F5-E5AD-674F-A2F5-AFF4A14E4026}"/>
-    <hyperlink ref="B489" r:id="rId436" xr:uid="{27A13A65-56CE-BF4D-BA0D-EB87D910272D}"/>
-    <hyperlink ref="B490" r:id="rId437" xr:uid="{2C72A52E-6F06-0246-AEB5-93CD0DEA8866}"/>
-    <hyperlink ref="B491" r:id="rId438" xr:uid="{24B29046-B4DD-674B-9EDF-6C94BEC3FDD8}"/>
-    <hyperlink ref="B492" r:id="rId439" xr:uid="{D018EBC3-3FB3-AC4D-9D64-D218345A46C8}"/>
-    <hyperlink ref="B495" r:id="rId440" xr:uid="{1E1D3964-01E0-3145-ACFE-B6A5BF0EECB0}"/>
-    <hyperlink ref="B493" r:id="rId441" xr:uid="{FA0E5061-A7E2-C045-9671-1CD9446D1932}"/>
-    <hyperlink ref="B494" r:id="rId442" location=":~:text=Given%20an%20integer%20n%2C%20calculate,*%2C%20%2F%20and%20pow().&amp;text=A%20Simple%20Solution%20is%20to%20repeatedly%20add%20n%20to%20result." xr:uid="{92704F5B-7B31-2F42-80DD-764B2206D9DB}"/>
+    <hyperlink ref="B400" r:id="rId352" xr:uid="{3EC43646-EAB1-E443-A2F6-8E6E5FC77083}"/>
+    <hyperlink ref="B401" r:id="rId353" xr:uid="{659D9F20-C862-C947-B422-84143CFE317F}"/>
+    <hyperlink ref="B402" r:id="rId354" xr:uid="{3F5192FE-1C50-C049-88D5-68FA0F5430A0}"/>
+    <hyperlink ref="B403" r:id="rId355" xr:uid="{5EAD7CDA-9545-454B-BE77-9AFEC6AC1083}"/>
+    <hyperlink ref="B404" r:id="rId356" xr:uid="{761E5451-736B-6745-9CF5-4C6EF5D4C099}"/>
+    <hyperlink ref="B405" r:id="rId357" xr:uid="{4C8677A9-D94C-134F-AF31-E424751BF867}"/>
+    <hyperlink ref="B406" r:id="rId358" xr:uid="{CCF7920F-D5CE-004A-86C3-D821FB230970}"/>
+    <hyperlink ref="B407" r:id="rId359" xr:uid="{B4C07A0A-1EDD-7947-9646-3FD603441AD7}"/>
+    <hyperlink ref="B408" r:id="rId360" xr:uid="{49F7BB43-6851-0641-9DC5-27DBC66706F6}"/>
+    <hyperlink ref="B409" r:id="rId361" xr:uid="{77038647-48C7-5547-8E0F-898610362465}"/>
+    <hyperlink ref="B411" r:id="rId362" xr:uid="{EEFFE19C-6571-C64F-A0E1-5A4A700D94D4}"/>
+    <hyperlink ref="B410" r:id="rId363" xr:uid="{A4A2BFC4-6B88-2E4E-B362-17D8EE041C89}"/>
+    <hyperlink ref="B412" r:id="rId364" xr:uid="{DC5B603A-8D65-3648-A08A-E5FFA0FAE879}"/>
+    <hyperlink ref="B413" r:id="rId365" xr:uid="{F8807DD9-F4F2-B147-9C31-DBC93B2E477B}"/>
+    <hyperlink ref="B414" r:id="rId366" xr:uid="{6F7B396C-D7E9-C04E-BAE2-53D2EE07172B}"/>
+    <hyperlink ref="B417" r:id="rId367" xr:uid="{0D4A5941-C669-4A49-BAE3-9B553D03BD0F}"/>
+    <hyperlink ref="B418" r:id="rId368" xr:uid="{54144336-5BCA-D749-962A-E448C2CED3D3}"/>
+    <hyperlink ref="B419" r:id="rId369" xr:uid="{3A41DD21-CACF-1F48-A7C7-F568C6F31F3E}"/>
+    <hyperlink ref="B420" r:id="rId370" xr:uid="{A36160A8-F45E-3443-9645-42C1004B8F8C}"/>
+    <hyperlink ref="B421" r:id="rId371" xr:uid="{8B0A00A3-6AC0-DF46-AD87-A4DA016A2A00}"/>
+    <hyperlink ref="B422" r:id="rId372" xr:uid="{62A81CB4-A961-C543-B31C-92059DB6C105}"/>
+    <hyperlink ref="B425" r:id="rId373" xr:uid="{08030975-009C-C34A-A875-72FE2718F44C}"/>
+    <hyperlink ref="B426" r:id="rId374" xr:uid="{A113C7A9-2359-B643-9C08-E845813439C0}"/>
+    <hyperlink ref="B427" r:id="rId375" xr:uid="{FE300343-4633-AD47-A64D-2086629EB398}"/>
+    <hyperlink ref="B428" r:id="rId376" xr:uid="{4FC9F782-D38F-C642-A863-887B17AD05CD}"/>
+    <hyperlink ref="B429" r:id="rId377" xr:uid="{830C5466-10E3-7A48-B3E7-35C15A1CA4EF}"/>
+    <hyperlink ref="B430" r:id="rId378" xr:uid="{1B987077-E9D3-6F40-89EE-0D4E7180D884}"/>
+    <hyperlink ref="B431" r:id="rId379" xr:uid="{D4843E1F-7226-864E-A4BB-264D5A487B6D}"/>
+    <hyperlink ref="B432" r:id="rId380" xr:uid="{61816592-2D19-9946-8253-47A60218F2EA}"/>
+    <hyperlink ref="B433" r:id="rId381" xr:uid="{736C840F-19A3-0A4B-8863-ECB772B46385}"/>
+    <hyperlink ref="B434" r:id="rId382" xr:uid="{05A238AD-3C5B-C546-94E9-75BBF964711A}"/>
+    <hyperlink ref="B435" r:id="rId383" xr:uid="{7029629C-3F2A-4A49-997B-CFE86EC8B3C2}"/>
+    <hyperlink ref="B436" r:id="rId384" xr:uid="{ADA66B57-2FAC-AB42-BD83-4931708F3AB5}"/>
+    <hyperlink ref="B437" r:id="rId385" xr:uid="{F16BF1F9-755B-B045-B9A8-0B97E3BAC8B0}"/>
+    <hyperlink ref="B438" r:id="rId386" xr:uid="{ECCE930A-B960-234C-81EC-4B8514282AE9}"/>
+    <hyperlink ref="B439" r:id="rId387" xr:uid="{7AA58141-7D24-7C42-A0C1-F852B21CFFD9}"/>
+    <hyperlink ref="B440" r:id="rId388" xr:uid="{B1FCB47D-7921-3446-B2C7-72CBA815D056}"/>
+    <hyperlink ref="B441" r:id="rId389" xr:uid="{8C547719-AA03-3543-B31F-7300674AF4C5}"/>
+    <hyperlink ref="B442" r:id="rId390" xr:uid="{09922668-AFC0-F242-860E-9967E0F0FEF4}"/>
+    <hyperlink ref="B443" r:id="rId391" xr:uid="{0DA963DA-238B-D44E-9E03-6E6BD933B35E}"/>
+    <hyperlink ref="B444" r:id="rId392" xr:uid="{89518AFF-2526-C845-BC9D-95FE77AF416E}"/>
+    <hyperlink ref="B445" r:id="rId393" xr:uid="{FAECBBBE-196C-7A41-A0FB-E0597CB2CF51}"/>
+    <hyperlink ref="B446" r:id="rId394" xr:uid="{8126B039-0B25-B040-A0F6-C3457341A2E9}"/>
+    <hyperlink ref="B447" r:id="rId395" xr:uid="{6CB326E6-E698-EB42-884B-C89FFA33E3BA}"/>
+    <hyperlink ref="B448" r:id="rId396" xr:uid="{8C97EFD1-933F-A44F-A1CF-6386233104A2}"/>
+    <hyperlink ref="B449" r:id="rId397" xr:uid="{8F019F07-8532-E147-8BE1-4EBE833F61CA}"/>
+    <hyperlink ref="B450" r:id="rId398" xr:uid="{00F1A08F-3767-784A-97A3-4603DE38BACC}"/>
+    <hyperlink ref="B451" r:id="rId399" xr:uid="{2A84ADCB-071F-9A48-994D-7A838307EFD8}"/>
+    <hyperlink ref="B452" r:id="rId400" xr:uid="{132F8C6D-D5E8-6440-AC4E-B81EA2100416}"/>
+    <hyperlink ref="B453" r:id="rId401" xr:uid="{2DA6EAC2-1A1D-754F-9613-226CBC7890AF}"/>
+    <hyperlink ref="B454" r:id="rId402" xr:uid="{05BED99A-4562-D14E-8627-D07CF5335A9B}"/>
+    <hyperlink ref="B455" r:id="rId403" xr:uid="{111D902A-3F60-2D4B-89D3-5BCBD8AA38DD}"/>
+    <hyperlink ref="B456" r:id="rId404" xr:uid="{F19236BE-AC32-3542-9214-DFC3BAE04ED0}"/>
+    <hyperlink ref="B457" r:id="rId405" xr:uid="{4D97CD96-EA1B-664E-9380-EFD27077D273}"/>
+    <hyperlink ref="B458" r:id="rId406" xr:uid="{49A46D91-633F-A148-ACFA-49B7D1AA4B33}"/>
+    <hyperlink ref="B459" r:id="rId407" xr:uid="{7C3B7901-67E3-EA4D-BC64-21A78BC03AC6}"/>
+    <hyperlink ref="B460" r:id="rId408" xr:uid="{B27CA8C3-D34F-5E4D-94A5-11D14AFD0F82}"/>
+    <hyperlink ref="B461" r:id="rId409" xr:uid="{8FECE038-9764-5E4A-8C6E-9B3209812651}"/>
+    <hyperlink ref="B462" r:id="rId410" xr:uid="{95696D4B-89CB-5640-BE92-53B3C043F7EB}"/>
+    <hyperlink ref="B463" r:id="rId411" xr:uid="{DA74B737-802A-4944-A93E-0B9C8417630B}"/>
+    <hyperlink ref="B464" r:id="rId412" xr:uid="{B2C4C168-50FA-AF41-8F56-9E70613CF17D}"/>
+    <hyperlink ref="B466" r:id="rId413" xr:uid="{B7090C60-AC27-3F4F-8F0D-42F0791928C6}"/>
+    <hyperlink ref="B465" r:id="rId414" xr:uid="{07400041-66C6-514B-B3E3-427F2947C2B7}"/>
+    <hyperlink ref="B467" r:id="rId415" xr:uid="{B7E78172-8FB8-4E42-87D8-6A4654D79C62}"/>
+    <hyperlink ref="B468" r:id="rId416" xr:uid="{9A5D4670-BC64-334A-88CF-6F8287692C5E}"/>
+    <hyperlink ref="B469" r:id="rId417" xr:uid="{604283B6-53BC-044F-8D9D-E6094E798317}"/>
+    <hyperlink ref="B470" r:id="rId418" xr:uid="{5EB15AC7-3E0E-E44C-A5B9-32F30F234B5A}"/>
+    <hyperlink ref="B471" r:id="rId419" xr:uid="{3076BD5F-4B23-4146-A50A-499C9FF4C3D2}"/>
+    <hyperlink ref="B472" r:id="rId420" xr:uid="{6A29D9C2-1E78-1B43-A251-0AB0A97FA70E}"/>
+    <hyperlink ref="B473" r:id="rId421" xr:uid="{00597D5E-D693-DF4E-84C0-47E58A6ACA8F}"/>
+    <hyperlink ref="B474" r:id="rId422" xr:uid="{48640988-9964-0B4C-A014-83E2CEB3D632}"/>
+    <hyperlink ref="B475" r:id="rId423" xr:uid="{617AADC9-7534-FE45-96B0-EF4C1867B793}"/>
+    <hyperlink ref="B476" r:id="rId424" xr:uid="{7F8CDAA4-5094-8E4E-961B-41CDE5ACC0C0}"/>
+    <hyperlink ref="B477" r:id="rId425" xr:uid="{63F28ABD-12CF-5947-80DA-229E3CA3133E}"/>
+    <hyperlink ref="B484" r:id="rId426" xr:uid="{0A1DB92C-3315-1942-B27D-4B90986A6D9D}"/>
+    <hyperlink ref="B483" r:id="rId427" xr:uid="{11738B67-CADD-5D45-8417-8BE7A03FC79F}"/>
+    <hyperlink ref="B482" r:id="rId428" xr:uid="{B2B23748-D9E4-BE4F-A93E-49ECB4063831}"/>
+    <hyperlink ref="B481" r:id="rId429" xr:uid="{A2FB8A72-37B9-7E4A-B050-FD6CD20BCE73}"/>
+    <hyperlink ref="B480" r:id="rId430" xr:uid="{5A93C9AF-BFEB-EB40-95AC-C309ED09A604}"/>
+    <hyperlink ref="B479" r:id="rId431" xr:uid="{CC203923-2DC2-874B-B846-A8455E3CC2F2}"/>
+    <hyperlink ref="B478" r:id="rId432" xr:uid="{FCB0246E-0179-B447-B3CE-C60CDB388472}"/>
+    <hyperlink ref="B487" r:id="rId433" xr:uid="{F06CEE72-8CA4-C547-862C-39B86CD3226A}"/>
+    <hyperlink ref="B488" r:id="rId434" xr:uid="{CB3045F2-8D63-0F4E-85BC-AF016DB4F247}"/>
+    <hyperlink ref="B489" r:id="rId435" xr:uid="{667D57F5-E5AD-674F-A2F5-AFF4A14E4026}"/>
+    <hyperlink ref="B490" r:id="rId436" xr:uid="{27A13A65-56CE-BF4D-BA0D-EB87D910272D}"/>
+    <hyperlink ref="B491" r:id="rId437" xr:uid="{2C72A52E-6F06-0246-AEB5-93CD0DEA8866}"/>
+    <hyperlink ref="B492" r:id="rId438" xr:uid="{24B29046-B4DD-674B-9EDF-6C94BEC3FDD8}"/>
+    <hyperlink ref="B493" r:id="rId439" xr:uid="{D018EBC3-3FB3-AC4D-9D64-D218345A46C8}"/>
+    <hyperlink ref="B496" r:id="rId440" xr:uid="{1E1D3964-01E0-3145-ACFE-B6A5BF0EECB0}"/>
+    <hyperlink ref="B494" r:id="rId441" xr:uid="{FA0E5061-A7E2-C045-9671-1CD9446D1932}"/>
+    <hyperlink ref="B495" r:id="rId442" location=":~:text=Given%20an%20integer%20n%2C%20calculate,*%2C%20%2F%20and%20pow().&amp;text=A%20Simple%20Solution%20is%20to%20repeatedly%20add%20n%20to%20result." xr:uid="{92704F5B-7B31-2F42-80DD-764B2206D9DB}"/>
     <hyperlink ref="B368" r:id="rId443" xr:uid="{A48B1A24-83B1-7A4C-8129-CD37804DF849}"/>
     <hyperlink ref="B2" r:id="rId444" xr:uid="{E07D4FE5-46C7-AC4D-9E01-2300AA43B58A}"/>
     <hyperlink ref="B39" r:id="rId445" xr:uid="{F2DE2162-BD02-7549-AC1A-27455F78131F}"/>
@@ -7763,8 +7777,9 @@
     <hyperlink ref="B185" r:id="rId458" xr:uid="{AEB61F80-6C73-454E-98EC-F97D434F5EB5}"/>
     <hyperlink ref="B391" r:id="rId459" xr:uid="{FF5FD771-6B03-42F1-BD02-B7B19A3A0362}"/>
     <hyperlink ref="B392" r:id="rId460" xr:uid="{AF14A62A-C14A-4BBC-950D-CDB33CBB158B}"/>
+    <hyperlink ref="B399" r:id="rId461" xr:uid="{3DC6B9E0-05DC-4888-815A-CDBB63BDF598}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId461"/>
+  <pageSetup orientation="portrait" r:id="rId462"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Longest Path in a Directed Acyclic Graph
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harsh\Desktop\Data-Structures-and-Algorithms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E0E1B1C-1CD6-4E7F-9DE5-7A7031AAEE05}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C336B5B-8E94-47C7-B6DE-FCC8F7B1B099}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -2036,7 +2036,7 @@
   <dimension ref="A1:D496"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A390" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B399" sqref="B399"/>
+      <selection activeCell="B401" sqref="B401"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -6296,8 +6296,8 @@
       <c r="B400" s="6" t="s">
         <v>372</v>
       </c>
-      <c r="C400" s="4" t="s">
-        <v>4</v>
+      <c r="C400" s="11" t="s">
+        <v>464</v>
       </c>
     </row>
     <row r="401" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Find if there is a path of more than k length from a source
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harsh\Desktop\Data-Structures-and-Algorithms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C336B5B-8E94-47C7-B6DE-FCC8F7B1B099}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86D335EF-58A9-4406-AF3B-687EB431E6A3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -2035,8 +2035,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:D496"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A390" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B401" sqref="B401"/>
+    <sheetView tabSelected="1" topLeftCell="A396" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B406" sqref="B406"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -6362,8 +6362,8 @@
       <c r="B406" s="6" t="s">
         <v>377</v>
       </c>
-      <c r="C406" s="4" t="s">
-        <v>4</v>
+      <c r="C406" s="11" t="s">
+        <v>464</v>
       </c>
     </row>
     <row r="407" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Minimum edges to reverse to make path from a source to a destination.
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harsh\Desktop\Data-Structures-and-Algorithms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86D335EF-58A9-4406-AF3B-687EB431E6A3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53114897-172F-445E-83AF-EF214DB421C8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -2035,8 +2035,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:D496"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A396" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B406" sqref="B406"/>
+    <sheetView tabSelected="1" topLeftCell="A398" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C409" sqref="C409"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -6384,8 +6384,8 @@
       <c r="B408" s="6" t="s">
         <v>379</v>
       </c>
-      <c r="C408" s="4" t="s">
-        <v>4</v>
+      <c r="C408" s="11" t="s">
+        <v>464</v>
       </c>
     </row>
     <row r="409" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Number of Triangles in Directed and Undirected Graphs
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harsh\Desktop\Data-Structures-and-Algorithms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53114897-172F-445E-83AF-EF214DB421C8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A53DA6B-6E99-47CC-8C08-500D24414BAE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1576,7 +1576,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1649,6 +1649,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1663,7 +1669,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1716,6 +1722,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2036,7 +2045,7 @@
   <dimension ref="A1:D496"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A398" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C409" sqref="C409"/>
+      <selection activeCell="C412" sqref="C412"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -6307,8 +6316,8 @@
       <c r="B401" s="6" t="s">
         <v>373</v>
       </c>
-      <c r="C401" s="4" t="s">
-        <v>4</v>
+      <c r="C401" s="11" t="s">
+        <v>464</v>
       </c>
     </row>
     <row r="402" spans="1:3" ht="21">
@@ -6318,7 +6327,7 @@
       <c r="B402" s="6" t="s">
         <v>374</v>
       </c>
-      <c r="C402" s="4" t="s">
+      <c r="C402" s="22" t="s">
         <v>4</v>
       </c>
     </row>
@@ -6428,8 +6437,8 @@
       <c r="B412" s="6" t="s">
         <v>383</v>
       </c>
-      <c r="C412" s="4" t="s">
-        <v>4</v>
+      <c r="C412" s="11" t="s">
+        <v>464</v>
       </c>
     </row>
     <row r="413" spans="1:3" ht="21">

</xml_diff>

<commit_message>
N meetings in one room
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harsh\Desktop\Data-Structures-and-Algorithms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B43CA53B-F305-4C00-9448-A10BE42853A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE52EA4D-AE9C-4959-8C3D-5BC67FFFF140}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -2044,8 +2044,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:D496"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A404" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C414" sqref="C414"/>
+    <sheetView tabSelected="1" topLeftCell="A244" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C247" sqref="C247"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -4669,8 +4669,8 @@
       <c r="B247" s="6" t="s">
         <v>230</v>
       </c>
-      <c r="C247" s="4" t="s">
-        <v>4</v>
+      <c r="C247" s="11" t="s">
+        <v>464</v>
       </c>
     </row>
     <row r="248" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Minimum number of Coins
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harsh\Desktop\Data-Structures-and-Algorithms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BAAC0CF-A539-4840-BA51-336A656A5A9E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D49E0CAD-710E-429B-B6E5-AAE40D214EA6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -2044,8 +2044,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:D496"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A242" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C251" sqref="C251"/>
+    <sheetView tabSelected="1" topLeftCell="A248" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C253" sqref="C253"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -4724,8 +4724,8 @@
       <c r="B252" s="6" t="s">
         <v>235</v>
       </c>
-      <c r="C252" s="4" t="s">
-        <v>4</v>
+      <c r="C252" s="11" t="s">
+        <v>464</v>
       </c>
     </row>
     <row r="253" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Buy Maximum Stocks if i stocks can be bought on i-th day
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harsh\Desktop\Data-Structures-and-Algorithms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FCD2645-D7F7-46AB-BFAF-597F63C45C6E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5991605-1E66-4D50-8943-F8C14E000861}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -2047,8 +2047,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:D497"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A245" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B250" sqref="B250"/>
+    <sheetView tabSelected="1" topLeftCell="A244" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B256" sqref="B256"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -4771,8 +4771,8 @@
       <c r="B256" s="6" t="s">
         <v>238</v>
       </c>
-      <c r="C256" s="4" t="s">
-        <v>4</v>
+      <c r="C256" s="11" t="s">
+        <v>464</v>
       </c>
     </row>
     <row r="257" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Shop in Candy Store
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harsh\Desktop\Data-Structures-and-Algorithms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5991605-1E66-4D50-8943-F8C14E000861}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C589EF40-5818-4AD5-A4BA-E4C1B270E66E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -2047,8 +2047,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:D497"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A244" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B256" sqref="B256"/>
+    <sheetView tabSelected="1" topLeftCell="A247" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C257" sqref="C257"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -4782,8 +4782,8 @@
       <c r="B257" s="6" t="s">
         <v>239</v>
       </c>
-      <c r="C257" s="4" t="s">
-        <v>4</v>
+      <c r="C257" s="11" t="s">
+        <v>464</v>
       </c>
     </row>
     <row r="258" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Minimum Cost to cut a board into squares
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harsh\Desktop\Data-Structures-and-Algorithms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C589EF40-5818-4AD5-A4BA-E4C1B270E66E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AA891C8-B4F8-4F90-8DDE-83DB5A06CECB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1415" uniqueCount="495">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1416" uniqueCount="496">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1510,6 +1510,9 @@
   </si>
   <si>
     <t>Choose and Swap</t>
+  </si>
+  <si>
+    <t>https://www.spoj.com/problems/CHOCOLA/</t>
   </si>
 </sst>
 </file>
@@ -2048,7 +2051,7 @@
   <dimension ref="A1:D497"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A247" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C257" sqref="C257"/>
+      <selection activeCell="B259" sqref="B259"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -2056,7 +2059,7 @@
     <col min="1" max="1" width="28.5" customWidth="1"/>
     <col min="2" max="2" width="123" customWidth="1"/>
     <col min="3" max="3" width="27.5" customWidth="1"/>
-    <col min="4" max="4" width="27.375" customWidth="1"/>
+    <col min="4" max="4" width="65.375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="26.25">
@@ -4775,7 +4778,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="257" spans="1:3" ht="21">
+    <row r="257" spans="1:4" ht="21">
       <c r="A257" s="5" t="s">
         <v>229</v>
       </c>
@@ -4786,7 +4789,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="258" spans="1:3" ht="21">
+    <row r="258" spans="1:4" ht="21">
       <c r="A258" s="5" t="s">
         <v>229</v>
       </c>
@@ -4797,18 +4800,21 @@
         <v>4</v>
       </c>
     </row>
-    <row r="259" spans="1:3" ht="21">
+    <row r="259" spans="1:4" ht="21">
       <c r="A259" s="5" t="s">
         <v>229</v>
       </c>
       <c r="B259" s="6" t="s">
         <v>241</v>
       </c>
-      <c r="C259" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="260" spans="1:3" ht="21">
+      <c r="C259" s="11" t="s">
+        <v>464</v>
+      </c>
+      <c r="D259" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="260" spans="1:4" ht="21">
       <c r="A260" s="5" t="s">
         <v>229</v>
       </c>
@@ -4819,7 +4825,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="261" spans="1:3" ht="21">
+    <row r="261" spans="1:4" ht="21">
       <c r="A261" s="5" t="s">
         <v>229</v>
       </c>
@@ -4830,7 +4836,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="262" spans="1:3" ht="21">
+    <row r="262" spans="1:4" ht="21">
       <c r="A262" s="5" t="s">
         <v>229</v>
       </c>
@@ -4841,7 +4847,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="263" spans="1:3" ht="21">
+    <row r="263" spans="1:4" ht="21">
       <c r="A263" s="5" t="s">
         <v>229</v>
       </c>
@@ -4852,7 +4858,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="264" spans="1:3" ht="21">
+    <row r="264" spans="1:4" ht="21">
       <c r="A264" s="5" t="s">
         <v>229</v>
       </c>
@@ -4863,7 +4869,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="265" spans="1:3" ht="21">
+    <row r="265" spans="1:4" ht="21">
       <c r="A265" s="5" t="s">
         <v>229</v>
       </c>
@@ -4874,7 +4880,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="266" spans="1:3" ht="21">
+    <row r="266" spans="1:4" ht="21">
       <c r="A266" s="5" t="s">
         <v>229</v>
       </c>
@@ -4885,7 +4891,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="267" spans="1:3" ht="21">
+    <row r="267" spans="1:4" ht="21">
       <c r="A267" s="5" t="s">
         <v>229</v>
       </c>
@@ -4896,7 +4902,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="268" spans="1:3" ht="21">
+    <row r="268" spans="1:4" ht="21">
       <c r="A268" s="5" t="s">
         <v>229</v>
       </c>
@@ -4907,7 +4913,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="269" spans="1:3" ht="21">
+    <row r="269" spans="1:4" ht="21">
       <c r="A269" s="5" t="s">
         <v>229</v>
       </c>
@@ -4918,7 +4924,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="270" spans="1:3" ht="21">
+    <row r="270" spans="1:4" ht="21">
       <c r="A270" s="5" t="s">
         <v>229</v>
       </c>
@@ -4929,7 +4935,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="271" spans="1:3" ht="21">
+    <row r="271" spans="1:4" ht="21">
       <c r="A271" s="5" t="s">
         <v>229</v>
       </c>
@@ -4940,7 +4946,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="272" spans="1:3" ht="21">
+    <row r="272" spans="1:4" ht="21">
       <c r="A272" s="5" t="s">
         <v>229</v>
       </c>

</xml_diff>

<commit_message>
Check if it is possible to survive on Island
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harsh\Desktop\Data-Structures-and-Algorithms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AA891C8-B4F8-4F90-8DDE-83DB5A06CECB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{205EC62F-5BF9-430F-ABB6-B86B8A9EA983}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -2050,8 +2050,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:D497"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A247" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B259" sqref="B259"/>
+    <sheetView tabSelected="1" topLeftCell="A248" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C261" sqref="C261"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -4821,8 +4821,8 @@
       <c r="B260" s="6" t="s">
         <v>242</v>
       </c>
-      <c r="C260" s="4" t="s">
-        <v>4</v>
+      <c r="C260" s="11" t="s">
+        <v>464</v>
       </c>
     </row>
     <row r="261" spans="1:4" ht="21">

</xml_diff>

<commit_message>
Maximum product subset of an array
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harsh\Desktop\Data-Structures-and-Algorithms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{205EC62F-5BF9-430F-ABB6-B86B8A9EA983}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CB36233-BCEF-4699-A525-0A328EC2A981}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1416" uniqueCount="496">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1416" uniqueCount="497">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1513,6 +1513,9 @@
   </si>
   <si>
     <t>https://www.spoj.com/problems/CHOCOLA/</t>
+  </si>
+  <si>
+    <t>&lt;YES&gt; Same as N Meetings ina room</t>
   </si>
 </sst>
 </file>
@@ -1582,7 +1585,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1661,6 +1664,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1675,7 +1684,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1731,6 +1740,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2050,8 +2062,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:D497"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A248" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C261" sqref="C261"/>
+    <sheetView tabSelected="1" topLeftCell="A251" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B264" sqref="B264"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -2969,7 +2981,7 @@
         <v>86</v>
       </c>
       <c r="C88" s="11" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="89" spans="1:3" ht="21">
@@ -2980,7 +2992,7 @@
         <v>87</v>
       </c>
       <c r="C89" s="11" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="90" spans="1:3" ht="21">
@@ -2991,7 +3003,7 @@
         <v>88</v>
       </c>
       <c r="C90" s="11" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="91" spans="1:3" ht="21">
@@ -3002,7 +3014,7 @@
         <v>89</v>
       </c>
       <c r="C91" s="11" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="92" spans="1:3" ht="21">
@@ -3013,7 +3025,7 @@
         <v>90</v>
       </c>
       <c r="C92" s="11" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="93" spans="1:3" ht="21">
@@ -3046,7 +3058,7 @@
         <v>93</v>
       </c>
       <c r="C95" s="11" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="96" spans="1:3" ht="21">
@@ -3057,7 +3069,7 @@
         <v>94</v>
       </c>
       <c r="C96" s="11" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="97" spans="1:3" ht="21">
@@ -3068,7 +3080,7 @@
         <v>95</v>
       </c>
       <c r="C97" s="11" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="98" spans="1:3" ht="21">
@@ -3079,7 +3091,7 @@
         <v>96</v>
       </c>
       <c r="C98" s="11" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="100" spans="1:3" ht="21">
@@ -4832,8 +4844,8 @@
       <c r="B261" s="6" t="s">
         <v>243</v>
       </c>
-      <c r="C261" s="4" t="s">
-        <v>4</v>
+      <c r="C261" s="23" t="s">
+        <v>496</v>
       </c>
     </row>
     <row r="262" spans="1:4" ht="21">
@@ -4843,8 +4855,8 @@
       <c r="B262" s="6" t="s">
         <v>244</v>
       </c>
-      <c r="C262" s="4" t="s">
-        <v>4</v>
+      <c r="C262" s="11" t="s">
+        <v>464</v>
       </c>
     </row>
     <row r="263" spans="1:4" ht="21">

</xml_diff>

<commit_message>
Maximize sum after K negations
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harsh\Desktop\Data-Structures-and-Algorithms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CB36233-BCEF-4699-A525-0A328EC2A981}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58EC356D-30BF-41CD-AD93-F1BF56709F5C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -2063,7 +2063,7 @@
   <dimension ref="A1:D497"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A251" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B264" sqref="B264"/>
+      <selection activeCell="C264" sqref="C264"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -4866,8 +4866,8 @@
       <c r="B263" s="6" t="s">
         <v>245</v>
       </c>
-      <c r="C263" s="4" t="s">
-        <v>4</v>
+      <c r="C263" s="11" t="s">
+        <v>464</v>
       </c>
     </row>
     <row r="264" spans="1:4" ht="21">

</xml_diff>

<commit_message>
Maximum sum of absolute difference of any permutation
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harsh\Desktop\Data-Structures-and-Algorithms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58EC356D-30BF-41CD-AD93-F1BF56709F5C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C82F50F7-3935-4614-BEDB-284310B69BA4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -2062,8 +2062,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:D497"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A251" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C264" sqref="C264"/>
+    <sheetView tabSelected="1" topLeftCell="A260" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B266" sqref="B266"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -4877,8 +4877,8 @@
       <c r="B264" s="6" t="s">
         <v>246</v>
       </c>
-      <c r="C264" s="4" t="s">
-        <v>4</v>
+      <c r="C264" s="11" t="s">
+        <v>464</v>
       </c>
     </row>
     <row r="265" spans="1:4" ht="21">
@@ -4888,8 +4888,8 @@
       <c r="B265" s="6" t="s">
         <v>247</v>
       </c>
-      <c r="C265" s="4" t="s">
-        <v>4</v>
+      <c r="C265" s="11" t="s">
+        <v>464</v>
       </c>
     </row>
     <row r="266" spans="1:4" ht="21">

</xml_diff>

<commit_message>
Minimum sum of absolute difference of pairs of two arrays
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harsh\Desktop\Data-Structures-and-Algorithms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C82F50F7-3935-4614-BEDB-284310B69BA4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4D8C7E4-79F8-4C44-8AF8-41CB9833D00E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1416" uniqueCount="497">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1418" uniqueCount="497">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -2062,8 +2062,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:D497"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A260" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B266" sqref="B266"/>
+    <sheetView tabSelected="1" topLeftCell="A257" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C267" sqref="C267"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -4891,6 +4891,9 @@
       <c r="C265" s="11" t="s">
         <v>464</v>
       </c>
+      <c r="D265" t="s">
+        <v>465</v>
+      </c>
     </row>
     <row r="266" spans="1:4" ht="21">
       <c r="A266" s="5" t="s">
@@ -4899,8 +4902,11 @@
       <c r="B266" s="6" t="s">
         <v>248</v>
       </c>
-      <c r="C266" s="4" t="s">
-        <v>4</v>
+      <c r="C266" s="11" t="s">
+        <v>464</v>
+      </c>
+      <c r="D266" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="267" spans="1:4" ht="21">
@@ -4910,8 +4916,8 @@
       <c r="B267" s="6" t="s">
         <v>249</v>
       </c>
-      <c r="C267" s="4" t="s">
-        <v>4</v>
+      <c r="C267" s="11" t="s">
+        <v>464</v>
       </c>
     </row>
     <row r="268" spans="1:4" ht="21">
@@ -5009,8 +5015,8 @@
       <c r="B276" s="6" t="s">
         <v>258</v>
       </c>
-      <c r="C276" s="4" t="s">
-        <v>4</v>
+      <c r="C276" s="11" t="s">
+        <v>464</v>
       </c>
     </row>
     <row r="277" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Page Faults in LRU
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harsh\Desktop\Data-Structures-and-Algorithms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FE6C15A-F85F-4968-AAFD-5244C7BD0516}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69062B60-4AC3-4E91-80D8-9A28FC98CD29}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -2062,8 +2062,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:D497"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A263" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C269" sqref="C269"/>
+    <sheetView tabSelected="1" topLeftCell="A265" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C270" sqref="C270"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -4938,8 +4938,8 @@
       <c r="B269" s="6" t="s">
         <v>251</v>
       </c>
-      <c r="C269" s="4" t="s">
-        <v>4</v>
+      <c r="C269" s="11" t="s">
+        <v>464</v>
       </c>
     </row>
     <row r="270" spans="1:4" ht="21">

</xml_diff>

<commit_message>
Smallest subset with sum greater than all other elements
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harsh\Desktop\Data-Structures-and-Algorithms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69062B60-4AC3-4E91-80D8-9A28FC98CD29}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE3749CD-B460-4B17-94E3-47D185577D94}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -2062,8 +2062,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:D497"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A265" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C270" sqref="C270"/>
+    <sheetView tabSelected="1" topLeftCell="A262" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C271" sqref="C271"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -4949,8 +4949,8 @@
       <c r="B270" s="6" t="s">
         <v>252</v>
       </c>
-      <c r="C270" s="4" t="s">
-        <v>4</v>
+      <c r="C270" s="11" t="s">
+        <v>464</v>
       </c>
     </row>
     <row r="271" spans="1:4" ht="21">

</xml_diff>

<commit_message>
Minimum Cost of Ropes
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harsh\Desktop\Data-Structures-and-Algorithms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F2BE760-5283-467B-8213-0749911C577D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0AF43E8-B0ED-41A8-9572-08161EF0A4A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -2063,7 +2063,7 @@
   <dimension ref="A1:D497"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A262" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B271" sqref="B271"/>
+      <selection activeCell="C278" sqref="C278"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -5048,8 +5048,8 @@
       <c r="B279" s="6" t="s">
         <v>261</v>
       </c>
-      <c r="C279" s="4" t="s">
-        <v>4</v>
+      <c r="C279" s="11" t="s">
+        <v>464</v>
       </c>
     </row>
     <row r="280" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Rearrange characters in a string such that no two adjacent are same
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harsh\Desktop\Data-Structures-and-Algorithms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0AF43E8-B0ED-41A8-9572-08161EF0A4A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0196951-87B4-4789-AD9C-2C7F66B8FBEF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -2062,8 +2062,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:D497"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A262" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C278" sqref="C278"/>
+    <sheetView tabSelected="1" topLeftCell="A265" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B274" sqref="B274"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -5070,8 +5070,8 @@
       <c r="B281" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="C281" s="4" t="s">
-        <v>4</v>
+      <c r="C281" s="11" t="s">
+        <v>464</v>
       </c>
     </row>
     <row r="282" spans="1:3" ht="21">

</xml_diff>

<commit_message>
DEFKIN - Defense of a Kingdom
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harsh\Desktop\Data-Structures-and-Algorithms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0196951-87B4-4789-AD9C-2C7F66B8FBEF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43BDDDF9-0937-42C7-942F-46F3230FA573}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -2063,7 +2063,7 @@
   <dimension ref="A1:D497"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A265" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B274" sqref="B274"/>
+      <selection activeCell="C273" sqref="C273"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -4971,8 +4971,8 @@
       <c r="B272" s="6" t="s">
         <v>254</v>
       </c>
-      <c r="C272" s="4" t="s">
-        <v>4</v>
+      <c r="C272" s="11" t="s">
+        <v>464</v>
       </c>
     </row>
     <row r="273" spans="1:3" ht="21">

</xml_diff>

<commit_message>
ARRANGE - Arranging Amplifiers
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harsh\Desktop\Data-Structures-and-Algorithms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F28AE44-3B08-4C11-B70B-BC89CECDE4CE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{513675B1-2DDA-4837-A255-C7F683E3F8F4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -2063,7 +2063,7 @@
   <dimension ref="A1:D497"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A265" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C274" sqref="C274"/>
+      <selection activeCell="D277" sqref="D277"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -5026,8 +5026,8 @@
       <c r="B277" s="6" t="s">
         <v>259</v>
       </c>
-      <c r="C277" s="4" t="s">
-        <v>4</v>
+      <c r="C277" s="11" t="s">
+        <v>464</v>
       </c>
     </row>
     <row r="278" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Find smallest number with given number of digits and sum of digits
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harsh\Desktop\Data-Structures-and-Algorithms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{513675B1-2DDA-4837-A255-C7F683E3F8F4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89E54DC8-A593-4D97-8C38-9ED267F2D17A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -2063,7 +2063,7 @@
   <dimension ref="A1:D497"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A265" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D277" sqref="D277"/>
+      <selection activeCell="B277" sqref="B277"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -5059,8 +5059,8 @@
       <c r="B280" s="6" t="s">
         <v>262</v>
       </c>
-      <c r="C280" s="4" t="s">
-        <v>4</v>
+      <c r="C280" s="11" t="s">
+        <v>464</v>
       </c>
     </row>
     <row r="281" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Find maximum sum possible equal sum of three stacks
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harsh\Desktop\Data-Structures-and-Algorithms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89E54DC8-A593-4D97-8C38-9ED267F2D17A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2060ED2-6FB9-469C-AEBA-3B15516A62B2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -2063,7 +2063,7 @@
   <dimension ref="A1:D497"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A265" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B277" sqref="B277"/>
+      <selection activeCell="B276" sqref="B276"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -5081,8 +5081,8 @@
       <c r="B282" s="6" t="s">
         <v>263</v>
       </c>
-      <c r="C282" s="4" t="s">
-        <v>4</v>
+      <c r="C282" s="11" t="s">
+        <v>464</v>
       </c>
     </row>
     <row r="283" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Find all possible palindromic partitions of a String
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harsh\Desktop\Data-Structures-and-Algorithms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29E45012-6A34-4A2C-9040-E771E43F5377}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2F218AA-F54D-4589-BEAB-0ECD0B33D525}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -2063,7 +2063,7 @@
   <dimension ref="A1:D497"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A282" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C290" sqref="C290"/>
+      <selection activeCell="B294" sqref="B294"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -5155,8 +5155,8 @@
       <c r="B290" s="6" t="s">
         <v>270</v>
       </c>
-      <c r="C290" s="4" t="s">
-        <v>4</v>
+      <c r="C290" s="11" t="s">
+        <v>464</v>
       </c>
     </row>
     <row r="291" spans="1:3" ht="21">
@@ -5166,8 +5166,8 @@
       <c r="B291" s="6" t="s">
         <v>271</v>
       </c>
-      <c r="C291" s="4" t="s">
-        <v>4</v>
+      <c r="C291" s="11" t="s">
+        <v>464</v>
       </c>
     </row>
     <row r="292" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Largest number in K swaps
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harsh\Desktop\Data-Structures-and-Algorithms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AEF1112-60D9-4440-A9CC-0B5D0DFA77F4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{477E33C0-C004-4981-B455-5B9CBE464148}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -2069,7 +2069,7 @@
   <dimension ref="A1:D498"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A286" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C298" sqref="C298"/>
+      <selection activeCell="C300" sqref="C300"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -5255,8 +5255,8 @@
       <c r="B298" s="6" t="s">
         <v>277</v>
       </c>
-      <c r="C298" s="4" t="s">
-        <v>4</v>
+      <c r="C298" s="11" t="s">
+        <v>464</v>
       </c>
     </row>
     <row r="299" spans="1:4" ht="21">
@@ -5266,8 +5266,8 @@
       <c r="B299" s="6" t="s">
         <v>278</v>
       </c>
-      <c r="C299" s="4" t="s">
-        <v>4</v>
+      <c r="C299" s="11" t="s">
+        <v>464</v>
       </c>
     </row>
     <row r="300" spans="1:4" ht="21">

</xml_diff>

<commit_message>
Partition of a set into K subsets with equal sum
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harsh\Desktop\Data-Structures-and-Algorithms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{477E33C0-C004-4981-B455-5B9CBE464148}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D528362-7920-4AAC-912B-5D4C20C5F01D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1423" uniqueCount="499">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1424" uniqueCount="500">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1522,6 +1522,9 @@
   </si>
   <si>
     <t>same</t>
+  </si>
+  <si>
+    <t>Hard, Must revise</t>
   </si>
 </sst>
 </file>
@@ -2068,8 +2071,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:D498"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A286" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C300" sqref="C300"/>
+    <sheetView tabSelected="1" topLeftCell="A292" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C304" sqref="C304"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -5255,7 +5258,7 @@
       <c r="B298" s="6" t="s">
         <v>277</v>
       </c>
-      <c r="C298" s="11" t="s">
+      <c r="C298" s="21" t="s">
         <v>464</v>
       </c>
     </row>
@@ -5310,8 +5313,11 @@
       <c r="B303" s="6" t="s">
         <v>282</v>
       </c>
-      <c r="C303" s="4" t="s">
-        <v>4</v>
+      <c r="C303" s="21" t="s">
+        <v>464</v>
+      </c>
+      <c r="D303" t="s">
+        <v>499</v>
       </c>
     </row>
     <row r="304" spans="1:4" ht="21">

</xml_diff>

<commit_message>
Find shortest unique prefix for every word in a given list
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harsh\Desktop\Data-Structures-and-Algorithms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{889EE37F-1E21-42DF-AC0F-F729D39FF164}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14E2687B-774A-46FF-8C8F-B84111CB4C52}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -2072,7 +2072,7 @@
   <dimension ref="A1:D498"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A412" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C420" sqref="C420"/>
+      <selection activeCell="C421" sqref="C421"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -6556,8 +6556,8 @@
       <c r="B420" s="6" t="s">
         <v>388</v>
       </c>
-      <c r="C420" s="4" t="s">
-        <v>4</v>
+      <c r="C420" s="11" t="s">
+        <v>464</v>
       </c>
     </row>
     <row r="421" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Coin Change Problem : Count minimum number of coins.
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harsh\Desktop\Data-Structures-and-Algorithms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ACBE3F0-23E1-4252-BD22-F3464C845458}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F78AC08C-EE44-47DB-9F81-0127F098DA62}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1425" uniqueCount="501">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1428" uniqueCount="502">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1528,6 +1528,9 @@
   </si>
   <si>
     <t>No. of ways. Space : O(N) Time : O(MN)</t>
+  </si>
+  <si>
+    <t>Coin Change Problem : Minimim no. of coins</t>
   </si>
 </sst>
 </file>
@@ -2072,10 +2075,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
-  <dimension ref="A1:D498"/>
+  <dimension ref="A1:D499"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A424" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C427" sqref="C427"/>
+      <selection activeCell="B428" sqref="B428"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -6634,10 +6637,10 @@
         <v>392</v>
       </c>
       <c r="B428" s="6" t="s">
-        <v>394</v>
-      </c>
-      <c r="C428" s="4" t="s">
-        <v>4</v>
+        <v>501</v>
+      </c>
+      <c r="C428" s="11" t="s">
+        <v>464</v>
       </c>
     </row>
     <row r="429" spans="1:4" ht="21">
@@ -6645,7 +6648,7 @@
         <v>392</v>
       </c>
       <c r="B429" s="6" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C429" s="4" t="s">
         <v>4</v>
@@ -6656,7 +6659,7 @@
         <v>392</v>
       </c>
       <c r="B430" s="6" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="C430" s="4" t="s">
         <v>4</v>
@@ -6667,7 +6670,7 @@
         <v>392</v>
       </c>
       <c r="B431" s="6" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="C431" s="4" t="s">
         <v>4</v>
@@ -6678,7 +6681,7 @@
         <v>392</v>
       </c>
       <c r="B432" s="6" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="C432" s="4" t="s">
         <v>4</v>
@@ -6689,7 +6692,7 @@
         <v>392</v>
       </c>
       <c r="B433" s="6" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="C433" s="4" t="s">
         <v>4</v>
@@ -6700,7 +6703,7 @@
         <v>392</v>
       </c>
       <c r="B434" s="6" t="s">
-        <v>272</v>
+        <v>399</v>
       </c>
       <c r="C434" s="4" t="s">
         <v>4</v>
@@ -6711,7 +6714,7 @@
         <v>392</v>
       </c>
       <c r="B435" s="6" t="s">
-        <v>400</v>
+        <v>272</v>
       </c>
       <c r="C435" s="4" t="s">
         <v>4</v>
@@ -6722,7 +6725,7 @@
         <v>392</v>
       </c>
       <c r="B436" s="6" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="C436" s="4" t="s">
         <v>4</v>
@@ -6733,7 +6736,7 @@
         <v>392</v>
       </c>
       <c r="B437" s="6" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="C437" s="4" t="s">
         <v>4</v>
@@ -6744,7 +6747,7 @@
         <v>392</v>
       </c>
       <c r="B438" s="6" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="C438" s="4" t="s">
         <v>4</v>
@@ -6755,7 +6758,7 @@
         <v>392</v>
       </c>
       <c r="B439" s="6" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="C439" s="4" t="s">
         <v>4</v>
@@ -6766,7 +6769,7 @@
         <v>392</v>
       </c>
       <c r="B440" s="6" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="C440" s="4" t="s">
         <v>4</v>
@@ -6777,7 +6780,7 @@
         <v>392</v>
       </c>
       <c r="B441" s="6" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="C441" s="4" t="s">
         <v>4</v>
@@ -6788,7 +6791,7 @@
         <v>392</v>
       </c>
       <c r="B442" s="6" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="C442" s="4" t="s">
         <v>4</v>
@@ -6799,7 +6802,7 @@
         <v>392</v>
       </c>
       <c r="B443" s="6" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="C443" s="4" t="s">
         <v>4</v>
@@ -6810,7 +6813,7 @@
         <v>392</v>
       </c>
       <c r="B444" s="6" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="C444" s="4" t="s">
         <v>4</v>
@@ -6821,7 +6824,7 @@
         <v>392</v>
       </c>
       <c r="B445" s="6" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="C445" s="4" t="s">
         <v>4</v>
@@ -6832,7 +6835,7 @@
         <v>392</v>
       </c>
       <c r="B446" s="6" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="C446" s="4" t="s">
         <v>4</v>
@@ -6843,7 +6846,7 @@
         <v>392</v>
       </c>
       <c r="B447" s="6" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C447" s="4" t="s">
         <v>4</v>
@@ -6854,7 +6857,7 @@
         <v>392</v>
       </c>
       <c r="B448" s="6" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="C448" s="4" t="s">
         <v>4</v>
@@ -6865,7 +6868,7 @@
         <v>392</v>
       </c>
       <c r="B449" s="6" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C449" s="4" t="s">
         <v>4</v>
@@ -6876,7 +6879,7 @@
         <v>392</v>
       </c>
       <c r="B450" s="6" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C450" s="4" t="s">
         <v>4</v>
@@ -6887,7 +6890,7 @@
         <v>392</v>
       </c>
       <c r="B451" s="6" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C451" s="4" t="s">
         <v>4</v>
@@ -6898,7 +6901,7 @@
         <v>392</v>
       </c>
       <c r="B452" s="6" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C452" s="4" t="s">
         <v>4</v>
@@ -6909,7 +6912,7 @@
         <v>392</v>
       </c>
       <c r="B453" s="6" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="C453" s="4" t="s">
         <v>4</v>
@@ -6920,7 +6923,7 @@
         <v>392</v>
       </c>
       <c r="B454" s="6" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="C454" s="4" t="s">
         <v>4</v>
@@ -6931,7 +6934,7 @@
         <v>392</v>
       </c>
       <c r="B455" s="6" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="C455" s="4" t="s">
         <v>4</v>
@@ -6942,7 +6945,7 @@
         <v>392</v>
       </c>
       <c r="B456" s="6" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="C456" s="4" t="s">
         <v>4</v>
@@ -6953,7 +6956,7 @@
         <v>392</v>
       </c>
       <c r="B457" s="6" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="C457" s="4" t="s">
         <v>4</v>
@@ -6964,7 +6967,7 @@
         <v>392</v>
       </c>
       <c r="B458" s="6" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="C458" s="4" t="s">
         <v>4</v>
@@ -6975,7 +6978,7 @@
         <v>392</v>
       </c>
       <c r="B459" s="6" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="C459" s="4" t="s">
         <v>4</v>
@@ -6986,7 +6989,7 @@
         <v>392</v>
       </c>
       <c r="B460" s="6" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C460" s="4" t="s">
         <v>4</v>
@@ -6997,7 +7000,7 @@
         <v>392</v>
       </c>
       <c r="B461" s="6" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="C461" s="4" t="s">
         <v>4</v>
@@ -7008,7 +7011,7 @@
         <v>392</v>
       </c>
       <c r="B462" s="6" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="C462" s="4" t="s">
         <v>4</v>
@@ -7019,7 +7022,7 @@
         <v>392</v>
       </c>
       <c r="B463" s="6" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="C463" s="4" t="s">
         <v>4</v>
@@ -7030,7 +7033,7 @@
         <v>392</v>
       </c>
       <c r="B464" s="6" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="C464" s="4" t="s">
         <v>4</v>
@@ -7041,7 +7044,7 @@
         <v>392</v>
       </c>
       <c r="B465" s="6" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="C465" s="4" t="s">
         <v>4</v>
@@ -7052,7 +7055,7 @@
         <v>392</v>
       </c>
       <c r="B466" s="6" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C466" s="4" t="s">
         <v>4</v>
@@ -7063,7 +7066,7 @@
         <v>392</v>
       </c>
       <c r="B467" s="6" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="C467" s="4" t="s">
         <v>4</v>
@@ -7074,7 +7077,7 @@
         <v>392</v>
       </c>
       <c r="B468" s="6" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C468" s="4" t="s">
         <v>4</v>
@@ -7085,7 +7088,7 @@
         <v>392</v>
       </c>
       <c r="B469" s="6" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C469" s="4" t="s">
         <v>4</v>
@@ -7096,7 +7099,7 @@
         <v>392</v>
       </c>
       <c r="B470" s="6" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="C470" s="4" t="s">
         <v>4</v>
@@ -7107,7 +7110,7 @@
         <v>392</v>
       </c>
       <c r="B471" s="6" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="C471" s="4" t="s">
         <v>4</v>
@@ -7118,7 +7121,7 @@
         <v>392</v>
       </c>
       <c r="B472" s="6" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="C472" s="4" t="s">
         <v>4</v>
@@ -7129,7 +7132,7 @@
         <v>392</v>
       </c>
       <c r="B473" s="6" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="C473" s="4" t="s">
         <v>4</v>
@@ -7140,7 +7143,7 @@
         <v>392</v>
       </c>
       <c r="B474" s="6" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="C474" s="4" t="s">
         <v>4</v>
@@ -7151,7 +7154,7 @@
         <v>392</v>
       </c>
       <c r="B475" s="6" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="C475" s="4" t="s">
         <v>4</v>
@@ -7162,7 +7165,7 @@
         <v>392</v>
       </c>
       <c r="B476" s="6" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="C476" s="4" t="s">
         <v>4</v>
@@ -7173,7 +7176,7 @@
         <v>392</v>
       </c>
       <c r="B477" s="6" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="C477" s="4" t="s">
         <v>4</v>
@@ -7184,7 +7187,7 @@
         <v>392</v>
       </c>
       <c r="B478" s="6" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="C478" s="4" t="s">
         <v>4</v>
@@ -7195,7 +7198,7 @@
         <v>392</v>
       </c>
       <c r="B479" s="6" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="C479" s="4" t="s">
         <v>4</v>
@@ -7206,7 +7209,7 @@
         <v>392</v>
       </c>
       <c r="B480" s="6" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="C480" s="4" t="s">
         <v>4</v>
@@ -7217,7 +7220,7 @@
         <v>392</v>
       </c>
       <c r="B481" s="6" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="C481" s="4" t="s">
         <v>4</v>
@@ -7228,7 +7231,7 @@
         <v>392</v>
       </c>
       <c r="B482" s="6" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="C482" s="4" t="s">
         <v>4</v>
@@ -7239,7 +7242,7 @@
         <v>392</v>
       </c>
       <c r="B483" s="6" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="C483" s="4" t="s">
         <v>4</v>
@@ -7250,7 +7253,7 @@
         <v>392</v>
       </c>
       <c r="B484" s="6" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="C484" s="4" t="s">
         <v>4</v>
@@ -7261,7 +7264,7 @@
         <v>392</v>
       </c>
       <c r="B485" s="6" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="C485" s="4" t="s">
         <v>4</v>
@@ -7272,38 +7275,38 @@
         <v>392</v>
       </c>
       <c r="B486" s="6" t="s">
+        <v>450</v>
+      </c>
+      <c r="C486" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="487" spans="1:3" ht="21">
+      <c r="A487" s="5" t="s">
+        <v>392</v>
+      </c>
+      <c r="B487" s="6" t="s">
         <v>451</v>
       </c>
-      <c r="C486" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="487" spans="1:3" ht="21">
-      <c r="B487" s="7"/>
-      <c r="C487" s="4"/>
+      <c r="C487" s="4" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="488" spans="1:3" ht="21">
-      <c r="A488" s="8"/>
       <c r="B488" s="7"/>
       <c r="C488" s="4"/>
     </row>
     <row r="489" spans="1:3" ht="21">
-      <c r="A489" s="5" t="s">
-        <v>452</v>
-      </c>
-      <c r="B489" s="6" t="s">
-        <v>453</v>
-      </c>
-      <c r="C489" s="4" t="s">
-        <v>4</v>
-      </c>
+      <c r="A489" s="8"/>
+      <c r="B489" s="7"/>
+      <c r="C489" s="4"/>
     </row>
     <row r="490" spans="1:3" ht="21">
       <c r="A490" s="5" t="s">
         <v>452</v>
       </c>
       <c r="B490" s="6" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="C490" s="4" t="s">
         <v>4</v>
@@ -7314,7 +7317,7 @@
         <v>452</v>
       </c>
       <c r="B491" s="6" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="C491" s="4" t="s">
         <v>4</v>
@@ -7325,7 +7328,7 @@
         <v>452</v>
       </c>
       <c r="B492" s="6" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="C492" s="4" t="s">
         <v>4</v>
@@ -7336,7 +7339,7 @@
         <v>452</v>
       </c>
       <c r="B493" s="6" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="C493" s="4" t="s">
         <v>4</v>
@@ -7347,7 +7350,7 @@
         <v>452</v>
       </c>
       <c r="B494" s="6" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="C494" s="4" t="s">
         <v>4</v>
@@ -7358,7 +7361,7 @@
         <v>452</v>
       </c>
       <c r="B495" s="6" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="C495" s="4" t="s">
         <v>4</v>
@@ -7369,7 +7372,7 @@
         <v>452</v>
       </c>
       <c r="B496" s="6" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="C496" s="4" t="s">
         <v>4</v>
@@ -7380,7 +7383,7 @@
         <v>452</v>
       </c>
       <c r="B497" s="6" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="C497" s="4" t="s">
         <v>4</v>
@@ -7391,9 +7394,20 @@
         <v>452</v>
       </c>
       <c r="B498" s="6" t="s">
+        <v>461</v>
+      </c>
+      <c r="C498" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="499" spans="1:3" ht="21">
+      <c r="A499" s="5" t="s">
+        <v>452</v>
+      </c>
+      <c r="B499" s="6" t="s">
         <v>462</v>
       </c>
-      <c r="C498" s="4" t="s">
+      <c r="C499" s="4" t="s">
         <v>4</v>
       </c>
     </row>
@@ -7772,75 +7786,75 @@
     <hyperlink ref="B423" r:id="rId371" xr:uid="{8B0A00A3-6AC0-DF46-AD87-A4DA016A2A00}"/>
     <hyperlink ref="B424" r:id="rId372" xr:uid="{62A81CB4-A961-C543-B31C-92059DB6C105}"/>
     <hyperlink ref="B427" r:id="rId373" xr:uid="{08030975-009C-C34A-A875-72FE2718F44C}"/>
-    <hyperlink ref="B428" r:id="rId374" xr:uid="{A113C7A9-2359-B643-9C08-E845813439C0}"/>
-    <hyperlink ref="B429" r:id="rId375" xr:uid="{FE300343-4633-AD47-A64D-2086629EB398}"/>
-    <hyperlink ref="B430" r:id="rId376" xr:uid="{4FC9F782-D38F-C642-A863-887B17AD05CD}"/>
-    <hyperlink ref="B431" r:id="rId377" xr:uid="{830C5466-10E3-7A48-B3E7-35C15A1CA4EF}"/>
-    <hyperlink ref="B432" r:id="rId378" xr:uid="{1B987077-E9D3-6F40-89EE-0D4E7180D884}"/>
-    <hyperlink ref="B433" r:id="rId379" xr:uid="{D4843E1F-7226-864E-A4BB-264D5A487B6D}"/>
-    <hyperlink ref="B434" r:id="rId380" xr:uid="{61816592-2D19-9946-8253-47A60218F2EA}"/>
-    <hyperlink ref="B435" r:id="rId381" xr:uid="{736C840F-19A3-0A4B-8863-ECB772B46385}"/>
-    <hyperlink ref="B436" r:id="rId382" xr:uid="{05A238AD-3C5B-C546-94E9-75BBF964711A}"/>
-    <hyperlink ref="B437" r:id="rId383" xr:uid="{7029629C-3F2A-4A49-997B-CFE86EC8B3C2}"/>
-    <hyperlink ref="B438" r:id="rId384" xr:uid="{ADA66B57-2FAC-AB42-BD83-4931708F3AB5}"/>
-    <hyperlink ref="B439" r:id="rId385" xr:uid="{F16BF1F9-755B-B045-B9A8-0B97E3BAC8B0}"/>
-    <hyperlink ref="B440" r:id="rId386" xr:uid="{ECCE930A-B960-234C-81EC-4B8514282AE9}"/>
-    <hyperlink ref="B441" r:id="rId387" xr:uid="{7AA58141-7D24-7C42-A0C1-F852B21CFFD9}"/>
-    <hyperlink ref="B442" r:id="rId388" xr:uid="{B1FCB47D-7921-3446-B2C7-72CBA815D056}"/>
-    <hyperlink ref="B443" r:id="rId389" xr:uid="{8C547719-AA03-3543-B31F-7300674AF4C5}"/>
-    <hyperlink ref="B444" r:id="rId390" xr:uid="{09922668-AFC0-F242-860E-9967E0F0FEF4}"/>
-    <hyperlink ref="B445" r:id="rId391" xr:uid="{0DA963DA-238B-D44E-9E03-6E6BD933B35E}"/>
-    <hyperlink ref="B446" r:id="rId392" xr:uid="{89518AFF-2526-C845-BC9D-95FE77AF416E}"/>
-    <hyperlink ref="B447" r:id="rId393" xr:uid="{FAECBBBE-196C-7A41-A0FB-E0597CB2CF51}"/>
-    <hyperlink ref="B448" r:id="rId394" xr:uid="{8126B039-0B25-B040-A0F6-C3457341A2E9}"/>
-    <hyperlink ref="B449" r:id="rId395" xr:uid="{6CB326E6-E698-EB42-884B-C89FFA33E3BA}"/>
-    <hyperlink ref="B450" r:id="rId396" xr:uid="{8C97EFD1-933F-A44F-A1CF-6386233104A2}"/>
-    <hyperlink ref="B451" r:id="rId397" xr:uid="{8F019F07-8532-E147-8BE1-4EBE833F61CA}"/>
-    <hyperlink ref="B452" r:id="rId398" xr:uid="{00F1A08F-3767-784A-97A3-4603DE38BACC}"/>
-    <hyperlink ref="B453" r:id="rId399" xr:uid="{2A84ADCB-071F-9A48-994D-7A838307EFD8}"/>
-    <hyperlink ref="B454" r:id="rId400" xr:uid="{132F8C6D-D5E8-6440-AC4E-B81EA2100416}"/>
-    <hyperlink ref="B455" r:id="rId401" xr:uid="{2DA6EAC2-1A1D-754F-9613-226CBC7890AF}"/>
-    <hyperlink ref="B456" r:id="rId402" xr:uid="{05BED99A-4562-D14E-8627-D07CF5335A9B}"/>
-    <hyperlink ref="B457" r:id="rId403" xr:uid="{111D902A-3F60-2D4B-89D3-5BCBD8AA38DD}"/>
-    <hyperlink ref="B458" r:id="rId404" xr:uid="{F19236BE-AC32-3542-9214-DFC3BAE04ED0}"/>
-    <hyperlink ref="B459" r:id="rId405" xr:uid="{4D97CD96-EA1B-664E-9380-EFD27077D273}"/>
-    <hyperlink ref="B460" r:id="rId406" xr:uid="{49A46D91-633F-A148-ACFA-49B7D1AA4B33}"/>
-    <hyperlink ref="B461" r:id="rId407" xr:uid="{7C3B7901-67E3-EA4D-BC64-21A78BC03AC6}"/>
-    <hyperlink ref="B462" r:id="rId408" xr:uid="{B27CA8C3-D34F-5E4D-94A5-11D14AFD0F82}"/>
-    <hyperlink ref="B463" r:id="rId409" xr:uid="{8FECE038-9764-5E4A-8C6E-9B3209812651}"/>
-    <hyperlink ref="B464" r:id="rId410" xr:uid="{95696D4B-89CB-5640-BE92-53B3C043F7EB}"/>
-    <hyperlink ref="B465" r:id="rId411" xr:uid="{DA74B737-802A-4944-A93E-0B9C8417630B}"/>
-    <hyperlink ref="B466" r:id="rId412" xr:uid="{B2C4C168-50FA-AF41-8F56-9E70613CF17D}"/>
-    <hyperlink ref="B468" r:id="rId413" xr:uid="{B7090C60-AC27-3F4F-8F0D-42F0791928C6}"/>
-    <hyperlink ref="B467" r:id="rId414" xr:uid="{07400041-66C6-514B-B3E3-427F2947C2B7}"/>
-    <hyperlink ref="B469" r:id="rId415" xr:uid="{B7E78172-8FB8-4E42-87D8-6A4654D79C62}"/>
-    <hyperlink ref="B470" r:id="rId416" xr:uid="{9A5D4670-BC64-334A-88CF-6F8287692C5E}"/>
-    <hyperlink ref="B471" r:id="rId417" xr:uid="{604283B6-53BC-044F-8D9D-E6094E798317}"/>
-    <hyperlink ref="B472" r:id="rId418" xr:uid="{5EB15AC7-3E0E-E44C-A5B9-32F30F234B5A}"/>
-    <hyperlink ref="B473" r:id="rId419" xr:uid="{3076BD5F-4B23-4146-A50A-499C9FF4C3D2}"/>
-    <hyperlink ref="B474" r:id="rId420" xr:uid="{6A29D9C2-1E78-1B43-A251-0AB0A97FA70E}"/>
-    <hyperlink ref="B475" r:id="rId421" xr:uid="{00597D5E-D693-DF4E-84C0-47E58A6ACA8F}"/>
-    <hyperlink ref="B476" r:id="rId422" xr:uid="{48640988-9964-0B4C-A014-83E2CEB3D632}"/>
-    <hyperlink ref="B477" r:id="rId423" xr:uid="{617AADC9-7534-FE45-96B0-EF4C1867B793}"/>
-    <hyperlink ref="B478" r:id="rId424" xr:uid="{7F8CDAA4-5094-8E4E-961B-41CDE5ACC0C0}"/>
-    <hyperlink ref="B479" r:id="rId425" xr:uid="{63F28ABD-12CF-5947-80DA-229E3CA3133E}"/>
-    <hyperlink ref="B486" r:id="rId426" xr:uid="{0A1DB92C-3315-1942-B27D-4B90986A6D9D}"/>
-    <hyperlink ref="B485" r:id="rId427" xr:uid="{11738B67-CADD-5D45-8417-8BE7A03FC79F}"/>
-    <hyperlink ref="B484" r:id="rId428" xr:uid="{B2B23748-D9E4-BE4F-A93E-49ECB4063831}"/>
-    <hyperlink ref="B483" r:id="rId429" xr:uid="{A2FB8A72-37B9-7E4A-B050-FD6CD20BCE73}"/>
-    <hyperlink ref="B482" r:id="rId430" xr:uid="{5A93C9AF-BFEB-EB40-95AC-C309ED09A604}"/>
-    <hyperlink ref="B481" r:id="rId431" xr:uid="{CC203923-2DC2-874B-B846-A8455E3CC2F2}"/>
-    <hyperlink ref="B480" r:id="rId432" xr:uid="{FCB0246E-0179-B447-B3CE-C60CDB388472}"/>
-    <hyperlink ref="B489" r:id="rId433" xr:uid="{F06CEE72-8CA4-C547-862C-39B86CD3226A}"/>
-    <hyperlink ref="B490" r:id="rId434" xr:uid="{CB3045F2-8D63-0F4E-85BC-AF016DB4F247}"/>
-    <hyperlink ref="B491" r:id="rId435" xr:uid="{667D57F5-E5AD-674F-A2F5-AFF4A14E4026}"/>
-    <hyperlink ref="B492" r:id="rId436" xr:uid="{27A13A65-56CE-BF4D-BA0D-EB87D910272D}"/>
-    <hyperlink ref="B493" r:id="rId437" xr:uid="{2C72A52E-6F06-0246-AEB5-93CD0DEA8866}"/>
-    <hyperlink ref="B494" r:id="rId438" xr:uid="{24B29046-B4DD-674B-9EDF-6C94BEC3FDD8}"/>
-    <hyperlink ref="B495" r:id="rId439" xr:uid="{D018EBC3-3FB3-AC4D-9D64-D218345A46C8}"/>
-    <hyperlink ref="B498" r:id="rId440" xr:uid="{1E1D3964-01E0-3145-ACFE-B6A5BF0EECB0}"/>
-    <hyperlink ref="B496" r:id="rId441" xr:uid="{FA0E5061-A7E2-C045-9671-1CD9446D1932}"/>
-    <hyperlink ref="B497" r:id="rId442" location=":~:text=Given%20an%20integer%20n%2C%20calculate,*%2C%20%2F%20and%20pow().&amp;text=A%20Simple%20Solution%20is%20to%20repeatedly%20add%20n%20to%20result." xr:uid="{92704F5B-7B31-2F42-80DD-764B2206D9DB}"/>
+    <hyperlink ref="B429" r:id="rId374" xr:uid="{A113C7A9-2359-B643-9C08-E845813439C0}"/>
+    <hyperlink ref="B430" r:id="rId375" xr:uid="{FE300343-4633-AD47-A64D-2086629EB398}"/>
+    <hyperlink ref="B431" r:id="rId376" xr:uid="{4FC9F782-D38F-C642-A863-887B17AD05CD}"/>
+    <hyperlink ref="B432" r:id="rId377" xr:uid="{830C5466-10E3-7A48-B3E7-35C15A1CA4EF}"/>
+    <hyperlink ref="B433" r:id="rId378" xr:uid="{1B987077-E9D3-6F40-89EE-0D4E7180D884}"/>
+    <hyperlink ref="B434" r:id="rId379" xr:uid="{D4843E1F-7226-864E-A4BB-264D5A487B6D}"/>
+    <hyperlink ref="B435" r:id="rId380" xr:uid="{61816592-2D19-9946-8253-47A60218F2EA}"/>
+    <hyperlink ref="B436" r:id="rId381" xr:uid="{736C840F-19A3-0A4B-8863-ECB772B46385}"/>
+    <hyperlink ref="B437" r:id="rId382" xr:uid="{05A238AD-3C5B-C546-94E9-75BBF964711A}"/>
+    <hyperlink ref="B438" r:id="rId383" xr:uid="{7029629C-3F2A-4A49-997B-CFE86EC8B3C2}"/>
+    <hyperlink ref="B439" r:id="rId384" xr:uid="{ADA66B57-2FAC-AB42-BD83-4931708F3AB5}"/>
+    <hyperlink ref="B440" r:id="rId385" xr:uid="{F16BF1F9-755B-B045-B9A8-0B97E3BAC8B0}"/>
+    <hyperlink ref="B441" r:id="rId386" xr:uid="{ECCE930A-B960-234C-81EC-4B8514282AE9}"/>
+    <hyperlink ref="B442" r:id="rId387" xr:uid="{7AA58141-7D24-7C42-A0C1-F852B21CFFD9}"/>
+    <hyperlink ref="B443" r:id="rId388" xr:uid="{B1FCB47D-7921-3446-B2C7-72CBA815D056}"/>
+    <hyperlink ref="B444" r:id="rId389" xr:uid="{8C547719-AA03-3543-B31F-7300674AF4C5}"/>
+    <hyperlink ref="B445" r:id="rId390" xr:uid="{09922668-AFC0-F242-860E-9967E0F0FEF4}"/>
+    <hyperlink ref="B446" r:id="rId391" xr:uid="{0DA963DA-238B-D44E-9E03-6E6BD933B35E}"/>
+    <hyperlink ref="B447" r:id="rId392" xr:uid="{89518AFF-2526-C845-BC9D-95FE77AF416E}"/>
+    <hyperlink ref="B448" r:id="rId393" xr:uid="{FAECBBBE-196C-7A41-A0FB-E0597CB2CF51}"/>
+    <hyperlink ref="B449" r:id="rId394" xr:uid="{8126B039-0B25-B040-A0F6-C3457341A2E9}"/>
+    <hyperlink ref="B450" r:id="rId395" xr:uid="{6CB326E6-E698-EB42-884B-C89FFA33E3BA}"/>
+    <hyperlink ref="B451" r:id="rId396" xr:uid="{8C97EFD1-933F-A44F-A1CF-6386233104A2}"/>
+    <hyperlink ref="B452" r:id="rId397" xr:uid="{8F019F07-8532-E147-8BE1-4EBE833F61CA}"/>
+    <hyperlink ref="B453" r:id="rId398" xr:uid="{00F1A08F-3767-784A-97A3-4603DE38BACC}"/>
+    <hyperlink ref="B454" r:id="rId399" xr:uid="{2A84ADCB-071F-9A48-994D-7A838307EFD8}"/>
+    <hyperlink ref="B455" r:id="rId400" xr:uid="{132F8C6D-D5E8-6440-AC4E-B81EA2100416}"/>
+    <hyperlink ref="B456" r:id="rId401" xr:uid="{2DA6EAC2-1A1D-754F-9613-226CBC7890AF}"/>
+    <hyperlink ref="B457" r:id="rId402" xr:uid="{05BED99A-4562-D14E-8627-D07CF5335A9B}"/>
+    <hyperlink ref="B458" r:id="rId403" xr:uid="{111D902A-3F60-2D4B-89D3-5BCBD8AA38DD}"/>
+    <hyperlink ref="B459" r:id="rId404" xr:uid="{F19236BE-AC32-3542-9214-DFC3BAE04ED0}"/>
+    <hyperlink ref="B460" r:id="rId405" xr:uid="{4D97CD96-EA1B-664E-9380-EFD27077D273}"/>
+    <hyperlink ref="B461" r:id="rId406" xr:uid="{49A46D91-633F-A148-ACFA-49B7D1AA4B33}"/>
+    <hyperlink ref="B462" r:id="rId407" xr:uid="{7C3B7901-67E3-EA4D-BC64-21A78BC03AC6}"/>
+    <hyperlink ref="B463" r:id="rId408" xr:uid="{B27CA8C3-D34F-5E4D-94A5-11D14AFD0F82}"/>
+    <hyperlink ref="B464" r:id="rId409" xr:uid="{8FECE038-9764-5E4A-8C6E-9B3209812651}"/>
+    <hyperlink ref="B465" r:id="rId410" xr:uid="{95696D4B-89CB-5640-BE92-53B3C043F7EB}"/>
+    <hyperlink ref="B466" r:id="rId411" xr:uid="{DA74B737-802A-4944-A93E-0B9C8417630B}"/>
+    <hyperlink ref="B467" r:id="rId412" xr:uid="{B2C4C168-50FA-AF41-8F56-9E70613CF17D}"/>
+    <hyperlink ref="B469" r:id="rId413" xr:uid="{B7090C60-AC27-3F4F-8F0D-42F0791928C6}"/>
+    <hyperlink ref="B468" r:id="rId414" xr:uid="{07400041-66C6-514B-B3E3-427F2947C2B7}"/>
+    <hyperlink ref="B470" r:id="rId415" xr:uid="{B7E78172-8FB8-4E42-87D8-6A4654D79C62}"/>
+    <hyperlink ref="B471" r:id="rId416" xr:uid="{9A5D4670-BC64-334A-88CF-6F8287692C5E}"/>
+    <hyperlink ref="B472" r:id="rId417" xr:uid="{604283B6-53BC-044F-8D9D-E6094E798317}"/>
+    <hyperlink ref="B473" r:id="rId418" xr:uid="{5EB15AC7-3E0E-E44C-A5B9-32F30F234B5A}"/>
+    <hyperlink ref="B474" r:id="rId419" xr:uid="{3076BD5F-4B23-4146-A50A-499C9FF4C3D2}"/>
+    <hyperlink ref="B475" r:id="rId420" xr:uid="{6A29D9C2-1E78-1B43-A251-0AB0A97FA70E}"/>
+    <hyperlink ref="B476" r:id="rId421" xr:uid="{00597D5E-D693-DF4E-84C0-47E58A6ACA8F}"/>
+    <hyperlink ref="B477" r:id="rId422" xr:uid="{48640988-9964-0B4C-A014-83E2CEB3D632}"/>
+    <hyperlink ref="B478" r:id="rId423" xr:uid="{617AADC9-7534-FE45-96B0-EF4C1867B793}"/>
+    <hyperlink ref="B479" r:id="rId424" xr:uid="{7F8CDAA4-5094-8E4E-961B-41CDE5ACC0C0}"/>
+    <hyperlink ref="B480" r:id="rId425" xr:uid="{63F28ABD-12CF-5947-80DA-229E3CA3133E}"/>
+    <hyperlink ref="B487" r:id="rId426" xr:uid="{0A1DB92C-3315-1942-B27D-4B90986A6D9D}"/>
+    <hyperlink ref="B486" r:id="rId427" xr:uid="{11738B67-CADD-5D45-8417-8BE7A03FC79F}"/>
+    <hyperlink ref="B485" r:id="rId428" xr:uid="{B2B23748-D9E4-BE4F-A93E-49ECB4063831}"/>
+    <hyperlink ref="B484" r:id="rId429" xr:uid="{A2FB8A72-37B9-7E4A-B050-FD6CD20BCE73}"/>
+    <hyperlink ref="B483" r:id="rId430" xr:uid="{5A93C9AF-BFEB-EB40-95AC-C309ED09A604}"/>
+    <hyperlink ref="B482" r:id="rId431" xr:uid="{CC203923-2DC2-874B-B846-A8455E3CC2F2}"/>
+    <hyperlink ref="B481" r:id="rId432" xr:uid="{FCB0246E-0179-B447-B3CE-C60CDB388472}"/>
+    <hyperlink ref="B490" r:id="rId433" xr:uid="{F06CEE72-8CA4-C547-862C-39B86CD3226A}"/>
+    <hyperlink ref="B491" r:id="rId434" xr:uid="{CB3045F2-8D63-0F4E-85BC-AF016DB4F247}"/>
+    <hyperlink ref="B492" r:id="rId435" xr:uid="{667D57F5-E5AD-674F-A2F5-AFF4A14E4026}"/>
+    <hyperlink ref="B493" r:id="rId436" xr:uid="{27A13A65-56CE-BF4D-BA0D-EB87D910272D}"/>
+    <hyperlink ref="B494" r:id="rId437" xr:uid="{2C72A52E-6F06-0246-AEB5-93CD0DEA8866}"/>
+    <hyperlink ref="B495" r:id="rId438" xr:uid="{24B29046-B4DD-674B-9EDF-6C94BEC3FDD8}"/>
+    <hyperlink ref="B496" r:id="rId439" xr:uid="{D018EBC3-3FB3-AC4D-9D64-D218345A46C8}"/>
+    <hyperlink ref="B499" r:id="rId440" xr:uid="{1E1D3964-01E0-3145-ACFE-B6A5BF0EECB0}"/>
+    <hyperlink ref="B497" r:id="rId441" xr:uid="{FA0E5061-A7E2-C045-9671-1CD9446D1932}"/>
+    <hyperlink ref="B498" r:id="rId442" location=":~:text=Given%20an%20integer%20n%2C%20calculate,*%2C%20%2F%20and%20pow().&amp;text=A%20Simple%20Solution%20is%20to%20repeatedly%20add%20n%20to%20result." xr:uid="{92704F5B-7B31-2F42-80DD-764B2206D9DB}"/>
     <hyperlink ref="B370" r:id="rId443" xr:uid="{A48B1A24-83B1-7A4C-8129-CD37804DF849}"/>
     <hyperlink ref="B2" r:id="rId444" xr:uid="{E07D4FE5-46C7-AC4D-9E01-2300AA43B58A}"/>
     <hyperlink ref="B39" r:id="rId445" xr:uid="{F2DE2162-BD02-7549-AC1A-27455F78131F}"/>
@@ -7862,8 +7876,9 @@
     <hyperlink ref="B401" r:id="rId461" xr:uid="{3DC6B9E0-05DC-4888-815A-CDBB63BDF598}"/>
     <hyperlink ref="B252" r:id="rId462" xr:uid="{0EDEAD3A-F3F0-4D9B-BF0D-E0DDAE13C611}"/>
     <hyperlink ref="B293" r:id="rId463" xr:uid="{127345A9-71F3-49D6-AB7A-BF4305D0F725}"/>
+    <hyperlink ref="B428" r:id="rId464" xr:uid="{C4A51DBE-F043-4951-B51A-E48796555D08}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId464"/>
+  <pageSetup orientation="portrait" r:id="rId465"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
0 - 1 Knapsack Problem
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harsh\Desktop\Data-Structures-and-Algorithms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F78AC08C-EE44-47DB-9F81-0127F098DA62}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB3FCEF2-ACD3-4644-9531-05CF05AC8A4C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -2078,7 +2078,7 @@
   <dimension ref="A1:D499"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A424" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B428" sqref="B428"/>
+      <selection activeCell="C431" sqref="C431"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -6650,8 +6650,8 @@
       <c r="B429" s="6" t="s">
         <v>394</v>
       </c>
-      <c r="C429" s="4" t="s">
-        <v>4</v>
+      <c r="C429" s="11" t="s">
+        <v>464</v>
       </c>
     </row>
     <row r="430" spans="1:4" ht="21">

</xml_diff>

<commit_message>
Minimum Number of Taps to Open to Water a Garden
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harsh\Desktop\Data-Structures-and-Algorithms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB3FCEF2-ACD3-4644-9531-05CF05AC8A4C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9B6BA78-F931-4861-97D1-4F8D006246EB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1428" uniqueCount="502">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1431" uniqueCount="503">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1531,6 +1531,9 @@
   </si>
   <si>
     <t>Coin Change Problem : Minimim no. of coins</t>
+  </si>
+  <si>
+    <t>Minimum Number of Taps to Open to Water a Garden</t>
   </si>
 </sst>
 </file>
@@ -2075,10 +2078,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
-  <dimension ref="A1:D499"/>
+  <dimension ref="A1:D500"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A424" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C431" sqref="C431"/>
+      <selection activeCell="B430" sqref="B430"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -6659,10 +6662,10 @@
         <v>392</v>
       </c>
       <c r="B430" s="6" t="s">
-        <v>395</v>
-      </c>
-      <c r="C430" s="4" t="s">
-        <v>4</v>
+        <v>502</v>
+      </c>
+      <c r="C430" s="11" t="s">
+        <v>464</v>
       </c>
     </row>
     <row r="431" spans="1:4" ht="21">
@@ -6670,7 +6673,7 @@
         <v>392</v>
       </c>
       <c r="B431" s="6" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="C431" s="4" t="s">
         <v>4</v>
@@ -6681,7 +6684,7 @@
         <v>392</v>
       </c>
       <c r="B432" s="6" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="C432" s="4" t="s">
         <v>4</v>
@@ -6692,7 +6695,7 @@
         <v>392</v>
       </c>
       <c r="B433" s="6" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="C433" s="4" t="s">
         <v>4</v>
@@ -6703,7 +6706,7 @@
         <v>392</v>
       </c>
       <c r="B434" s="6" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="C434" s="4" t="s">
         <v>4</v>
@@ -6714,7 +6717,7 @@
         <v>392</v>
       </c>
       <c r="B435" s="6" t="s">
-        <v>272</v>
+        <v>399</v>
       </c>
       <c r="C435" s="4" t="s">
         <v>4</v>
@@ -6725,7 +6728,7 @@
         <v>392</v>
       </c>
       <c r="B436" s="6" t="s">
-        <v>400</v>
+        <v>272</v>
       </c>
       <c r="C436" s="4" t="s">
         <v>4</v>
@@ -6736,7 +6739,7 @@
         <v>392</v>
       </c>
       <c r="B437" s="6" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="C437" s="4" t="s">
         <v>4</v>
@@ -6747,7 +6750,7 @@
         <v>392</v>
       </c>
       <c r="B438" s="6" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="C438" s="4" t="s">
         <v>4</v>
@@ -6758,7 +6761,7 @@
         <v>392</v>
       </c>
       <c r="B439" s="6" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="C439" s="4" t="s">
         <v>4</v>
@@ -6769,7 +6772,7 @@
         <v>392</v>
       </c>
       <c r="B440" s="6" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="C440" s="4" t="s">
         <v>4</v>
@@ -6780,7 +6783,7 @@
         <v>392</v>
       </c>
       <c r="B441" s="6" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="C441" s="4" t="s">
         <v>4</v>
@@ -6791,7 +6794,7 @@
         <v>392</v>
       </c>
       <c r="B442" s="6" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="C442" s="4" t="s">
         <v>4</v>
@@ -6802,7 +6805,7 @@
         <v>392</v>
       </c>
       <c r="B443" s="6" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="C443" s="4" t="s">
         <v>4</v>
@@ -6813,7 +6816,7 @@
         <v>392</v>
       </c>
       <c r="B444" s="6" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="C444" s="4" t="s">
         <v>4</v>
@@ -6824,7 +6827,7 @@
         <v>392</v>
       </c>
       <c r="B445" s="6" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="C445" s="4" t="s">
         <v>4</v>
@@ -6835,7 +6838,7 @@
         <v>392</v>
       </c>
       <c r="B446" s="6" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="C446" s="4" t="s">
         <v>4</v>
@@ -6846,7 +6849,7 @@
         <v>392</v>
       </c>
       <c r="B447" s="6" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="C447" s="4" t="s">
         <v>4</v>
@@ -6857,7 +6860,7 @@
         <v>392</v>
       </c>
       <c r="B448" s="6" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C448" s="4" t="s">
         <v>4</v>
@@ -6868,7 +6871,7 @@
         <v>392</v>
       </c>
       <c r="B449" s="6" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="C449" s="4" t="s">
         <v>4</v>
@@ -6879,7 +6882,7 @@
         <v>392</v>
       </c>
       <c r="B450" s="6" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C450" s="4" t="s">
         <v>4</v>
@@ -6890,7 +6893,7 @@
         <v>392</v>
       </c>
       <c r="B451" s="6" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C451" s="4" t="s">
         <v>4</v>
@@ -6901,7 +6904,7 @@
         <v>392</v>
       </c>
       <c r="B452" s="6" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C452" s="4" t="s">
         <v>4</v>
@@ -6912,7 +6915,7 @@
         <v>392</v>
       </c>
       <c r="B453" s="6" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C453" s="4" t="s">
         <v>4</v>
@@ -6923,7 +6926,7 @@
         <v>392</v>
       </c>
       <c r="B454" s="6" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="C454" s="4" t="s">
         <v>4</v>
@@ -6934,7 +6937,7 @@
         <v>392</v>
       </c>
       <c r="B455" s="6" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="C455" s="4" t="s">
         <v>4</v>
@@ -6945,7 +6948,7 @@
         <v>392</v>
       </c>
       <c r="B456" s="6" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="C456" s="4" t="s">
         <v>4</v>
@@ -6956,7 +6959,7 @@
         <v>392</v>
       </c>
       <c r="B457" s="6" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="C457" s="4" t="s">
         <v>4</v>
@@ -6967,7 +6970,7 @@
         <v>392</v>
       </c>
       <c r="B458" s="6" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="C458" s="4" t="s">
         <v>4</v>
@@ -6978,7 +6981,7 @@
         <v>392</v>
       </c>
       <c r="B459" s="6" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="C459" s="4" t="s">
         <v>4</v>
@@ -6989,7 +6992,7 @@
         <v>392</v>
       </c>
       <c r="B460" s="6" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="C460" s="4" t="s">
         <v>4</v>
@@ -7000,7 +7003,7 @@
         <v>392</v>
       </c>
       <c r="B461" s="6" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C461" s="4" t="s">
         <v>4</v>
@@ -7011,7 +7014,7 @@
         <v>392</v>
       </c>
       <c r="B462" s="6" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="C462" s="4" t="s">
         <v>4</v>
@@ -7022,7 +7025,7 @@
         <v>392</v>
       </c>
       <c r="B463" s="6" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="C463" s="4" t="s">
         <v>4</v>
@@ -7033,7 +7036,7 @@
         <v>392</v>
       </c>
       <c r="B464" s="6" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="C464" s="4" t="s">
         <v>4</v>
@@ -7044,7 +7047,7 @@
         <v>392</v>
       </c>
       <c r="B465" s="6" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="C465" s="4" t="s">
         <v>4</v>
@@ -7055,7 +7058,7 @@
         <v>392</v>
       </c>
       <c r="B466" s="6" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="C466" s="4" t="s">
         <v>4</v>
@@ -7066,7 +7069,7 @@
         <v>392</v>
       </c>
       <c r="B467" s="6" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C467" s="4" t="s">
         <v>4</v>
@@ -7077,7 +7080,7 @@
         <v>392</v>
       </c>
       <c r="B468" s="6" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="C468" s="4" t="s">
         <v>4</v>
@@ -7088,7 +7091,7 @@
         <v>392</v>
       </c>
       <c r="B469" s="6" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C469" s="4" t="s">
         <v>4</v>
@@ -7099,7 +7102,7 @@
         <v>392</v>
       </c>
       <c r="B470" s="6" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C470" s="4" t="s">
         <v>4</v>
@@ -7110,7 +7113,7 @@
         <v>392</v>
       </c>
       <c r="B471" s="6" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="C471" s="4" t="s">
         <v>4</v>
@@ -7121,7 +7124,7 @@
         <v>392</v>
       </c>
       <c r="B472" s="6" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="C472" s="4" t="s">
         <v>4</v>
@@ -7132,7 +7135,7 @@
         <v>392</v>
       </c>
       <c r="B473" s="6" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="C473" s="4" t="s">
         <v>4</v>
@@ -7143,7 +7146,7 @@
         <v>392</v>
       </c>
       <c r="B474" s="6" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="C474" s="4" t="s">
         <v>4</v>
@@ -7154,7 +7157,7 @@
         <v>392</v>
       </c>
       <c r="B475" s="6" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="C475" s="4" t="s">
         <v>4</v>
@@ -7165,7 +7168,7 @@
         <v>392</v>
       </c>
       <c r="B476" s="6" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="C476" s="4" t="s">
         <v>4</v>
@@ -7176,7 +7179,7 @@
         <v>392</v>
       </c>
       <c r="B477" s="6" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="C477" s="4" t="s">
         <v>4</v>
@@ -7187,7 +7190,7 @@
         <v>392</v>
       </c>
       <c r="B478" s="6" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="C478" s="4" t="s">
         <v>4</v>
@@ -7198,7 +7201,7 @@
         <v>392</v>
       </c>
       <c r="B479" s="6" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="C479" s="4" t="s">
         <v>4</v>
@@ -7209,7 +7212,7 @@
         <v>392</v>
       </c>
       <c r="B480" s="6" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="C480" s="4" t="s">
         <v>4</v>
@@ -7220,7 +7223,7 @@
         <v>392</v>
       </c>
       <c r="B481" s="6" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="C481" s="4" t="s">
         <v>4</v>
@@ -7231,7 +7234,7 @@
         <v>392</v>
       </c>
       <c r="B482" s="6" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="C482" s="4" t="s">
         <v>4</v>
@@ -7242,7 +7245,7 @@
         <v>392</v>
       </c>
       <c r="B483" s="6" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="C483" s="4" t="s">
         <v>4</v>
@@ -7253,7 +7256,7 @@
         <v>392</v>
       </c>
       <c r="B484" s="6" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="C484" s="4" t="s">
         <v>4</v>
@@ -7264,7 +7267,7 @@
         <v>392</v>
       </c>
       <c r="B485" s="6" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="C485" s="4" t="s">
         <v>4</v>
@@ -7275,7 +7278,7 @@
         <v>392</v>
       </c>
       <c r="B486" s="6" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="C486" s="4" t="s">
         <v>4</v>
@@ -7286,38 +7289,38 @@
         <v>392</v>
       </c>
       <c r="B487" s="6" t="s">
+        <v>450</v>
+      </c>
+      <c r="C487" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="488" spans="1:3" ht="21">
+      <c r="A488" s="5" t="s">
+        <v>392</v>
+      </c>
+      <c r="B488" s="6" t="s">
         <v>451</v>
       </c>
-      <c r="C487" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="488" spans="1:3" ht="21">
-      <c r="B488" s="7"/>
-      <c r="C488" s="4"/>
+      <c r="C488" s="4" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="489" spans="1:3" ht="21">
-      <c r="A489" s="8"/>
       <c r="B489" s="7"/>
       <c r="C489" s="4"/>
     </row>
     <row r="490" spans="1:3" ht="21">
-      <c r="A490" s="5" t="s">
-        <v>452</v>
-      </c>
-      <c r="B490" s="6" t="s">
-        <v>453</v>
-      </c>
-      <c r="C490" s="4" t="s">
-        <v>4</v>
-      </c>
+      <c r="A490" s="8"/>
+      <c r="B490" s="7"/>
+      <c r="C490" s="4"/>
     </row>
     <row r="491" spans="1:3" ht="21">
       <c r="A491" s="5" t="s">
         <v>452</v>
       </c>
       <c r="B491" s="6" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="C491" s="4" t="s">
         <v>4</v>
@@ -7328,7 +7331,7 @@
         <v>452</v>
       </c>
       <c r="B492" s="6" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="C492" s="4" t="s">
         <v>4</v>
@@ -7339,7 +7342,7 @@
         <v>452</v>
       </c>
       <c r="B493" s="6" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="C493" s="4" t="s">
         <v>4</v>
@@ -7350,7 +7353,7 @@
         <v>452</v>
       </c>
       <c r="B494" s="6" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="C494" s="4" t="s">
         <v>4</v>
@@ -7361,7 +7364,7 @@
         <v>452</v>
       </c>
       <c r="B495" s="6" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="C495" s="4" t="s">
         <v>4</v>
@@ -7372,7 +7375,7 @@
         <v>452</v>
       </c>
       <c r="B496" s="6" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="C496" s="4" t="s">
         <v>4</v>
@@ -7383,7 +7386,7 @@
         <v>452</v>
       </c>
       <c r="B497" s="6" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="C497" s="4" t="s">
         <v>4</v>
@@ -7394,7 +7397,7 @@
         <v>452</v>
       </c>
       <c r="B498" s="6" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="C498" s="4" t="s">
         <v>4</v>
@@ -7405,9 +7408,20 @@
         <v>452</v>
       </c>
       <c r="B499" s="6" t="s">
+        <v>461</v>
+      </c>
+      <c r="C499" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="500" spans="1:3" ht="21">
+      <c r="A500" s="5" t="s">
+        <v>452</v>
+      </c>
+      <c r="B500" s="6" t="s">
         <v>462</v>
       </c>
-      <c r="C499" s="4" t="s">
+      <c r="C500" s="4" t="s">
         <v>4</v>
       </c>
     </row>
@@ -7787,74 +7801,74 @@
     <hyperlink ref="B424" r:id="rId372" xr:uid="{62A81CB4-A961-C543-B31C-92059DB6C105}"/>
     <hyperlink ref="B427" r:id="rId373" xr:uid="{08030975-009C-C34A-A875-72FE2718F44C}"/>
     <hyperlink ref="B429" r:id="rId374" xr:uid="{A113C7A9-2359-B643-9C08-E845813439C0}"/>
-    <hyperlink ref="B430" r:id="rId375" xr:uid="{FE300343-4633-AD47-A64D-2086629EB398}"/>
-    <hyperlink ref="B431" r:id="rId376" xr:uid="{4FC9F782-D38F-C642-A863-887B17AD05CD}"/>
-    <hyperlink ref="B432" r:id="rId377" xr:uid="{830C5466-10E3-7A48-B3E7-35C15A1CA4EF}"/>
-    <hyperlink ref="B433" r:id="rId378" xr:uid="{1B987077-E9D3-6F40-89EE-0D4E7180D884}"/>
-    <hyperlink ref="B434" r:id="rId379" xr:uid="{D4843E1F-7226-864E-A4BB-264D5A487B6D}"/>
-    <hyperlink ref="B435" r:id="rId380" xr:uid="{61816592-2D19-9946-8253-47A60218F2EA}"/>
-    <hyperlink ref="B436" r:id="rId381" xr:uid="{736C840F-19A3-0A4B-8863-ECB772B46385}"/>
-    <hyperlink ref="B437" r:id="rId382" xr:uid="{05A238AD-3C5B-C546-94E9-75BBF964711A}"/>
-    <hyperlink ref="B438" r:id="rId383" xr:uid="{7029629C-3F2A-4A49-997B-CFE86EC8B3C2}"/>
-    <hyperlink ref="B439" r:id="rId384" xr:uid="{ADA66B57-2FAC-AB42-BD83-4931708F3AB5}"/>
-    <hyperlink ref="B440" r:id="rId385" xr:uid="{F16BF1F9-755B-B045-B9A8-0B97E3BAC8B0}"/>
-    <hyperlink ref="B441" r:id="rId386" xr:uid="{ECCE930A-B960-234C-81EC-4B8514282AE9}"/>
-    <hyperlink ref="B442" r:id="rId387" xr:uid="{7AA58141-7D24-7C42-A0C1-F852B21CFFD9}"/>
-    <hyperlink ref="B443" r:id="rId388" xr:uid="{B1FCB47D-7921-3446-B2C7-72CBA815D056}"/>
-    <hyperlink ref="B444" r:id="rId389" xr:uid="{8C547719-AA03-3543-B31F-7300674AF4C5}"/>
-    <hyperlink ref="B445" r:id="rId390" xr:uid="{09922668-AFC0-F242-860E-9967E0F0FEF4}"/>
-    <hyperlink ref="B446" r:id="rId391" xr:uid="{0DA963DA-238B-D44E-9E03-6E6BD933B35E}"/>
-    <hyperlink ref="B447" r:id="rId392" xr:uid="{89518AFF-2526-C845-BC9D-95FE77AF416E}"/>
-    <hyperlink ref="B448" r:id="rId393" xr:uid="{FAECBBBE-196C-7A41-A0FB-E0597CB2CF51}"/>
-    <hyperlink ref="B449" r:id="rId394" xr:uid="{8126B039-0B25-B040-A0F6-C3457341A2E9}"/>
-    <hyperlink ref="B450" r:id="rId395" xr:uid="{6CB326E6-E698-EB42-884B-C89FFA33E3BA}"/>
-    <hyperlink ref="B451" r:id="rId396" xr:uid="{8C97EFD1-933F-A44F-A1CF-6386233104A2}"/>
-    <hyperlink ref="B452" r:id="rId397" xr:uid="{8F019F07-8532-E147-8BE1-4EBE833F61CA}"/>
-    <hyperlink ref="B453" r:id="rId398" xr:uid="{00F1A08F-3767-784A-97A3-4603DE38BACC}"/>
-    <hyperlink ref="B454" r:id="rId399" xr:uid="{2A84ADCB-071F-9A48-994D-7A838307EFD8}"/>
-    <hyperlink ref="B455" r:id="rId400" xr:uid="{132F8C6D-D5E8-6440-AC4E-B81EA2100416}"/>
-    <hyperlink ref="B456" r:id="rId401" xr:uid="{2DA6EAC2-1A1D-754F-9613-226CBC7890AF}"/>
-    <hyperlink ref="B457" r:id="rId402" xr:uid="{05BED99A-4562-D14E-8627-D07CF5335A9B}"/>
-    <hyperlink ref="B458" r:id="rId403" xr:uid="{111D902A-3F60-2D4B-89D3-5BCBD8AA38DD}"/>
-    <hyperlink ref="B459" r:id="rId404" xr:uid="{F19236BE-AC32-3542-9214-DFC3BAE04ED0}"/>
-    <hyperlink ref="B460" r:id="rId405" xr:uid="{4D97CD96-EA1B-664E-9380-EFD27077D273}"/>
-    <hyperlink ref="B461" r:id="rId406" xr:uid="{49A46D91-633F-A148-ACFA-49B7D1AA4B33}"/>
-    <hyperlink ref="B462" r:id="rId407" xr:uid="{7C3B7901-67E3-EA4D-BC64-21A78BC03AC6}"/>
-    <hyperlink ref="B463" r:id="rId408" xr:uid="{B27CA8C3-D34F-5E4D-94A5-11D14AFD0F82}"/>
-    <hyperlink ref="B464" r:id="rId409" xr:uid="{8FECE038-9764-5E4A-8C6E-9B3209812651}"/>
-    <hyperlink ref="B465" r:id="rId410" xr:uid="{95696D4B-89CB-5640-BE92-53B3C043F7EB}"/>
-    <hyperlink ref="B466" r:id="rId411" xr:uid="{DA74B737-802A-4944-A93E-0B9C8417630B}"/>
-    <hyperlink ref="B467" r:id="rId412" xr:uid="{B2C4C168-50FA-AF41-8F56-9E70613CF17D}"/>
-    <hyperlink ref="B469" r:id="rId413" xr:uid="{B7090C60-AC27-3F4F-8F0D-42F0791928C6}"/>
-    <hyperlink ref="B468" r:id="rId414" xr:uid="{07400041-66C6-514B-B3E3-427F2947C2B7}"/>
-    <hyperlink ref="B470" r:id="rId415" xr:uid="{B7E78172-8FB8-4E42-87D8-6A4654D79C62}"/>
-    <hyperlink ref="B471" r:id="rId416" xr:uid="{9A5D4670-BC64-334A-88CF-6F8287692C5E}"/>
-    <hyperlink ref="B472" r:id="rId417" xr:uid="{604283B6-53BC-044F-8D9D-E6094E798317}"/>
-    <hyperlink ref="B473" r:id="rId418" xr:uid="{5EB15AC7-3E0E-E44C-A5B9-32F30F234B5A}"/>
-    <hyperlink ref="B474" r:id="rId419" xr:uid="{3076BD5F-4B23-4146-A50A-499C9FF4C3D2}"/>
-    <hyperlink ref="B475" r:id="rId420" xr:uid="{6A29D9C2-1E78-1B43-A251-0AB0A97FA70E}"/>
-    <hyperlink ref="B476" r:id="rId421" xr:uid="{00597D5E-D693-DF4E-84C0-47E58A6ACA8F}"/>
-    <hyperlink ref="B477" r:id="rId422" xr:uid="{48640988-9964-0B4C-A014-83E2CEB3D632}"/>
-    <hyperlink ref="B478" r:id="rId423" xr:uid="{617AADC9-7534-FE45-96B0-EF4C1867B793}"/>
-    <hyperlink ref="B479" r:id="rId424" xr:uid="{7F8CDAA4-5094-8E4E-961B-41CDE5ACC0C0}"/>
-    <hyperlink ref="B480" r:id="rId425" xr:uid="{63F28ABD-12CF-5947-80DA-229E3CA3133E}"/>
-    <hyperlink ref="B487" r:id="rId426" xr:uid="{0A1DB92C-3315-1942-B27D-4B90986A6D9D}"/>
-    <hyperlink ref="B486" r:id="rId427" xr:uid="{11738B67-CADD-5D45-8417-8BE7A03FC79F}"/>
-    <hyperlink ref="B485" r:id="rId428" xr:uid="{B2B23748-D9E4-BE4F-A93E-49ECB4063831}"/>
-    <hyperlink ref="B484" r:id="rId429" xr:uid="{A2FB8A72-37B9-7E4A-B050-FD6CD20BCE73}"/>
-    <hyperlink ref="B483" r:id="rId430" xr:uid="{5A93C9AF-BFEB-EB40-95AC-C309ED09A604}"/>
-    <hyperlink ref="B482" r:id="rId431" xr:uid="{CC203923-2DC2-874B-B846-A8455E3CC2F2}"/>
-    <hyperlink ref="B481" r:id="rId432" xr:uid="{FCB0246E-0179-B447-B3CE-C60CDB388472}"/>
-    <hyperlink ref="B490" r:id="rId433" xr:uid="{F06CEE72-8CA4-C547-862C-39B86CD3226A}"/>
-    <hyperlink ref="B491" r:id="rId434" xr:uid="{CB3045F2-8D63-0F4E-85BC-AF016DB4F247}"/>
-    <hyperlink ref="B492" r:id="rId435" xr:uid="{667D57F5-E5AD-674F-A2F5-AFF4A14E4026}"/>
-    <hyperlink ref="B493" r:id="rId436" xr:uid="{27A13A65-56CE-BF4D-BA0D-EB87D910272D}"/>
-    <hyperlink ref="B494" r:id="rId437" xr:uid="{2C72A52E-6F06-0246-AEB5-93CD0DEA8866}"/>
-    <hyperlink ref="B495" r:id="rId438" xr:uid="{24B29046-B4DD-674B-9EDF-6C94BEC3FDD8}"/>
-    <hyperlink ref="B496" r:id="rId439" xr:uid="{D018EBC3-3FB3-AC4D-9D64-D218345A46C8}"/>
-    <hyperlink ref="B499" r:id="rId440" xr:uid="{1E1D3964-01E0-3145-ACFE-B6A5BF0EECB0}"/>
-    <hyperlink ref="B497" r:id="rId441" xr:uid="{FA0E5061-A7E2-C045-9671-1CD9446D1932}"/>
-    <hyperlink ref="B498" r:id="rId442" location=":~:text=Given%20an%20integer%20n%2C%20calculate,*%2C%20%2F%20and%20pow().&amp;text=A%20Simple%20Solution%20is%20to%20repeatedly%20add%20n%20to%20result." xr:uid="{92704F5B-7B31-2F42-80DD-764B2206D9DB}"/>
+    <hyperlink ref="B431" r:id="rId375" xr:uid="{FE300343-4633-AD47-A64D-2086629EB398}"/>
+    <hyperlink ref="B432" r:id="rId376" xr:uid="{4FC9F782-D38F-C642-A863-887B17AD05CD}"/>
+    <hyperlink ref="B433" r:id="rId377" xr:uid="{830C5466-10E3-7A48-B3E7-35C15A1CA4EF}"/>
+    <hyperlink ref="B434" r:id="rId378" xr:uid="{1B987077-E9D3-6F40-89EE-0D4E7180D884}"/>
+    <hyperlink ref="B435" r:id="rId379" xr:uid="{D4843E1F-7226-864E-A4BB-264D5A487B6D}"/>
+    <hyperlink ref="B436" r:id="rId380" xr:uid="{61816592-2D19-9946-8253-47A60218F2EA}"/>
+    <hyperlink ref="B437" r:id="rId381" xr:uid="{736C840F-19A3-0A4B-8863-ECB772B46385}"/>
+    <hyperlink ref="B438" r:id="rId382" xr:uid="{05A238AD-3C5B-C546-94E9-75BBF964711A}"/>
+    <hyperlink ref="B439" r:id="rId383" xr:uid="{7029629C-3F2A-4A49-997B-CFE86EC8B3C2}"/>
+    <hyperlink ref="B440" r:id="rId384" xr:uid="{ADA66B57-2FAC-AB42-BD83-4931708F3AB5}"/>
+    <hyperlink ref="B441" r:id="rId385" xr:uid="{F16BF1F9-755B-B045-B9A8-0B97E3BAC8B0}"/>
+    <hyperlink ref="B442" r:id="rId386" xr:uid="{ECCE930A-B960-234C-81EC-4B8514282AE9}"/>
+    <hyperlink ref="B443" r:id="rId387" xr:uid="{7AA58141-7D24-7C42-A0C1-F852B21CFFD9}"/>
+    <hyperlink ref="B444" r:id="rId388" xr:uid="{B1FCB47D-7921-3446-B2C7-72CBA815D056}"/>
+    <hyperlink ref="B445" r:id="rId389" xr:uid="{8C547719-AA03-3543-B31F-7300674AF4C5}"/>
+    <hyperlink ref="B446" r:id="rId390" xr:uid="{09922668-AFC0-F242-860E-9967E0F0FEF4}"/>
+    <hyperlink ref="B447" r:id="rId391" xr:uid="{0DA963DA-238B-D44E-9E03-6E6BD933B35E}"/>
+    <hyperlink ref="B448" r:id="rId392" xr:uid="{89518AFF-2526-C845-BC9D-95FE77AF416E}"/>
+    <hyperlink ref="B449" r:id="rId393" xr:uid="{FAECBBBE-196C-7A41-A0FB-E0597CB2CF51}"/>
+    <hyperlink ref="B450" r:id="rId394" xr:uid="{8126B039-0B25-B040-A0F6-C3457341A2E9}"/>
+    <hyperlink ref="B451" r:id="rId395" xr:uid="{6CB326E6-E698-EB42-884B-C89FFA33E3BA}"/>
+    <hyperlink ref="B452" r:id="rId396" xr:uid="{8C97EFD1-933F-A44F-A1CF-6386233104A2}"/>
+    <hyperlink ref="B453" r:id="rId397" xr:uid="{8F019F07-8532-E147-8BE1-4EBE833F61CA}"/>
+    <hyperlink ref="B454" r:id="rId398" xr:uid="{00F1A08F-3767-784A-97A3-4603DE38BACC}"/>
+    <hyperlink ref="B455" r:id="rId399" xr:uid="{2A84ADCB-071F-9A48-994D-7A838307EFD8}"/>
+    <hyperlink ref="B456" r:id="rId400" xr:uid="{132F8C6D-D5E8-6440-AC4E-B81EA2100416}"/>
+    <hyperlink ref="B457" r:id="rId401" xr:uid="{2DA6EAC2-1A1D-754F-9613-226CBC7890AF}"/>
+    <hyperlink ref="B458" r:id="rId402" xr:uid="{05BED99A-4562-D14E-8627-D07CF5335A9B}"/>
+    <hyperlink ref="B459" r:id="rId403" xr:uid="{111D902A-3F60-2D4B-89D3-5BCBD8AA38DD}"/>
+    <hyperlink ref="B460" r:id="rId404" xr:uid="{F19236BE-AC32-3542-9214-DFC3BAE04ED0}"/>
+    <hyperlink ref="B461" r:id="rId405" xr:uid="{4D97CD96-EA1B-664E-9380-EFD27077D273}"/>
+    <hyperlink ref="B462" r:id="rId406" xr:uid="{49A46D91-633F-A148-ACFA-49B7D1AA4B33}"/>
+    <hyperlink ref="B463" r:id="rId407" xr:uid="{7C3B7901-67E3-EA4D-BC64-21A78BC03AC6}"/>
+    <hyperlink ref="B464" r:id="rId408" xr:uid="{B27CA8C3-D34F-5E4D-94A5-11D14AFD0F82}"/>
+    <hyperlink ref="B465" r:id="rId409" xr:uid="{8FECE038-9764-5E4A-8C6E-9B3209812651}"/>
+    <hyperlink ref="B466" r:id="rId410" xr:uid="{95696D4B-89CB-5640-BE92-53B3C043F7EB}"/>
+    <hyperlink ref="B467" r:id="rId411" xr:uid="{DA74B737-802A-4944-A93E-0B9C8417630B}"/>
+    <hyperlink ref="B468" r:id="rId412" xr:uid="{B2C4C168-50FA-AF41-8F56-9E70613CF17D}"/>
+    <hyperlink ref="B470" r:id="rId413" xr:uid="{B7090C60-AC27-3F4F-8F0D-42F0791928C6}"/>
+    <hyperlink ref="B469" r:id="rId414" xr:uid="{07400041-66C6-514B-B3E3-427F2947C2B7}"/>
+    <hyperlink ref="B471" r:id="rId415" xr:uid="{B7E78172-8FB8-4E42-87D8-6A4654D79C62}"/>
+    <hyperlink ref="B472" r:id="rId416" xr:uid="{9A5D4670-BC64-334A-88CF-6F8287692C5E}"/>
+    <hyperlink ref="B473" r:id="rId417" xr:uid="{604283B6-53BC-044F-8D9D-E6094E798317}"/>
+    <hyperlink ref="B474" r:id="rId418" xr:uid="{5EB15AC7-3E0E-E44C-A5B9-32F30F234B5A}"/>
+    <hyperlink ref="B475" r:id="rId419" xr:uid="{3076BD5F-4B23-4146-A50A-499C9FF4C3D2}"/>
+    <hyperlink ref="B476" r:id="rId420" xr:uid="{6A29D9C2-1E78-1B43-A251-0AB0A97FA70E}"/>
+    <hyperlink ref="B477" r:id="rId421" xr:uid="{00597D5E-D693-DF4E-84C0-47E58A6ACA8F}"/>
+    <hyperlink ref="B478" r:id="rId422" xr:uid="{48640988-9964-0B4C-A014-83E2CEB3D632}"/>
+    <hyperlink ref="B479" r:id="rId423" xr:uid="{617AADC9-7534-FE45-96B0-EF4C1867B793}"/>
+    <hyperlink ref="B480" r:id="rId424" xr:uid="{7F8CDAA4-5094-8E4E-961B-41CDE5ACC0C0}"/>
+    <hyperlink ref="B481" r:id="rId425" xr:uid="{63F28ABD-12CF-5947-80DA-229E3CA3133E}"/>
+    <hyperlink ref="B488" r:id="rId426" xr:uid="{0A1DB92C-3315-1942-B27D-4B90986A6D9D}"/>
+    <hyperlink ref="B487" r:id="rId427" xr:uid="{11738B67-CADD-5D45-8417-8BE7A03FC79F}"/>
+    <hyperlink ref="B486" r:id="rId428" xr:uid="{B2B23748-D9E4-BE4F-A93E-49ECB4063831}"/>
+    <hyperlink ref="B485" r:id="rId429" xr:uid="{A2FB8A72-37B9-7E4A-B050-FD6CD20BCE73}"/>
+    <hyperlink ref="B484" r:id="rId430" xr:uid="{5A93C9AF-BFEB-EB40-95AC-C309ED09A604}"/>
+    <hyperlink ref="B483" r:id="rId431" xr:uid="{CC203923-2DC2-874B-B846-A8455E3CC2F2}"/>
+    <hyperlink ref="B482" r:id="rId432" xr:uid="{FCB0246E-0179-B447-B3CE-C60CDB388472}"/>
+    <hyperlink ref="B491" r:id="rId433" xr:uid="{F06CEE72-8CA4-C547-862C-39B86CD3226A}"/>
+    <hyperlink ref="B492" r:id="rId434" xr:uid="{CB3045F2-8D63-0F4E-85BC-AF016DB4F247}"/>
+    <hyperlink ref="B493" r:id="rId435" xr:uid="{667D57F5-E5AD-674F-A2F5-AFF4A14E4026}"/>
+    <hyperlink ref="B494" r:id="rId436" xr:uid="{27A13A65-56CE-BF4D-BA0D-EB87D910272D}"/>
+    <hyperlink ref="B495" r:id="rId437" xr:uid="{2C72A52E-6F06-0246-AEB5-93CD0DEA8866}"/>
+    <hyperlink ref="B496" r:id="rId438" xr:uid="{24B29046-B4DD-674B-9EDF-6C94BEC3FDD8}"/>
+    <hyperlink ref="B497" r:id="rId439" xr:uid="{D018EBC3-3FB3-AC4D-9D64-D218345A46C8}"/>
+    <hyperlink ref="B500" r:id="rId440" xr:uid="{1E1D3964-01E0-3145-ACFE-B6A5BF0EECB0}"/>
+    <hyperlink ref="B498" r:id="rId441" xr:uid="{FA0E5061-A7E2-C045-9671-1CD9446D1932}"/>
+    <hyperlink ref="B499" r:id="rId442" location=":~:text=Given%20an%20integer%20n%2C%20calculate,*%2C%20%2F%20and%20pow().&amp;text=A%20Simple%20Solution%20is%20to%20repeatedly%20add%20n%20to%20result." xr:uid="{92704F5B-7B31-2F42-80DD-764B2206D9DB}"/>
     <hyperlink ref="B370" r:id="rId443" xr:uid="{A48B1A24-83B1-7A4C-8129-CD37804DF849}"/>
     <hyperlink ref="B2" r:id="rId444" xr:uid="{E07D4FE5-46C7-AC4D-9E01-2300AA43B58A}"/>
     <hyperlink ref="B39" r:id="rId445" xr:uid="{F2DE2162-BD02-7549-AC1A-27455F78131F}"/>
@@ -7877,8 +7891,9 @@
     <hyperlink ref="B252" r:id="rId462" xr:uid="{0EDEAD3A-F3F0-4D9B-BF0D-E0DDAE13C611}"/>
     <hyperlink ref="B293" r:id="rId463" xr:uid="{127345A9-71F3-49D6-AB7A-BF4305D0F725}"/>
     <hyperlink ref="B428" r:id="rId464" xr:uid="{C4A51DBE-F043-4951-B51A-E48796555D08}"/>
+    <hyperlink ref="B430" r:id="rId465" xr:uid="{910FE4FA-F82F-4691-9E2F-22E8206DA592}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId465"/>
+  <pageSetup orientation="portrait" r:id="rId466"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Count minimum number of fountains to be activated to cover the entire garden
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harsh\Desktop\Data-Structures-and-Algorithms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9B6BA78-F931-4861-97D1-4F8D006246EB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD2B8041-4285-4069-B520-AEB66A0E3E59}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1431" uniqueCount="503">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1434" uniqueCount="504">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1534,6 +1534,9 @@
   </si>
   <si>
     <t>Minimum Number of Taps to Open to Water a Garden</t>
+  </si>
+  <si>
+    <t>Count minimum number of fountains to be activated to cover the entire garden</t>
   </si>
 </sst>
 </file>
@@ -1702,7 +1705,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1762,6 +1765,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2078,10 +2084,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
-  <dimension ref="A1:D500"/>
+  <dimension ref="A1:D501"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A424" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B430" sqref="B430"/>
+      <selection activeCell="B432" sqref="B432"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -6672,11 +6678,11 @@
       <c r="A431" s="5" t="s">
         <v>392</v>
       </c>
-      <c r="B431" s="6" t="s">
-        <v>395</v>
-      </c>
-      <c r="C431" s="4" t="s">
-        <v>4</v>
+      <c r="B431" s="24" t="s">
+        <v>503</v>
+      </c>
+      <c r="C431" s="11" t="s">
+        <v>464</v>
       </c>
     </row>
     <row r="432" spans="1:4" ht="21">
@@ -6684,7 +6690,7 @@
         <v>392</v>
       </c>
       <c r="B432" s="6" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="C432" s="4" t="s">
         <v>4</v>
@@ -6695,7 +6701,7 @@
         <v>392</v>
       </c>
       <c r="B433" s="6" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="C433" s="4" t="s">
         <v>4</v>
@@ -6706,7 +6712,7 @@
         <v>392</v>
       </c>
       <c r="B434" s="6" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="C434" s="4" t="s">
         <v>4</v>
@@ -6717,7 +6723,7 @@
         <v>392</v>
       </c>
       <c r="B435" s="6" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="C435" s="4" t="s">
         <v>4</v>
@@ -6728,7 +6734,7 @@
         <v>392</v>
       </c>
       <c r="B436" s="6" t="s">
-        <v>272</v>
+        <v>399</v>
       </c>
       <c r="C436" s="4" t="s">
         <v>4</v>
@@ -6739,7 +6745,7 @@
         <v>392</v>
       </c>
       <c r="B437" s="6" t="s">
-        <v>400</v>
+        <v>272</v>
       </c>
       <c r="C437" s="4" t="s">
         <v>4</v>
@@ -6750,7 +6756,7 @@
         <v>392</v>
       </c>
       <c r="B438" s="6" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="C438" s="4" t="s">
         <v>4</v>
@@ -6761,7 +6767,7 @@
         <v>392</v>
       </c>
       <c r="B439" s="6" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="C439" s="4" t="s">
         <v>4</v>
@@ -6772,7 +6778,7 @@
         <v>392</v>
       </c>
       <c r="B440" s="6" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="C440" s="4" t="s">
         <v>4</v>
@@ -6783,7 +6789,7 @@
         <v>392</v>
       </c>
       <c r="B441" s="6" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="C441" s="4" t="s">
         <v>4</v>
@@ -6794,7 +6800,7 @@
         <v>392</v>
       </c>
       <c r="B442" s="6" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="C442" s="4" t="s">
         <v>4</v>
@@ -6805,7 +6811,7 @@
         <v>392</v>
       </c>
       <c r="B443" s="6" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="C443" s="4" t="s">
         <v>4</v>
@@ -6816,7 +6822,7 @@
         <v>392</v>
       </c>
       <c r="B444" s="6" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="C444" s="4" t="s">
         <v>4</v>
@@ -6827,7 +6833,7 @@
         <v>392</v>
       </c>
       <c r="B445" s="6" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="C445" s="4" t="s">
         <v>4</v>
@@ -6838,7 +6844,7 @@
         <v>392</v>
       </c>
       <c r="B446" s="6" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="C446" s="4" t="s">
         <v>4</v>
@@ -6849,7 +6855,7 @@
         <v>392</v>
       </c>
       <c r="B447" s="6" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="C447" s="4" t="s">
         <v>4</v>
@@ -6860,7 +6866,7 @@
         <v>392</v>
       </c>
       <c r="B448" s="6" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="C448" s="4" t="s">
         <v>4</v>
@@ -6871,7 +6877,7 @@
         <v>392</v>
       </c>
       <c r="B449" s="6" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C449" s="4" t="s">
         <v>4</v>
@@ -6882,7 +6888,7 @@
         <v>392</v>
       </c>
       <c r="B450" s="6" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="C450" s="4" t="s">
         <v>4</v>
@@ -6893,7 +6899,7 @@
         <v>392</v>
       </c>
       <c r="B451" s="6" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C451" s="4" t="s">
         <v>4</v>
@@ -6904,7 +6910,7 @@
         <v>392</v>
       </c>
       <c r="B452" s="6" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C452" s="4" t="s">
         <v>4</v>
@@ -6915,7 +6921,7 @@
         <v>392</v>
       </c>
       <c r="B453" s="6" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C453" s="4" t="s">
         <v>4</v>
@@ -6926,7 +6932,7 @@
         <v>392</v>
       </c>
       <c r="B454" s="6" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C454" s="4" t="s">
         <v>4</v>
@@ -6937,7 +6943,7 @@
         <v>392</v>
       </c>
       <c r="B455" s="6" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="C455" s="4" t="s">
         <v>4</v>
@@ -6948,7 +6954,7 @@
         <v>392</v>
       </c>
       <c r="B456" s="6" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="C456" s="4" t="s">
         <v>4</v>
@@ -6959,7 +6965,7 @@
         <v>392</v>
       </c>
       <c r="B457" s="6" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="C457" s="4" t="s">
         <v>4</v>
@@ -6970,7 +6976,7 @@
         <v>392</v>
       </c>
       <c r="B458" s="6" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="C458" s="4" t="s">
         <v>4</v>
@@ -6981,7 +6987,7 @@
         <v>392</v>
       </c>
       <c r="B459" s="6" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="C459" s="4" t="s">
         <v>4</v>
@@ -6992,7 +6998,7 @@
         <v>392</v>
       </c>
       <c r="B460" s="6" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="C460" s="4" t="s">
         <v>4</v>
@@ -7003,7 +7009,7 @@
         <v>392</v>
       </c>
       <c r="B461" s="6" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="C461" s="4" t="s">
         <v>4</v>
@@ -7014,7 +7020,7 @@
         <v>392</v>
       </c>
       <c r="B462" s="6" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C462" s="4" t="s">
         <v>4</v>
@@ -7025,7 +7031,7 @@
         <v>392</v>
       </c>
       <c r="B463" s="6" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="C463" s="4" t="s">
         <v>4</v>
@@ -7036,7 +7042,7 @@
         <v>392</v>
       </c>
       <c r="B464" s="6" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="C464" s="4" t="s">
         <v>4</v>
@@ -7047,7 +7053,7 @@
         <v>392</v>
       </c>
       <c r="B465" s="6" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="C465" s="4" t="s">
         <v>4</v>
@@ -7058,7 +7064,7 @@
         <v>392</v>
       </c>
       <c r="B466" s="6" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="C466" s="4" t="s">
         <v>4</v>
@@ -7069,7 +7075,7 @@
         <v>392</v>
       </c>
       <c r="B467" s="6" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="C467" s="4" t="s">
         <v>4</v>
@@ -7080,7 +7086,7 @@
         <v>392</v>
       </c>
       <c r="B468" s="6" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C468" s="4" t="s">
         <v>4</v>
@@ -7091,7 +7097,7 @@
         <v>392</v>
       </c>
       <c r="B469" s="6" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="C469" s="4" t="s">
         <v>4</v>
@@ -7102,7 +7108,7 @@
         <v>392</v>
       </c>
       <c r="B470" s="6" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C470" s="4" t="s">
         <v>4</v>
@@ -7113,7 +7119,7 @@
         <v>392</v>
       </c>
       <c r="B471" s="6" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C471" s="4" t="s">
         <v>4</v>
@@ -7124,7 +7130,7 @@
         <v>392</v>
       </c>
       <c r="B472" s="6" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="C472" s="4" t="s">
         <v>4</v>
@@ -7135,7 +7141,7 @@
         <v>392</v>
       </c>
       <c r="B473" s="6" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="C473" s="4" t="s">
         <v>4</v>
@@ -7146,7 +7152,7 @@
         <v>392</v>
       </c>
       <c r="B474" s="6" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="C474" s="4" t="s">
         <v>4</v>
@@ -7157,7 +7163,7 @@
         <v>392</v>
       </c>
       <c r="B475" s="6" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="C475" s="4" t="s">
         <v>4</v>
@@ -7168,7 +7174,7 @@
         <v>392</v>
       </c>
       <c r="B476" s="6" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="C476" s="4" t="s">
         <v>4</v>
@@ -7179,7 +7185,7 @@
         <v>392</v>
       </c>
       <c r="B477" s="6" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="C477" s="4" t="s">
         <v>4</v>
@@ -7190,7 +7196,7 @@
         <v>392</v>
       </c>
       <c r="B478" s="6" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="C478" s="4" t="s">
         <v>4</v>
@@ -7201,7 +7207,7 @@
         <v>392</v>
       </c>
       <c r="B479" s="6" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="C479" s="4" t="s">
         <v>4</v>
@@ -7212,7 +7218,7 @@
         <v>392</v>
       </c>
       <c r="B480" s="6" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="C480" s="4" t="s">
         <v>4</v>
@@ -7223,7 +7229,7 @@
         <v>392</v>
       </c>
       <c r="B481" s="6" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="C481" s="4" t="s">
         <v>4</v>
@@ -7234,7 +7240,7 @@
         <v>392</v>
       </c>
       <c r="B482" s="6" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="C482" s="4" t="s">
         <v>4</v>
@@ -7245,7 +7251,7 @@
         <v>392</v>
       </c>
       <c r="B483" s="6" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="C483" s="4" t="s">
         <v>4</v>
@@ -7256,7 +7262,7 @@
         <v>392</v>
       </c>
       <c r="B484" s="6" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="C484" s="4" t="s">
         <v>4</v>
@@ -7267,7 +7273,7 @@
         <v>392</v>
       </c>
       <c r="B485" s="6" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="C485" s="4" t="s">
         <v>4</v>
@@ -7278,7 +7284,7 @@
         <v>392</v>
       </c>
       <c r="B486" s="6" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="C486" s="4" t="s">
         <v>4</v>
@@ -7289,7 +7295,7 @@
         <v>392</v>
       </c>
       <c r="B487" s="6" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="C487" s="4" t="s">
         <v>4</v>
@@ -7300,38 +7306,38 @@
         <v>392</v>
       </c>
       <c r="B488" s="6" t="s">
+        <v>450</v>
+      </c>
+      <c r="C488" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="489" spans="1:3" ht="21">
+      <c r="A489" s="5" t="s">
+        <v>392</v>
+      </c>
+      <c r="B489" s="6" t="s">
         <v>451</v>
       </c>
-      <c r="C488" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="489" spans="1:3" ht="21">
-      <c r="B489" s="7"/>
-      <c r="C489" s="4"/>
+      <c r="C489" s="4" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="490" spans="1:3" ht="21">
-      <c r="A490" s="8"/>
       <c r="B490" s="7"/>
       <c r="C490" s="4"/>
     </row>
     <row r="491" spans="1:3" ht="21">
-      <c r="A491" s="5" t="s">
-        <v>452</v>
-      </c>
-      <c r="B491" s="6" t="s">
-        <v>453</v>
-      </c>
-      <c r="C491" s="4" t="s">
-        <v>4</v>
-      </c>
+      <c r="A491" s="8"/>
+      <c r="B491" s="7"/>
+      <c r="C491" s="4"/>
     </row>
     <row r="492" spans="1:3" ht="21">
       <c r="A492" s="5" t="s">
         <v>452</v>
       </c>
       <c r="B492" s="6" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="C492" s="4" t="s">
         <v>4</v>
@@ -7342,7 +7348,7 @@
         <v>452</v>
       </c>
       <c r="B493" s="6" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="C493" s="4" t="s">
         <v>4</v>
@@ -7353,7 +7359,7 @@
         <v>452</v>
       </c>
       <c r="B494" s="6" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="C494" s="4" t="s">
         <v>4</v>
@@ -7364,7 +7370,7 @@
         <v>452</v>
       </c>
       <c r="B495" s="6" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="C495" s="4" t="s">
         <v>4</v>
@@ -7375,7 +7381,7 @@
         <v>452</v>
       </c>
       <c r="B496" s="6" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="C496" s="4" t="s">
         <v>4</v>
@@ -7386,7 +7392,7 @@
         <v>452</v>
       </c>
       <c r="B497" s="6" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="C497" s="4" t="s">
         <v>4</v>
@@ -7397,7 +7403,7 @@
         <v>452</v>
       </c>
       <c r="B498" s="6" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="C498" s="4" t="s">
         <v>4</v>
@@ -7408,7 +7414,7 @@
         <v>452</v>
       </c>
       <c r="B499" s="6" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="C499" s="4" t="s">
         <v>4</v>
@@ -7419,9 +7425,20 @@
         <v>452</v>
       </c>
       <c r="B500" s="6" t="s">
+        <v>461</v>
+      </c>
+      <c r="C500" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="501" spans="1:3" ht="21">
+      <c r="A501" s="5" t="s">
+        <v>452</v>
+      </c>
+      <c r="B501" s="6" t="s">
         <v>462</v>
       </c>
-      <c r="C500" s="4" t="s">
+      <c r="C501" s="4" t="s">
         <v>4</v>
       </c>
     </row>
@@ -7801,74 +7818,74 @@
     <hyperlink ref="B424" r:id="rId372" xr:uid="{62A81CB4-A961-C543-B31C-92059DB6C105}"/>
     <hyperlink ref="B427" r:id="rId373" xr:uid="{08030975-009C-C34A-A875-72FE2718F44C}"/>
     <hyperlink ref="B429" r:id="rId374" xr:uid="{A113C7A9-2359-B643-9C08-E845813439C0}"/>
-    <hyperlink ref="B431" r:id="rId375" xr:uid="{FE300343-4633-AD47-A64D-2086629EB398}"/>
-    <hyperlink ref="B432" r:id="rId376" xr:uid="{4FC9F782-D38F-C642-A863-887B17AD05CD}"/>
-    <hyperlink ref="B433" r:id="rId377" xr:uid="{830C5466-10E3-7A48-B3E7-35C15A1CA4EF}"/>
-    <hyperlink ref="B434" r:id="rId378" xr:uid="{1B987077-E9D3-6F40-89EE-0D4E7180D884}"/>
-    <hyperlink ref="B435" r:id="rId379" xr:uid="{D4843E1F-7226-864E-A4BB-264D5A487B6D}"/>
-    <hyperlink ref="B436" r:id="rId380" xr:uid="{61816592-2D19-9946-8253-47A60218F2EA}"/>
-    <hyperlink ref="B437" r:id="rId381" xr:uid="{736C840F-19A3-0A4B-8863-ECB772B46385}"/>
-    <hyperlink ref="B438" r:id="rId382" xr:uid="{05A238AD-3C5B-C546-94E9-75BBF964711A}"/>
-    <hyperlink ref="B439" r:id="rId383" xr:uid="{7029629C-3F2A-4A49-997B-CFE86EC8B3C2}"/>
-    <hyperlink ref="B440" r:id="rId384" xr:uid="{ADA66B57-2FAC-AB42-BD83-4931708F3AB5}"/>
-    <hyperlink ref="B441" r:id="rId385" xr:uid="{F16BF1F9-755B-B045-B9A8-0B97E3BAC8B0}"/>
-    <hyperlink ref="B442" r:id="rId386" xr:uid="{ECCE930A-B960-234C-81EC-4B8514282AE9}"/>
-    <hyperlink ref="B443" r:id="rId387" xr:uid="{7AA58141-7D24-7C42-A0C1-F852B21CFFD9}"/>
-    <hyperlink ref="B444" r:id="rId388" xr:uid="{B1FCB47D-7921-3446-B2C7-72CBA815D056}"/>
-    <hyperlink ref="B445" r:id="rId389" xr:uid="{8C547719-AA03-3543-B31F-7300674AF4C5}"/>
-    <hyperlink ref="B446" r:id="rId390" xr:uid="{09922668-AFC0-F242-860E-9967E0F0FEF4}"/>
-    <hyperlink ref="B447" r:id="rId391" xr:uid="{0DA963DA-238B-D44E-9E03-6E6BD933B35E}"/>
-    <hyperlink ref="B448" r:id="rId392" xr:uid="{89518AFF-2526-C845-BC9D-95FE77AF416E}"/>
-    <hyperlink ref="B449" r:id="rId393" xr:uid="{FAECBBBE-196C-7A41-A0FB-E0597CB2CF51}"/>
-    <hyperlink ref="B450" r:id="rId394" xr:uid="{8126B039-0B25-B040-A0F6-C3457341A2E9}"/>
-    <hyperlink ref="B451" r:id="rId395" xr:uid="{6CB326E6-E698-EB42-884B-C89FFA33E3BA}"/>
-    <hyperlink ref="B452" r:id="rId396" xr:uid="{8C97EFD1-933F-A44F-A1CF-6386233104A2}"/>
-    <hyperlink ref="B453" r:id="rId397" xr:uid="{8F019F07-8532-E147-8BE1-4EBE833F61CA}"/>
-    <hyperlink ref="B454" r:id="rId398" xr:uid="{00F1A08F-3767-784A-97A3-4603DE38BACC}"/>
-    <hyperlink ref="B455" r:id="rId399" xr:uid="{2A84ADCB-071F-9A48-994D-7A838307EFD8}"/>
-    <hyperlink ref="B456" r:id="rId400" xr:uid="{132F8C6D-D5E8-6440-AC4E-B81EA2100416}"/>
-    <hyperlink ref="B457" r:id="rId401" xr:uid="{2DA6EAC2-1A1D-754F-9613-226CBC7890AF}"/>
-    <hyperlink ref="B458" r:id="rId402" xr:uid="{05BED99A-4562-D14E-8627-D07CF5335A9B}"/>
-    <hyperlink ref="B459" r:id="rId403" xr:uid="{111D902A-3F60-2D4B-89D3-5BCBD8AA38DD}"/>
-    <hyperlink ref="B460" r:id="rId404" xr:uid="{F19236BE-AC32-3542-9214-DFC3BAE04ED0}"/>
-    <hyperlink ref="B461" r:id="rId405" xr:uid="{4D97CD96-EA1B-664E-9380-EFD27077D273}"/>
-    <hyperlink ref="B462" r:id="rId406" xr:uid="{49A46D91-633F-A148-ACFA-49B7D1AA4B33}"/>
-    <hyperlink ref="B463" r:id="rId407" xr:uid="{7C3B7901-67E3-EA4D-BC64-21A78BC03AC6}"/>
-    <hyperlink ref="B464" r:id="rId408" xr:uid="{B27CA8C3-D34F-5E4D-94A5-11D14AFD0F82}"/>
-    <hyperlink ref="B465" r:id="rId409" xr:uid="{8FECE038-9764-5E4A-8C6E-9B3209812651}"/>
-    <hyperlink ref="B466" r:id="rId410" xr:uid="{95696D4B-89CB-5640-BE92-53B3C043F7EB}"/>
-    <hyperlink ref="B467" r:id="rId411" xr:uid="{DA74B737-802A-4944-A93E-0B9C8417630B}"/>
-    <hyperlink ref="B468" r:id="rId412" xr:uid="{B2C4C168-50FA-AF41-8F56-9E70613CF17D}"/>
-    <hyperlink ref="B470" r:id="rId413" xr:uid="{B7090C60-AC27-3F4F-8F0D-42F0791928C6}"/>
-    <hyperlink ref="B469" r:id="rId414" xr:uid="{07400041-66C6-514B-B3E3-427F2947C2B7}"/>
-    <hyperlink ref="B471" r:id="rId415" xr:uid="{B7E78172-8FB8-4E42-87D8-6A4654D79C62}"/>
-    <hyperlink ref="B472" r:id="rId416" xr:uid="{9A5D4670-BC64-334A-88CF-6F8287692C5E}"/>
-    <hyperlink ref="B473" r:id="rId417" xr:uid="{604283B6-53BC-044F-8D9D-E6094E798317}"/>
-    <hyperlink ref="B474" r:id="rId418" xr:uid="{5EB15AC7-3E0E-E44C-A5B9-32F30F234B5A}"/>
-    <hyperlink ref="B475" r:id="rId419" xr:uid="{3076BD5F-4B23-4146-A50A-499C9FF4C3D2}"/>
-    <hyperlink ref="B476" r:id="rId420" xr:uid="{6A29D9C2-1E78-1B43-A251-0AB0A97FA70E}"/>
-    <hyperlink ref="B477" r:id="rId421" xr:uid="{00597D5E-D693-DF4E-84C0-47E58A6ACA8F}"/>
-    <hyperlink ref="B478" r:id="rId422" xr:uid="{48640988-9964-0B4C-A014-83E2CEB3D632}"/>
-    <hyperlink ref="B479" r:id="rId423" xr:uid="{617AADC9-7534-FE45-96B0-EF4C1867B793}"/>
-    <hyperlink ref="B480" r:id="rId424" xr:uid="{7F8CDAA4-5094-8E4E-961B-41CDE5ACC0C0}"/>
-    <hyperlink ref="B481" r:id="rId425" xr:uid="{63F28ABD-12CF-5947-80DA-229E3CA3133E}"/>
-    <hyperlink ref="B488" r:id="rId426" xr:uid="{0A1DB92C-3315-1942-B27D-4B90986A6D9D}"/>
-    <hyperlink ref="B487" r:id="rId427" xr:uid="{11738B67-CADD-5D45-8417-8BE7A03FC79F}"/>
-    <hyperlink ref="B486" r:id="rId428" xr:uid="{B2B23748-D9E4-BE4F-A93E-49ECB4063831}"/>
-    <hyperlink ref="B485" r:id="rId429" xr:uid="{A2FB8A72-37B9-7E4A-B050-FD6CD20BCE73}"/>
-    <hyperlink ref="B484" r:id="rId430" xr:uid="{5A93C9AF-BFEB-EB40-95AC-C309ED09A604}"/>
-    <hyperlink ref="B483" r:id="rId431" xr:uid="{CC203923-2DC2-874B-B846-A8455E3CC2F2}"/>
-    <hyperlink ref="B482" r:id="rId432" xr:uid="{FCB0246E-0179-B447-B3CE-C60CDB388472}"/>
-    <hyperlink ref="B491" r:id="rId433" xr:uid="{F06CEE72-8CA4-C547-862C-39B86CD3226A}"/>
-    <hyperlink ref="B492" r:id="rId434" xr:uid="{CB3045F2-8D63-0F4E-85BC-AF016DB4F247}"/>
-    <hyperlink ref="B493" r:id="rId435" xr:uid="{667D57F5-E5AD-674F-A2F5-AFF4A14E4026}"/>
-    <hyperlink ref="B494" r:id="rId436" xr:uid="{27A13A65-56CE-BF4D-BA0D-EB87D910272D}"/>
-    <hyperlink ref="B495" r:id="rId437" xr:uid="{2C72A52E-6F06-0246-AEB5-93CD0DEA8866}"/>
-    <hyperlink ref="B496" r:id="rId438" xr:uid="{24B29046-B4DD-674B-9EDF-6C94BEC3FDD8}"/>
-    <hyperlink ref="B497" r:id="rId439" xr:uid="{D018EBC3-3FB3-AC4D-9D64-D218345A46C8}"/>
-    <hyperlink ref="B500" r:id="rId440" xr:uid="{1E1D3964-01E0-3145-ACFE-B6A5BF0EECB0}"/>
-    <hyperlink ref="B498" r:id="rId441" xr:uid="{FA0E5061-A7E2-C045-9671-1CD9446D1932}"/>
-    <hyperlink ref="B499" r:id="rId442" location=":~:text=Given%20an%20integer%20n%2C%20calculate,*%2C%20%2F%20and%20pow().&amp;text=A%20Simple%20Solution%20is%20to%20repeatedly%20add%20n%20to%20result." xr:uid="{92704F5B-7B31-2F42-80DD-764B2206D9DB}"/>
+    <hyperlink ref="B432" r:id="rId375" xr:uid="{FE300343-4633-AD47-A64D-2086629EB398}"/>
+    <hyperlink ref="B433" r:id="rId376" xr:uid="{4FC9F782-D38F-C642-A863-887B17AD05CD}"/>
+    <hyperlink ref="B434" r:id="rId377" xr:uid="{830C5466-10E3-7A48-B3E7-35C15A1CA4EF}"/>
+    <hyperlink ref="B435" r:id="rId378" xr:uid="{1B987077-E9D3-6F40-89EE-0D4E7180D884}"/>
+    <hyperlink ref="B436" r:id="rId379" xr:uid="{D4843E1F-7226-864E-A4BB-264D5A487B6D}"/>
+    <hyperlink ref="B437" r:id="rId380" xr:uid="{61816592-2D19-9946-8253-47A60218F2EA}"/>
+    <hyperlink ref="B438" r:id="rId381" xr:uid="{736C840F-19A3-0A4B-8863-ECB772B46385}"/>
+    <hyperlink ref="B439" r:id="rId382" xr:uid="{05A238AD-3C5B-C546-94E9-75BBF964711A}"/>
+    <hyperlink ref="B440" r:id="rId383" xr:uid="{7029629C-3F2A-4A49-997B-CFE86EC8B3C2}"/>
+    <hyperlink ref="B441" r:id="rId384" xr:uid="{ADA66B57-2FAC-AB42-BD83-4931708F3AB5}"/>
+    <hyperlink ref="B442" r:id="rId385" xr:uid="{F16BF1F9-755B-B045-B9A8-0B97E3BAC8B0}"/>
+    <hyperlink ref="B443" r:id="rId386" xr:uid="{ECCE930A-B960-234C-81EC-4B8514282AE9}"/>
+    <hyperlink ref="B444" r:id="rId387" xr:uid="{7AA58141-7D24-7C42-A0C1-F852B21CFFD9}"/>
+    <hyperlink ref="B445" r:id="rId388" xr:uid="{B1FCB47D-7921-3446-B2C7-72CBA815D056}"/>
+    <hyperlink ref="B446" r:id="rId389" xr:uid="{8C547719-AA03-3543-B31F-7300674AF4C5}"/>
+    <hyperlink ref="B447" r:id="rId390" xr:uid="{09922668-AFC0-F242-860E-9967E0F0FEF4}"/>
+    <hyperlink ref="B448" r:id="rId391" xr:uid="{0DA963DA-238B-D44E-9E03-6E6BD933B35E}"/>
+    <hyperlink ref="B449" r:id="rId392" xr:uid="{89518AFF-2526-C845-BC9D-95FE77AF416E}"/>
+    <hyperlink ref="B450" r:id="rId393" xr:uid="{FAECBBBE-196C-7A41-A0FB-E0597CB2CF51}"/>
+    <hyperlink ref="B451" r:id="rId394" xr:uid="{8126B039-0B25-B040-A0F6-C3457341A2E9}"/>
+    <hyperlink ref="B452" r:id="rId395" xr:uid="{6CB326E6-E698-EB42-884B-C89FFA33E3BA}"/>
+    <hyperlink ref="B453" r:id="rId396" xr:uid="{8C97EFD1-933F-A44F-A1CF-6386233104A2}"/>
+    <hyperlink ref="B454" r:id="rId397" xr:uid="{8F019F07-8532-E147-8BE1-4EBE833F61CA}"/>
+    <hyperlink ref="B455" r:id="rId398" xr:uid="{00F1A08F-3767-784A-97A3-4603DE38BACC}"/>
+    <hyperlink ref="B456" r:id="rId399" xr:uid="{2A84ADCB-071F-9A48-994D-7A838307EFD8}"/>
+    <hyperlink ref="B457" r:id="rId400" xr:uid="{132F8C6D-D5E8-6440-AC4E-B81EA2100416}"/>
+    <hyperlink ref="B458" r:id="rId401" xr:uid="{2DA6EAC2-1A1D-754F-9613-226CBC7890AF}"/>
+    <hyperlink ref="B459" r:id="rId402" xr:uid="{05BED99A-4562-D14E-8627-D07CF5335A9B}"/>
+    <hyperlink ref="B460" r:id="rId403" xr:uid="{111D902A-3F60-2D4B-89D3-5BCBD8AA38DD}"/>
+    <hyperlink ref="B461" r:id="rId404" xr:uid="{F19236BE-AC32-3542-9214-DFC3BAE04ED0}"/>
+    <hyperlink ref="B462" r:id="rId405" xr:uid="{4D97CD96-EA1B-664E-9380-EFD27077D273}"/>
+    <hyperlink ref="B463" r:id="rId406" xr:uid="{49A46D91-633F-A148-ACFA-49B7D1AA4B33}"/>
+    <hyperlink ref="B464" r:id="rId407" xr:uid="{7C3B7901-67E3-EA4D-BC64-21A78BC03AC6}"/>
+    <hyperlink ref="B465" r:id="rId408" xr:uid="{B27CA8C3-D34F-5E4D-94A5-11D14AFD0F82}"/>
+    <hyperlink ref="B466" r:id="rId409" xr:uid="{8FECE038-9764-5E4A-8C6E-9B3209812651}"/>
+    <hyperlink ref="B467" r:id="rId410" xr:uid="{95696D4B-89CB-5640-BE92-53B3C043F7EB}"/>
+    <hyperlink ref="B468" r:id="rId411" xr:uid="{DA74B737-802A-4944-A93E-0B9C8417630B}"/>
+    <hyperlink ref="B469" r:id="rId412" xr:uid="{B2C4C168-50FA-AF41-8F56-9E70613CF17D}"/>
+    <hyperlink ref="B471" r:id="rId413" xr:uid="{B7090C60-AC27-3F4F-8F0D-42F0791928C6}"/>
+    <hyperlink ref="B470" r:id="rId414" xr:uid="{07400041-66C6-514B-B3E3-427F2947C2B7}"/>
+    <hyperlink ref="B472" r:id="rId415" xr:uid="{B7E78172-8FB8-4E42-87D8-6A4654D79C62}"/>
+    <hyperlink ref="B473" r:id="rId416" xr:uid="{9A5D4670-BC64-334A-88CF-6F8287692C5E}"/>
+    <hyperlink ref="B474" r:id="rId417" xr:uid="{604283B6-53BC-044F-8D9D-E6094E798317}"/>
+    <hyperlink ref="B475" r:id="rId418" xr:uid="{5EB15AC7-3E0E-E44C-A5B9-32F30F234B5A}"/>
+    <hyperlink ref="B476" r:id="rId419" xr:uid="{3076BD5F-4B23-4146-A50A-499C9FF4C3D2}"/>
+    <hyperlink ref="B477" r:id="rId420" xr:uid="{6A29D9C2-1E78-1B43-A251-0AB0A97FA70E}"/>
+    <hyperlink ref="B478" r:id="rId421" xr:uid="{00597D5E-D693-DF4E-84C0-47E58A6ACA8F}"/>
+    <hyperlink ref="B479" r:id="rId422" xr:uid="{48640988-9964-0B4C-A014-83E2CEB3D632}"/>
+    <hyperlink ref="B480" r:id="rId423" xr:uid="{617AADC9-7534-FE45-96B0-EF4C1867B793}"/>
+    <hyperlink ref="B481" r:id="rId424" xr:uid="{7F8CDAA4-5094-8E4E-961B-41CDE5ACC0C0}"/>
+    <hyperlink ref="B482" r:id="rId425" xr:uid="{63F28ABD-12CF-5947-80DA-229E3CA3133E}"/>
+    <hyperlink ref="B489" r:id="rId426" xr:uid="{0A1DB92C-3315-1942-B27D-4B90986A6D9D}"/>
+    <hyperlink ref="B488" r:id="rId427" xr:uid="{11738B67-CADD-5D45-8417-8BE7A03FC79F}"/>
+    <hyperlink ref="B487" r:id="rId428" xr:uid="{B2B23748-D9E4-BE4F-A93E-49ECB4063831}"/>
+    <hyperlink ref="B486" r:id="rId429" xr:uid="{A2FB8A72-37B9-7E4A-B050-FD6CD20BCE73}"/>
+    <hyperlink ref="B485" r:id="rId430" xr:uid="{5A93C9AF-BFEB-EB40-95AC-C309ED09A604}"/>
+    <hyperlink ref="B484" r:id="rId431" xr:uid="{CC203923-2DC2-874B-B846-A8455E3CC2F2}"/>
+    <hyperlink ref="B483" r:id="rId432" xr:uid="{FCB0246E-0179-B447-B3CE-C60CDB388472}"/>
+    <hyperlink ref="B492" r:id="rId433" xr:uid="{F06CEE72-8CA4-C547-862C-39B86CD3226A}"/>
+    <hyperlink ref="B493" r:id="rId434" xr:uid="{CB3045F2-8D63-0F4E-85BC-AF016DB4F247}"/>
+    <hyperlink ref="B494" r:id="rId435" xr:uid="{667D57F5-E5AD-674F-A2F5-AFF4A14E4026}"/>
+    <hyperlink ref="B495" r:id="rId436" xr:uid="{27A13A65-56CE-BF4D-BA0D-EB87D910272D}"/>
+    <hyperlink ref="B496" r:id="rId437" xr:uid="{2C72A52E-6F06-0246-AEB5-93CD0DEA8866}"/>
+    <hyperlink ref="B497" r:id="rId438" xr:uid="{24B29046-B4DD-674B-9EDF-6C94BEC3FDD8}"/>
+    <hyperlink ref="B498" r:id="rId439" xr:uid="{D018EBC3-3FB3-AC4D-9D64-D218345A46C8}"/>
+    <hyperlink ref="B501" r:id="rId440" xr:uid="{1E1D3964-01E0-3145-ACFE-B6A5BF0EECB0}"/>
+    <hyperlink ref="B499" r:id="rId441" xr:uid="{FA0E5061-A7E2-C045-9671-1CD9446D1932}"/>
+    <hyperlink ref="B500" r:id="rId442" location=":~:text=Given%20an%20integer%20n%2C%20calculate,*%2C%20%2F%20and%20pow().&amp;text=A%20Simple%20Solution%20is%20to%20repeatedly%20add%20n%20to%20result." xr:uid="{92704F5B-7B31-2F42-80DD-764B2206D9DB}"/>
     <hyperlink ref="B370" r:id="rId443" xr:uid="{A48B1A24-83B1-7A4C-8129-CD37804DF849}"/>
     <hyperlink ref="B2" r:id="rId444" xr:uid="{E07D4FE5-46C7-AC4D-9E01-2300AA43B58A}"/>
     <hyperlink ref="B39" r:id="rId445" xr:uid="{F2DE2162-BD02-7549-AC1A-27455F78131F}"/>
@@ -7892,8 +7909,9 @@
     <hyperlink ref="B293" r:id="rId463" xr:uid="{127345A9-71F3-49D6-AB7A-BF4305D0F725}"/>
     <hyperlink ref="B428" r:id="rId464" xr:uid="{C4A51DBE-F043-4951-B51A-E48796555D08}"/>
     <hyperlink ref="B430" r:id="rId465" xr:uid="{910FE4FA-F82F-4691-9E2F-22E8206DA592}"/>
+    <hyperlink ref="B431" r:id="rId466" xr:uid="{7765BDB0-9A3B-4694-9899-1513A0FC9809}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId466"/>
+  <pageSetup orientation="portrait" r:id="rId467"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Program for nth Catalan Number
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harsh\Desktop\Data-Structures-and-Algorithms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71D0D2BF-AF3E-4F28-915A-5D0D6DDAC722}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17E6F248-9296-445A-BBFC-89CE14DDEA4F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -2087,7 +2087,7 @@
   <dimension ref="A1:D501"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A422" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B433" sqref="B433"/>
+      <selection activeCell="C435" sqref="C435"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -6714,8 +6714,8 @@
       <c r="B434" s="6" t="s">
         <v>397</v>
       </c>
-      <c r="C434" s="4" t="s">
-        <v>4</v>
+      <c r="C434" s="11" t="s">
+        <v>464</v>
       </c>
     </row>
     <row r="435" spans="1:3" ht="21">

</xml_diff>

<commit_message>
LeetCode 1512. Number of Good Pairs
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harsh\Desktop\Data-Structures-and-Algorithms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17E6F248-9296-445A-BBFC-89CE14DDEA4F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D1BD42C-70BF-41AA-8D22-4C4DFEA6A628}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1434" uniqueCount="504">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1437" uniqueCount="505">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1537,6 +1537,9 @@
   </si>
   <si>
     <t>Count minimum number of fountains to be activated to cover the entire garden</t>
+  </si>
+  <si>
+    <t>Number of Good Pairs</t>
   </si>
 </sst>
 </file>
@@ -2084,10 +2087,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
-  <dimension ref="A1:D501"/>
+  <dimension ref="A1:D502"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A422" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C435" sqref="C435"/>
+      <selection activeCell="B434" sqref="B434"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -6712,7 +6715,7 @@
         <v>392</v>
       </c>
       <c r="B434" s="6" t="s">
-        <v>397</v>
+        <v>504</v>
       </c>
       <c r="C434" s="11" t="s">
         <v>464</v>
@@ -6723,10 +6726,10 @@
         <v>392</v>
       </c>
       <c r="B435" s="6" t="s">
-        <v>398</v>
-      </c>
-      <c r="C435" s="4" t="s">
-        <v>4</v>
+        <v>397</v>
+      </c>
+      <c r="C435" s="11" t="s">
+        <v>464</v>
       </c>
     </row>
     <row r="436" spans="1:3" ht="21">
@@ -6734,7 +6737,7 @@
         <v>392</v>
       </c>
       <c r="B436" s="6" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="C436" s="4" t="s">
         <v>4</v>
@@ -6745,7 +6748,7 @@
         <v>392</v>
       </c>
       <c r="B437" s="6" t="s">
-        <v>272</v>
+        <v>399</v>
       </c>
       <c r="C437" s="4" t="s">
         <v>4</v>
@@ -6756,7 +6759,7 @@
         <v>392</v>
       </c>
       <c r="B438" s="6" t="s">
-        <v>400</v>
+        <v>272</v>
       </c>
       <c r="C438" s="4" t="s">
         <v>4</v>
@@ -6767,7 +6770,7 @@
         <v>392</v>
       </c>
       <c r="B439" s="6" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="C439" s="4" t="s">
         <v>4</v>
@@ -6778,7 +6781,7 @@
         <v>392</v>
       </c>
       <c r="B440" s="6" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="C440" s="4" t="s">
         <v>4</v>
@@ -6789,7 +6792,7 @@
         <v>392</v>
       </c>
       <c r="B441" s="6" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="C441" s="4" t="s">
         <v>4</v>
@@ -6800,7 +6803,7 @@
         <v>392</v>
       </c>
       <c r="B442" s="6" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="C442" s="4" t="s">
         <v>4</v>
@@ -6811,7 +6814,7 @@
         <v>392</v>
       </c>
       <c r="B443" s="6" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="C443" s="4" t="s">
         <v>4</v>
@@ -6822,7 +6825,7 @@
         <v>392</v>
       </c>
       <c r="B444" s="6" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="C444" s="4" t="s">
         <v>4</v>
@@ -6833,7 +6836,7 @@
         <v>392</v>
       </c>
       <c r="B445" s="6" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="C445" s="4" t="s">
         <v>4</v>
@@ -6844,7 +6847,7 @@
         <v>392</v>
       </c>
       <c r="B446" s="6" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="C446" s="4" t="s">
         <v>4</v>
@@ -6855,7 +6858,7 @@
         <v>392</v>
       </c>
       <c r="B447" s="6" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="C447" s="4" t="s">
         <v>4</v>
@@ -6866,7 +6869,7 @@
         <v>392</v>
       </c>
       <c r="B448" s="6" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="C448" s="4" t="s">
         <v>4</v>
@@ -6877,7 +6880,7 @@
         <v>392</v>
       </c>
       <c r="B449" s="6" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="C449" s="4" t="s">
         <v>4</v>
@@ -6888,7 +6891,7 @@
         <v>392</v>
       </c>
       <c r="B450" s="6" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C450" s="4" t="s">
         <v>4</v>
@@ -6899,7 +6902,7 @@
         <v>392</v>
       </c>
       <c r="B451" s="6" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="C451" s="4" t="s">
         <v>4</v>
@@ -6910,7 +6913,7 @@
         <v>392</v>
       </c>
       <c r="B452" s="6" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C452" s="4" t="s">
         <v>4</v>
@@ -6921,7 +6924,7 @@
         <v>392</v>
       </c>
       <c r="B453" s="6" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C453" s="4" t="s">
         <v>4</v>
@@ -6932,7 +6935,7 @@
         <v>392</v>
       </c>
       <c r="B454" s="6" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C454" s="4" t="s">
         <v>4</v>
@@ -6943,7 +6946,7 @@
         <v>392</v>
       </c>
       <c r="B455" s="6" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C455" s="4" t="s">
         <v>4</v>
@@ -6954,7 +6957,7 @@
         <v>392</v>
       </c>
       <c r="B456" s="6" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="C456" s="4" t="s">
         <v>4</v>
@@ -6965,7 +6968,7 @@
         <v>392</v>
       </c>
       <c r="B457" s="6" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="C457" s="4" t="s">
         <v>4</v>
@@ -6976,7 +6979,7 @@
         <v>392</v>
       </c>
       <c r="B458" s="6" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="C458" s="4" t="s">
         <v>4</v>
@@ -6987,7 +6990,7 @@
         <v>392</v>
       </c>
       <c r="B459" s="6" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="C459" s="4" t="s">
         <v>4</v>
@@ -6998,7 +7001,7 @@
         <v>392</v>
       </c>
       <c r="B460" s="6" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="C460" s="4" t="s">
         <v>4</v>
@@ -7009,7 +7012,7 @@
         <v>392</v>
       </c>
       <c r="B461" s="6" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="C461" s="4" t="s">
         <v>4</v>
@@ -7020,7 +7023,7 @@
         <v>392</v>
       </c>
       <c r="B462" s="6" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="C462" s="4" t="s">
         <v>4</v>
@@ -7031,7 +7034,7 @@
         <v>392</v>
       </c>
       <c r="B463" s="6" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C463" s="4" t="s">
         <v>4</v>
@@ -7042,7 +7045,7 @@
         <v>392</v>
       </c>
       <c r="B464" s="6" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="C464" s="4" t="s">
         <v>4</v>
@@ -7053,7 +7056,7 @@
         <v>392</v>
       </c>
       <c r="B465" s="6" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="C465" s="4" t="s">
         <v>4</v>
@@ -7064,7 +7067,7 @@
         <v>392</v>
       </c>
       <c r="B466" s="6" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="C466" s="4" t="s">
         <v>4</v>
@@ -7075,7 +7078,7 @@
         <v>392</v>
       </c>
       <c r="B467" s="6" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="C467" s="4" t="s">
         <v>4</v>
@@ -7086,7 +7089,7 @@
         <v>392</v>
       </c>
       <c r="B468" s="6" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="C468" s="4" t="s">
         <v>4</v>
@@ -7097,7 +7100,7 @@
         <v>392</v>
       </c>
       <c r="B469" s="6" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C469" s="4" t="s">
         <v>4</v>
@@ -7108,7 +7111,7 @@
         <v>392</v>
       </c>
       <c r="B470" s="6" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="C470" s="4" t="s">
         <v>4</v>
@@ -7119,7 +7122,7 @@
         <v>392</v>
       </c>
       <c r="B471" s="6" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C471" s="4" t="s">
         <v>4</v>
@@ -7130,7 +7133,7 @@
         <v>392</v>
       </c>
       <c r="B472" s="6" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C472" s="4" t="s">
         <v>4</v>
@@ -7141,7 +7144,7 @@
         <v>392</v>
       </c>
       <c r="B473" s="6" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="C473" s="4" t="s">
         <v>4</v>
@@ -7152,7 +7155,7 @@
         <v>392</v>
       </c>
       <c r="B474" s="6" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="C474" s="4" t="s">
         <v>4</v>
@@ -7163,7 +7166,7 @@
         <v>392</v>
       </c>
       <c r="B475" s="6" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="C475" s="4" t="s">
         <v>4</v>
@@ -7174,7 +7177,7 @@
         <v>392</v>
       </c>
       <c r="B476" s="6" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="C476" s="4" t="s">
         <v>4</v>
@@ -7185,7 +7188,7 @@
         <v>392</v>
       </c>
       <c r="B477" s="6" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="C477" s="4" t="s">
         <v>4</v>
@@ -7196,7 +7199,7 @@
         <v>392</v>
       </c>
       <c r="B478" s="6" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="C478" s="4" t="s">
         <v>4</v>
@@ -7207,7 +7210,7 @@
         <v>392</v>
       </c>
       <c r="B479" s="6" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="C479" s="4" t="s">
         <v>4</v>
@@ -7218,7 +7221,7 @@
         <v>392</v>
       </c>
       <c r="B480" s="6" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="C480" s="4" t="s">
         <v>4</v>
@@ -7229,7 +7232,7 @@
         <v>392</v>
       </c>
       <c r="B481" s="6" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="C481" s="4" t="s">
         <v>4</v>
@@ -7240,7 +7243,7 @@
         <v>392</v>
       </c>
       <c r="B482" s="6" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="C482" s="4" t="s">
         <v>4</v>
@@ -7251,7 +7254,7 @@
         <v>392</v>
       </c>
       <c r="B483" s="6" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="C483" s="4" t="s">
         <v>4</v>
@@ -7262,7 +7265,7 @@
         <v>392</v>
       </c>
       <c r="B484" s="6" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="C484" s="4" t="s">
         <v>4</v>
@@ -7273,7 +7276,7 @@
         <v>392</v>
       </c>
       <c r="B485" s="6" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="C485" s="4" t="s">
         <v>4</v>
@@ -7284,7 +7287,7 @@
         <v>392</v>
       </c>
       <c r="B486" s="6" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="C486" s="4" t="s">
         <v>4</v>
@@ -7295,7 +7298,7 @@
         <v>392</v>
       </c>
       <c r="B487" s="6" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="C487" s="4" t="s">
         <v>4</v>
@@ -7306,7 +7309,7 @@
         <v>392</v>
       </c>
       <c r="B488" s="6" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="C488" s="4" t="s">
         <v>4</v>
@@ -7317,38 +7320,38 @@
         <v>392</v>
       </c>
       <c r="B489" s="6" t="s">
+        <v>450</v>
+      </c>
+      <c r="C489" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="490" spans="1:3" ht="21">
+      <c r="A490" s="5" t="s">
+        <v>392</v>
+      </c>
+      <c r="B490" s="6" t="s">
         <v>451</v>
       </c>
-      <c r="C489" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="490" spans="1:3" ht="21">
-      <c r="B490" s="7"/>
-      <c r="C490" s="4"/>
+      <c r="C490" s="4" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="491" spans="1:3" ht="21">
-      <c r="A491" s="8"/>
       <c r="B491" s="7"/>
       <c r="C491" s="4"/>
     </row>
     <row r="492" spans="1:3" ht="21">
-      <c r="A492" s="5" t="s">
-        <v>452</v>
-      </c>
-      <c r="B492" s="6" t="s">
-        <v>453</v>
-      </c>
-      <c r="C492" s="4" t="s">
-        <v>4</v>
-      </c>
+      <c r="A492" s="8"/>
+      <c r="B492" s="7"/>
+      <c r="C492" s="4"/>
     </row>
     <row r="493" spans="1:3" ht="21">
       <c r="A493" s="5" t="s">
         <v>452</v>
       </c>
       <c r="B493" s="6" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="C493" s="4" t="s">
         <v>4</v>
@@ -7359,7 +7362,7 @@
         <v>452</v>
       </c>
       <c r="B494" s="6" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="C494" s="4" t="s">
         <v>4</v>
@@ -7370,7 +7373,7 @@
         <v>452</v>
       </c>
       <c r="B495" s="6" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="C495" s="4" t="s">
         <v>4</v>
@@ -7381,7 +7384,7 @@
         <v>452</v>
       </c>
       <c r="B496" s="6" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="C496" s="4" t="s">
         <v>4</v>
@@ -7392,7 +7395,7 @@
         <v>452</v>
       </c>
       <c r="B497" s="6" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="C497" s="4" t="s">
         <v>4</v>
@@ -7403,7 +7406,7 @@
         <v>452</v>
       </c>
       <c r="B498" s="6" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="C498" s="4" t="s">
         <v>4</v>
@@ -7414,7 +7417,7 @@
         <v>452</v>
       </c>
       <c r="B499" s="6" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="C499" s="4" t="s">
         <v>4</v>
@@ -7425,7 +7428,7 @@
         <v>452</v>
       </c>
       <c r="B500" s="6" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="C500" s="4" t="s">
         <v>4</v>
@@ -7436,9 +7439,20 @@
         <v>452</v>
       </c>
       <c r="B501" s="6" t="s">
+        <v>461</v>
+      </c>
+      <c r="C501" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="502" spans="1:3" ht="21">
+      <c r="A502" s="5" t="s">
+        <v>452</v>
+      </c>
+      <c r="B502" s="6" t="s">
         <v>462</v>
       </c>
-      <c r="C501" s="4" t="s">
+      <c r="C502" s="4" t="s">
         <v>4</v>
       </c>
     </row>
@@ -7820,72 +7834,72 @@
     <hyperlink ref="B429" r:id="rId374" xr:uid="{A113C7A9-2359-B643-9C08-E845813439C0}"/>
     <hyperlink ref="B432" r:id="rId375" xr:uid="{FE300343-4633-AD47-A64D-2086629EB398}"/>
     <hyperlink ref="B433" r:id="rId376" xr:uid="{4FC9F782-D38F-C642-A863-887B17AD05CD}"/>
-    <hyperlink ref="B434" r:id="rId377" xr:uid="{830C5466-10E3-7A48-B3E7-35C15A1CA4EF}"/>
-    <hyperlink ref="B435" r:id="rId378" xr:uid="{1B987077-E9D3-6F40-89EE-0D4E7180D884}"/>
-    <hyperlink ref="B436" r:id="rId379" xr:uid="{D4843E1F-7226-864E-A4BB-264D5A487B6D}"/>
-    <hyperlink ref="B437" r:id="rId380" xr:uid="{61816592-2D19-9946-8253-47A60218F2EA}"/>
-    <hyperlink ref="B438" r:id="rId381" xr:uid="{736C840F-19A3-0A4B-8863-ECB772B46385}"/>
-    <hyperlink ref="B439" r:id="rId382" xr:uid="{05A238AD-3C5B-C546-94E9-75BBF964711A}"/>
-    <hyperlink ref="B440" r:id="rId383" xr:uid="{7029629C-3F2A-4A49-997B-CFE86EC8B3C2}"/>
-    <hyperlink ref="B441" r:id="rId384" xr:uid="{ADA66B57-2FAC-AB42-BD83-4931708F3AB5}"/>
-    <hyperlink ref="B442" r:id="rId385" xr:uid="{F16BF1F9-755B-B045-B9A8-0B97E3BAC8B0}"/>
-    <hyperlink ref="B443" r:id="rId386" xr:uid="{ECCE930A-B960-234C-81EC-4B8514282AE9}"/>
-    <hyperlink ref="B444" r:id="rId387" xr:uid="{7AA58141-7D24-7C42-A0C1-F852B21CFFD9}"/>
-    <hyperlink ref="B445" r:id="rId388" xr:uid="{B1FCB47D-7921-3446-B2C7-72CBA815D056}"/>
-    <hyperlink ref="B446" r:id="rId389" xr:uid="{8C547719-AA03-3543-B31F-7300674AF4C5}"/>
-    <hyperlink ref="B447" r:id="rId390" xr:uid="{09922668-AFC0-F242-860E-9967E0F0FEF4}"/>
-    <hyperlink ref="B448" r:id="rId391" xr:uid="{0DA963DA-238B-D44E-9E03-6E6BD933B35E}"/>
-    <hyperlink ref="B449" r:id="rId392" xr:uid="{89518AFF-2526-C845-BC9D-95FE77AF416E}"/>
-    <hyperlink ref="B450" r:id="rId393" xr:uid="{FAECBBBE-196C-7A41-A0FB-E0597CB2CF51}"/>
-    <hyperlink ref="B451" r:id="rId394" xr:uid="{8126B039-0B25-B040-A0F6-C3457341A2E9}"/>
-    <hyperlink ref="B452" r:id="rId395" xr:uid="{6CB326E6-E698-EB42-884B-C89FFA33E3BA}"/>
-    <hyperlink ref="B453" r:id="rId396" xr:uid="{8C97EFD1-933F-A44F-A1CF-6386233104A2}"/>
-    <hyperlink ref="B454" r:id="rId397" xr:uid="{8F019F07-8532-E147-8BE1-4EBE833F61CA}"/>
-    <hyperlink ref="B455" r:id="rId398" xr:uid="{00F1A08F-3767-784A-97A3-4603DE38BACC}"/>
-    <hyperlink ref="B456" r:id="rId399" xr:uid="{2A84ADCB-071F-9A48-994D-7A838307EFD8}"/>
-    <hyperlink ref="B457" r:id="rId400" xr:uid="{132F8C6D-D5E8-6440-AC4E-B81EA2100416}"/>
-    <hyperlink ref="B458" r:id="rId401" xr:uid="{2DA6EAC2-1A1D-754F-9613-226CBC7890AF}"/>
-    <hyperlink ref="B459" r:id="rId402" xr:uid="{05BED99A-4562-D14E-8627-D07CF5335A9B}"/>
-    <hyperlink ref="B460" r:id="rId403" xr:uid="{111D902A-3F60-2D4B-89D3-5BCBD8AA38DD}"/>
-    <hyperlink ref="B461" r:id="rId404" xr:uid="{F19236BE-AC32-3542-9214-DFC3BAE04ED0}"/>
-    <hyperlink ref="B462" r:id="rId405" xr:uid="{4D97CD96-EA1B-664E-9380-EFD27077D273}"/>
-    <hyperlink ref="B463" r:id="rId406" xr:uid="{49A46D91-633F-A148-ACFA-49B7D1AA4B33}"/>
-    <hyperlink ref="B464" r:id="rId407" xr:uid="{7C3B7901-67E3-EA4D-BC64-21A78BC03AC6}"/>
-    <hyperlink ref="B465" r:id="rId408" xr:uid="{B27CA8C3-D34F-5E4D-94A5-11D14AFD0F82}"/>
-    <hyperlink ref="B466" r:id="rId409" xr:uid="{8FECE038-9764-5E4A-8C6E-9B3209812651}"/>
-    <hyperlink ref="B467" r:id="rId410" xr:uid="{95696D4B-89CB-5640-BE92-53B3C043F7EB}"/>
-    <hyperlink ref="B468" r:id="rId411" xr:uid="{DA74B737-802A-4944-A93E-0B9C8417630B}"/>
-    <hyperlink ref="B469" r:id="rId412" xr:uid="{B2C4C168-50FA-AF41-8F56-9E70613CF17D}"/>
-    <hyperlink ref="B471" r:id="rId413" xr:uid="{B7090C60-AC27-3F4F-8F0D-42F0791928C6}"/>
-    <hyperlink ref="B470" r:id="rId414" xr:uid="{07400041-66C6-514B-B3E3-427F2947C2B7}"/>
-    <hyperlink ref="B472" r:id="rId415" xr:uid="{B7E78172-8FB8-4E42-87D8-6A4654D79C62}"/>
-    <hyperlink ref="B473" r:id="rId416" xr:uid="{9A5D4670-BC64-334A-88CF-6F8287692C5E}"/>
-    <hyperlink ref="B474" r:id="rId417" xr:uid="{604283B6-53BC-044F-8D9D-E6094E798317}"/>
-    <hyperlink ref="B475" r:id="rId418" xr:uid="{5EB15AC7-3E0E-E44C-A5B9-32F30F234B5A}"/>
-    <hyperlink ref="B476" r:id="rId419" xr:uid="{3076BD5F-4B23-4146-A50A-499C9FF4C3D2}"/>
-    <hyperlink ref="B477" r:id="rId420" xr:uid="{6A29D9C2-1E78-1B43-A251-0AB0A97FA70E}"/>
-    <hyperlink ref="B478" r:id="rId421" xr:uid="{00597D5E-D693-DF4E-84C0-47E58A6ACA8F}"/>
-    <hyperlink ref="B479" r:id="rId422" xr:uid="{48640988-9964-0B4C-A014-83E2CEB3D632}"/>
-    <hyperlink ref="B480" r:id="rId423" xr:uid="{617AADC9-7534-FE45-96B0-EF4C1867B793}"/>
-    <hyperlink ref="B481" r:id="rId424" xr:uid="{7F8CDAA4-5094-8E4E-961B-41CDE5ACC0C0}"/>
-    <hyperlink ref="B482" r:id="rId425" xr:uid="{63F28ABD-12CF-5947-80DA-229E3CA3133E}"/>
-    <hyperlink ref="B489" r:id="rId426" xr:uid="{0A1DB92C-3315-1942-B27D-4B90986A6D9D}"/>
-    <hyperlink ref="B488" r:id="rId427" xr:uid="{11738B67-CADD-5D45-8417-8BE7A03FC79F}"/>
-    <hyperlink ref="B487" r:id="rId428" xr:uid="{B2B23748-D9E4-BE4F-A93E-49ECB4063831}"/>
-    <hyperlink ref="B486" r:id="rId429" xr:uid="{A2FB8A72-37B9-7E4A-B050-FD6CD20BCE73}"/>
-    <hyperlink ref="B485" r:id="rId430" xr:uid="{5A93C9AF-BFEB-EB40-95AC-C309ED09A604}"/>
-    <hyperlink ref="B484" r:id="rId431" xr:uid="{CC203923-2DC2-874B-B846-A8455E3CC2F2}"/>
-    <hyperlink ref="B483" r:id="rId432" xr:uid="{FCB0246E-0179-B447-B3CE-C60CDB388472}"/>
-    <hyperlink ref="B492" r:id="rId433" xr:uid="{F06CEE72-8CA4-C547-862C-39B86CD3226A}"/>
-    <hyperlink ref="B493" r:id="rId434" xr:uid="{CB3045F2-8D63-0F4E-85BC-AF016DB4F247}"/>
-    <hyperlink ref="B494" r:id="rId435" xr:uid="{667D57F5-E5AD-674F-A2F5-AFF4A14E4026}"/>
-    <hyperlink ref="B495" r:id="rId436" xr:uid="{27A13A65-56CE-BF4D-BA0D-EB87D910272D}"/>
-    <hyperlink ref="B496" r:id="rId437" xr:uid="{2C72A52E-6F06-0246-AEB5-93CD0DEA8866}"/>
-    <hyperlink ref="B497" r:id="rId438" xr:uid="{24B29046-B4DD-674B-9EDF-6C94BEC3FDD8}"/>
-    <hyperlink ref="B498" r:id="rId439" xr:uid="{D018EBC3-3FB3-AC4D-9D64-D218345A46C8}"/>
-    <hyperlink ref="B501" r:id="rId440" xr:uid="{1E1D3964-01E0-3145-ACFE-B6A5BF0EECB0}"/>
-    <hyperlink ref="B499" r:id="rId441" xr:uid="{FA0E5061-A7E2-C045-9671-1CD9446D1932}"/>
-    <hyperlink ref="B500" r:id="rId442" location=":~:text=Given%20an%20integer%20n%2C%20calculate,*%2C%20%2F%20and%20pow().&amp;text=A%20Simple%20Solution%20is%20to%20repeatedly%20add%20n%20to%20result." xr:uid="{92704F5B-7B31-2F42-80DD-764B2206D9DB}"/>
+    <hyperlink ref="B435" r:id="rId377" xr:uid="{830C5466-10E3-7A48-B3E7-35C15A1CA4EF}"/>
+    <hyperlink ref="B436" r:id="rId378" xr:uid="{1B987077-E9D3-6F40-89EE-0D4E7180D884}"/>
+    <hyperlink ref="B437" r:id="rId379" xr:uid="{D4843E1F-7226-864E-A4BB-264D5A487B6D}"/>
+    <hyperlink ref="B438" r:id="rId380" xr:uid="{61816592-2D19-9946-8253-47A60218F2EA}"/>
+    <hyperlink ref="B439" r:id="rId381" xr:uid="{736C840F-19A3-0A4B-8863-ECB772B46385}"/>
+    <hyperlink ref="B440" r:id="rId382" xr:uid="{05A238AD-3C5B-C546-94E9-75BBF964711A}"/>
+    <hyperlink ref="B441" r:id="rId383" xr:uid="{7029629C-3F2A-4A49-997B-CFE86EC8B3C2}"/>
+    <hyperlink ref="B442" r:id="rId384" xr:uid="{ADA66B57-2FAC-AB42-BD83-4931708F3AB5}"/>
+    <hyperlink ref="B443" r:id="rId385" xr:uid="{F16BF1F9-755B-B045-B9A8-0B97E3BAC8B0}"/>
+    <hyperlink ref="B444" r:id="rId386" xr:uid="{ECCE930A-B960-234C-81EC-4B8514282AE9}"/>
+    <hyperlink ref="B445" r:id="rId387" xr:uid="{7AA58141-7D24-7C42-A0C1-F852B21CFFD9}"/>
+    <hyperlink ref="B446" r:id="rId388" xr:uid="{B1FCB47D-7921-3446-B2C7-72CBA815D056}"/>
+    <hyperlink ref="B447" r:id="rId389" xr:uid="{8C547719-AA03-3543-B31F-7300674AF4C5}"/>
+    <hyperlink ref="B448" r:id="rId390" xr:uid="{09922668-AFC0-F242-860E-9967E0F0FEF4}"/>
+    <hyperlink ref="B449" r:id="rId391" xr:uid="{0DA963DA-238B-D44E-9E03-6E6BD933B35E}"/>
+    <hyperlink ref="B450" r:id="rId392" xr:uid="{89518AFF-2526-C845-BC9D-95FE77AF416E}"/>
+    <hyperlink ref="B451" r:id="rId393" xr:uid="{FAECBBBE-196C-7A41-A0FB-E0597CB2CF51}"/>
+    <hyperlink ref="B452" r:id="rId394" xr:uid="{8126B039-0B25-B040-A0F6-C3457341A2E9}"/>
+    <hyperlink ref="B453" r:id="rId395" xr:uid="{6CB326E6-E698-EB42-884B-C89FFA33E3BA}"/>
+    <hyperlink ref="B454" r:id="rId396" xr:uid="{8C97EFD1-933F-A44F-A1CF-6386233104A2}"/>
+    <hyperlink ref="B455" r:id="rId397" xr:uid="{8F019F07-8532-E147-8BE1-4EBE833F61CA}"/>
+    <hyperlink ref="B456" r:id="rId398" xr:uid="{00F1A08F-3767-784A-97A3-4603DE38BACC}"/>
+    <hyperlink ref="B457" r:id="rId399" xr:uid="{2A84ADCB-071F-9A48-994D-7A838307EFD8}"/>
+    <hyperlink ref="B458" r:id="rId400" xr:uid="{132F8C6D-D5E8-6440-AC4E-B81EA2100416}"/>
+    <hyperlink ref="B459" r:id="rId401" xr:uid="{2DA6EAC2-1A1D-754F-9613-226CBC7890AF}"/>
+    <hyperlink ref="B460" r:id="rId402" xr:uid="{05BED99A-4562-D14E-8627-D07CF5335A9B}"/>
+    <hyperlink ref="B461" r:id="rId403" xr:uid="{111D902A-3F60-2D4B-89D3-5BCBD8AA38DD}"/>
+    <hyperlink ref="B462" r:id="rId404" xr:uid="{F19236BE-AC32-3542-9214-DFC3BAE04ED0}"/>
+    <hyperlink ref="B463" r:id="rId405" xr:uid="{4D97CD96-EA1B-664E-9380-EFD27077D273}"/>
+    <hyperlink ref="B464" r:id="rId406" xr:uid="{49A46D91-633F-A148-ACFA-49B7D1AA4B33}"/>
+    <hyperlink ref="B465" r:id="rId407" xr:uid="{7C3B7901-67E3-EA4D-BC64-21A78BC03AC6}"/>
+    <hyperlink ref="B466" r:id="rId408" xr:uid="{B27CA8C3-D34F-5E4D-94A5-11D14AFD0F82}"/>
+    <hyperlink ref="B467" r:id="rId409" xr:uid="{8FECE038-9764-5E4A-8C6E-9B3209812651}"/>
+    <hyperlink ref="B468" r:id="rId410" xr:uid="{95696D4B-89CB-5640-BE92-53B3C043F7EB}"/>
+    <hyperlink ref="B469" r:id="rId411" xr:uid="{DA74B737-802A-4944-A93E-0B9C8417630B}"/>
+    <hyperlink ref="B470" r:id="rId412" xr:uid="{B2C4C168-50FA-AF41-8F56-9E70613CF17D}"/>
+    <hyperlink ref="B472" r:id="rId413" xr:uid="{B7090C60-AC27-3F4F-8F0D-42F0791928C6}"/>
+    <hyperlink ref="B471" r:id="rId414" xr:uid="{07400041-66C6-514B-B3E3-427F2947C2B7}"/>
+    <hyperlink ref="B473" r:id="rId415" xr:uid="{B7E78172-8FB8-4E42-87D8-6A4654D79C62}"/>
+    <hyperlink ref="B474" r:id="rId416" xr:uid="{9A5D4670-BC64-334A-88CF-6F8287692C5E}"/>
+    <hyperlink ref="B475" r:id="rId417" xr:uid="{604283B6-53BC-044F-8D9D-E6094E798317}"/>
+    <hyperlink ref="B476" r:id="rId418" xr:uid="{5EB15AC7-3E0E-E44C-A5B9-32F30F234B5A}"/>
+    <hyperlink ref="B477" r:id="rId419" xr:uid="{3076BD5F-4B23-4146-A50A-499C9FF4C3D2}"/>
+    <hyperlink ref="B478" r:id="rId420" xr:uid="{6A29D9C2-1E78-1B43-A251-0AB0A97FA70E}"/>
+    <hyperlink ref="B479" r:id="rId421" xr:uid="{00597D5E-D693-DF4E-84C0-47E58A6ACA8F}"/>
+    <hyperlink ref="B480" r:id="rId422" xr:uid="{48640988-9964-0B4C-A014-83E2CEB3D632}"/>
+    <hyperlink ref="B481" r:id="rId423" xr:uid="{617AADC9-7534-FE45-96B0-EF4C1867B793}"/>
+    <hyperlink ref="B482" r:id="rId424" xr:uid="{7F8CDAA4-5094-8E4E-961B-41CDE5ACC0C0}"/>
+    <hyperlink ref="B483" r:id="rId425" xr:uid="{63F28ABD-12CF-5947-80DA-229E3CA3133E}"/>
+    <hyperlink ref="B490" r:id="rId426" xr:uid="{0A1DB92C-3315-1942-B27D-4B90986A6D9D}"/>
+    <hyperlink ref="B489" r:id="rId427" xr:uid="{11738B67-CADD-5D45-8417-8BE7A03FC79F}"/>
+    <hyperlink ref="B488" r:id="rId428" xr:uid="{B2B23748-D9E4-BE4F-A93E-49ECB4063831}"/>
+    <hyperlink ref="B487" r:id="rId429" xr:uid="{A2FB8A72-37B9-7E4A-B050-FD6CD20BCE73}"/>
+    <hyperlink ref="B486" r:id="rId430" xr:uid="{5A93C9AF-BFEB-EB40-95AC-C309ED09A604}"/>
+    <hyperlink ref="B485" r:id="rId431" xr:uid="{CC203923-2DC2-874B-B846-A8455E3CC2F2}"/>
+    <hyperlink ref="B484" r:id="rId432" xr:uid="{FCB0246E-0179-B447-B3CE-C60CDB388472}"/>
+    <hyperlink ref="B493" r:id="rId433" xr:uid="{F06CEE72-8CA4-C547-862C-39B86CD3226A}"/>
+    <hyperlink ref="B494" r:id="rId434" xr:uid="{CB3045F2-8D63-0F4E-85BC-AF016DB4F247}"/>
+    <hyperlink ref="B495" r:id="rId435" xr:uid="{667D57F5-E5AD-674F-A2F5-AFF4A14E4026}"/>
+    <hyperlink ref="B496" r:id="rId436" xr:uid="{27A13A65-56CE-BF4D-BA0D-EB87D910272D}"/>
+    <hyperlink ref="B497" r:id="rId437" xr:uid="{2C72A52E-6F06-0246-AEB5-93CD0DEA8866}"/>
+    <hyperlink ref="B498" r:id="rId438" xr:uid="{24B29046-B4DD-674B-9EDF-6C94BEC3FDD8}"/>
+    <hyperlink ref="B499" r:id="rId439" xr:uid="{D018EBC3-3FB3-AC4D-9D64-D218345A46C8}"/>
+    <hyperlink ref="B502" r:id="rId440" xr:uid="{1E1D3964-01E0-3145-ACFE-B6A5BF0EECB0}"/>
+    <hyperlink ref="B500" r:id="rId441" xr:uid="{FA0E5061-A7E2-C045-9671-1CD9446D1932}"/>
+    <hyperlink ref="B501" r:id="rId442" location=":~:text=Given%20an%20integer%20n%2C%20calculate,*%2C%20%2F%20and%20pow().&amp;text=A%20Simple%20Solution%20is%20to%20repeatedly%20add%20n%20to%20result." xr:uid="{92704F5B-7B31-2F42-80DD-764B2206D9DB}"/>
     <hyperlink ref="B370" r:id="rId443" xr:uid="{A48B1A24-83B1-7A4C-8129-CD37804DF849}"/>
     <hyperlink ref="B2" r:id="rId444" xr:uid="{E07D4FE5-46C7-AC4D-9E01-2300AA43B58A}"/>
     <hyperlink ref="B39" r:id="rId445" xr:uid="{F2DE2162-BD02-7549-AC1A-27455F78131F}"/>
@@ -7910,8 +7924,9 @@
     <hyperlink ref="B428" r:id="rId464" xr:uid="{C4A51DBE-F043-4951-B51A-E48796555D08}"/>
     <hyperlink ref="B430" r:id="rId465" xr:uid="{910FE4FA-F82F-4691-9E2F-22E8206DA592}"/>
     <hyperlink ref="B431" r:id="rId466" xr:uid="{7765BDB0-9A3B-4694-9899-1513A0FC9809}"/>
+    <hyperlink ref="B434" r:id="rId467" xr:uid="{BA1143B7-CB98-4B8C-942F-0EFAF8EE5902}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId467"/>
+  <pageSetup orientation="portrait" r:id="rId468"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Partition Equal Subset Sum
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harsh\Desktop\Data-Structures-and-Algorithms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E84C4DE5-AAA7-4372-BC23-8EC3050493E7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0525C54-C9C9-4635-B2C0-9CE4AD301C67}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1439" uniqueCount="505">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1440" uniqueCount="505">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -2090,7 +2090,7 @@
   <dimension ref="A1:D503"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A433" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B438" sqref="B438"/>
+      <selection activeCell="B439" sqref="B439"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -6765,11 +6765,13 @@
         <v>464</v>
       </c>
     </row>
-    <row r="439" spans="1:3" ht="19.5">
+    <row r="439" spans="1:3" ht="21">
       <c r="A439" s="5" t="s">
         <v>392</v>
       </c>
-      <c r="B439" s="10"/>
+      <c r="B439" s="6" t="s">
+        <v>497</v>
+      </c>
       <c r="C439" s="11" t="s">
         <v>464</v>
       </c>
@@ -7934,8 +7936,9 @@
     <hyperlink ref="B430" r:id="rId465" xr:uid="{910FE4FA-F82F-4691-9E2F-22E8206DA592}"/>
     <hyperlink ref="B431" r:id="rId466" xr:uid="{7765BDB0-9A3B-4694-9899-1513A0FC9809}"/>
     <hyperlink ref="B434" r:id="rId467" xr:uid="{BA1143B7-CB98-4B8C-942F-0EFAF8EE5902}"/>
+    <hyperlink ref="B439" r:id="rId468" xr:uid="{6354E507-9FB5-49B4-B00E-53B7EFEC981B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId468"/>
+  <pageSetup orientation="portrait" r:id="rId469"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Maximize The Cut Segments
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harsh\Desktop\Data-Structures-and-Algorithms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{927C4289-F75E-4462-AB97-D5219C52A43B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{899CE9E9-ECA6-4340-936D-6BE1D12D8279}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -2090,7 +2090,7 @@
   <dimension ref="A1:D503"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A430" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C444" sqref="C444"/>
+      <selection activeCell="C445" sqref="C445"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -6827,8 +6827,8 @@
       <c r="B444" s="6" t="s">
         <v>404</v>
       </c>
-      <c r="C444" s="4" t="s">
-        <v>4</v>
+      <c r="C444" s="11" t="s">
+        <v>464</v>
       </c>
     </row>
     <row r="445" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Minimum no. of Jumps to reach end of an array
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harsh\Desktop\Data-Structures-and-Algorithms\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JARVIS\Desktop\Data-Structures-and-Algorithms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{899CE9E9-ECA6-4340-936D-6BE1D12D8279}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF74BAA1-1732-4928-8E50-CCB66EAEFD6E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -2089,8 +2089,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:D503"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A430" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C445" sqref="C445"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -2231,8 +2231,8 @@
       <c r="B15" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="12" t="s">
-        <v>4</v>
+      <c r="C15" s="11" t="s">
+        <v>464</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="21">

</xml_diff>